<commit_message>
Edits in the feedback loop
</commit_message>
<xml_diff>
--- a/QD_data.xlsx
+++ b/QD_data.xlsx
@@ -28,76 +28,76 @@
     <t>Description</t>
   </si>
   <si>
-    <t>[[2778, 2, 5, 0.2], [6935, 2, 7, 1.05], [6936, 2, 4, 1.57], [305, 2, 4, 0.53], [8672, 2, 5, 0.58], [615, 2, 4, 0.71], [1504, 2, 6, 0.37], [2775, 2, 5, 0.2], [145, 2, 5, 0.4], [2776, 2, 5, 0.8], [8853, 2, 4, 1.54], [2327, 2, 4, 0.63], [12721, 2, 5, 0.73], [130, 1, 4, 0.2], [143, 2, 4, 1.01], [146, 2, 4, 0.56], [2328, 2, 4, 0.78], [11681, 2, 5, 0.94], [11737, 2, 4, 0.53], [616, 2, 4, 1.09], [5491, 2, 4, 0.56], [141, 2, 4, 0.79], [362, 2, 5, 0.2], [144, 2, 4, 0.44], [2497, 2, 5, 0.45], [205, 2, 4, 0.46], [8650, 2, 4, 0.39], [5493, 2, 4, 0.2], [417, 2, 5, 0.57], [8676, 2, 4, 0.47], [8673, 2, 4, 0.24], [3670, 2, 4, 1.02], [2774, 2, 5, 0.33], [8648, 2, 4, 1.91], [589, 2, 5, 0.2], [3, 2, 5, 0.53], [206, 2, 4, 0.2], [6097, 80, 4, 1.14], [2423, 29, 4, 1.16], [22247, 2, 4, 1.01], [11836, 2, 4, 0.49], [6497, 1, 4, 0.5], [8674, 2, 5, 0.49], [624, 2, 4, 1.26], [2055, 3, 4, 1.18], [12343, 1, 4, 0.87], [2423, 80, 4, 1.1], [523, 2, 4, 0.68], [12344, 1, 4, 0.87], [593, 2, 5, 0.45], [6097, 29, 4, 1.14], [6098, 80, 5, 0.58], [12720, 2, 4, 0.82], [12345, 1, 4, 0.87], [11739, 2, 4, 0.53], [8915, 2, 4, 0.41], [75, 2, 4, 1.17], [88, 10, 8, 0.95], [326, 2, 4, 1.54], [6494, 1, 4, 0.46], [60, 3, 6, 0.19], [13260, 29, 4, 0.36], [142, 2, 4, 0.79], [3429, 15, 4, 0.46], [1492, 1, 4, 0.62], [411, 2, 4, 0.44], [21712, 3, 13, 0.67], [412, 1, 4, 1.0], [1050, 2, 4, 0.38], [2422, 80, 4, 1.31], [10149, 3, 13, 1.12], [2422, 29, 5, 1.19], [6098, 29, 4, 1.08], [378, 2, 4, 1.16], [12346, 1, 4, 0.87], [7704, 2, 4, 1.15], [151, 1, 4, 0.57], [11738, 2, 4, 0.53], [22316, 3, 4, 0.46], [1243, 2, 4, 0.72], [229, 1, 4, 2.0], [1049, 2, 4, 0.38], [13264, 29, 4, 0.51], [20252, 2, 4, 0.58], [345, 3, 4, 1.26], [13258, 29, 4, 0.67], [1490, 1, 4, 0.47], [964, 15, 4, 0.36], [12269, 2, 4, 0.51], [2438, 1, 4, 1.05], [2821, 3, 10, 0.23], [5208, 3, 5, 0.74], [10407, 10, 6, 1.18], [2331, 1, 4, 0.55], [1163, 3, 5, 0.58], [416, 1, 4, 1.66], [201, 3, 4, 1.26], [307, 2, 4, 1.04], [186, 3, 7, 0.5], [7004, 1, 4, 0.56], [149, 2, 4, 0.37], [418, 2, 4, 0.54], [957, 2, 4, 0.57], [13259, 29, 4, 1.13], [1309, 1, 4, 0.44], [7705, 2, 4, 1.15], [12229, 2, 4, 0.52], [7706, 2, 4, 1.15], [10406, 10, 7, 1.21], [11687, 2, 4, 0.56], [410, 1, 4, 0.71], [7036, 1, 4, 0.43], [3478, 2, 4, 0.57], [20255, 2, 4, 0.4], [9784, 1, 4, 0.91], [21713, 3, 7, 0.46], [8938, 2, 4, 0.57], [10408, 10, 6, 1.04], [5490, 2, 4, 0.49], [12870, 1, 4, 2.33], [11402, 1, 4, 0.46], [10410, 10, 6, 1.18], [19687, 1, 4, 1.21], [2438, 2, 5, 1.38], [11490, 1, 4, 0.43], [107, 7, 5, 1.24], [2703, 3, 4, 2.13], [11161, 1, 5, 1.8], [956, 2, 4, 0.53], [1886, 2, 4, 0.35], [21781, 2, 4, 0.47], [11690, 2, 4, 0.36], [10411, 10, 6, 1.12], [2778, 2, 104, 2.81], [6935, 2, 187, 6.0], [6936, 2, 141, 5.81], [305, 2, 74, 3.08], [8672, 2, 144, 3.33], [615, 2, 54, 3.4], [1504, 2, 102, 2.95], [2775, 2, 78, 3.13], [145, 2, 76, 2.84], [2776, 2, 78, 4.5], [8853, 2, 141, 5.13], [2327, 2, 76, 3.26], [12721, 2, 284, 3.49], [130, 1, 30, 2.98], [143, 2, 75, 3.04], [146, 2, 76, 3.13], [2328, 2, 76, 3.53], [11681, 2, 138, 5.48], [11737, 2, 56, 3.11], [616, 2, 107, 3.95], [5491, 2, 108, 2.82], [141, 2, 155, 4.16], [362, 2, 72, 2.96], [144, 2, 76, 2.91], [2497, 2, 102, 3.25], [205, 2, 109, 2.64], [8650, 2, 114, 4.44], [5493, 2, 55, 2.97], [417, 2, 78, 3.15], [8676, 2, 144, 2.97], [8673, 2, 144, 5.05], [3670, 2, 235, 5.79], [2774, 2, 102, 6.0], [8648, 2, 225, 5.29], [589, 2, 77, 2.91], [3, 2, 61, 3.09], [206, 2, 42, 2.64], [6097, 80, 35, 5.49], [2423, 29, 37, 4.81], [22247, 2, 144, 3.05], [11836, 2, 269, 2.69], [6497, 1, 32, 2.94], [8674, 2, 144, 3.57], [624, 2, 107, 4.11], [2055, 3, 158, 4.31], [12343, 1, 610, 4.37], [2423, 80, 185, 4.75], [523, 2, 155, 3.04], [12344, 1, 610, 3.38], [593, 2, 115, 2.86], [6097, 29, 18, 5.49], [6098, 80, 38, 3.97], [12720, 2, 284, 3.48], [12345, 1, 610, 4.37], [11739, 2, 56, 3.11], [8915, 2, 129, 2.36], [75, 2, 144, 3.94], [88, 10, 561, 4.69], [326, 2, 30, 3.9], [6494, 1, 52, 2.64], [60, 3, 405, 4.08], [13260, 29, 36, 2.76], [142, 2, 155, 4.16], [3429, 15, 53, 2.63], [1492, 1, 37, 2.92], [411, 2, 109, 2.6], [21712, 3, 2180, 2.89]]</t>
-  </si>
-  <si>
-    <t>[[141, 2, 4, 0.51], [2328, 2, 4, 0.28], [8650, 2, 5, 0.39], [362, 2, 4, 0.2], [5491, 2, 4, 0.6], [5493, 2, 4, 0.2], [130, 1, 5, 0.48], [589, 2, 4, 0.52], [2327, 2, 4, 0.2], [326, 2, 4, 0.97], [11685, 2, 4, 1.41], [8672, 2, 5, 0.58], [417, 2, 4, 0.56], [6935, 2, 8, 1.3], [205, 2, 4, 0.37], [11681, 2, 5, 1.41], [206, 2, 4, 0.2], [8648, 2, 4, 1.7], [6936, 2, 5, 1.32], [142, 2, 4, 0.2], [8915, 2, 5, 0.2], [11837, 2, 4, 0.55], [12721, 2, 5, 0.97], [11838, 2, 4, 0.2], [2049, 3, 9, 0.47], [1446, 2, 4, 0.78], [523, 2, 4, 0.56], [615, 2, 4, 1.55], [8676, 2, 4, 0.49], [11737, 2, 4, 1.04], [305, 2, 5, 0.53], [616, 2, 4, 1.29], [413, 1, 5, 0.51], [412, 1, 4, 1.0], [411, 2, 4, 0.46], [11739, 2, 4, 1.04], [10574, 3, 5, 1.26], [11835, 2, 4, 0.55], [145, 2, 5, 0.4], [21793, 1, 4, 1.38], [2775, 2, 4, 0.42], [1429, 2, 4, 0.48], [76, 2, 4, 1.11], [8675, 2, 4, 0.6], [8673, 2, 4, 1.45], [143, 2, 4, 0.65], [11836, 2, 4, 0.2], [8674, 2, 4, 0.49], [8938, 2, 4, 0.97], [146, 2, 4, 0.62], [6158, 2, 5, 1.33], [151, 1, 4, 0.57], [12720, 2, 4, 0.82], [10149, 3, 13, 0.39], [2776, 2, 4, 0.75], [3495, 3, 13, 0.85], [2055, 3, 4, 1.18], [75, 2, 4, 1.17], [2057, 3, 4, 1.0], [11738, 2, 4, 1.04], [144, 2, 4, 0.52], [8939, 2, 4, 0.94], [416, 1, 4, 0.73], [7885, 4, 5, 0.44], [22316, 3, 5, 0.19], [88, 10, 8, 0.95], [159, 3, 5, 0.72], [2859, 15, 4, 0.44], [7084, 3, 4, 1.75], [418, 2, 4, 0.2], [10993, 2, 4, 0.49], [20252, 2, 4, 0.37], [9784, 1, 4, 0.88], [7705, 2, 4, 1.15], [5165, 1, 4, 0.59], [12526, 2, 4, 0.74], [410, 1, 4, 0.47], [11844, 2, 4, 0.47], [414, 1, 4, 0.73], [12351, 1, 5, 0.61], [2423, 80, 5, 1.25], [378, 2, 4, 1.16], [2424, 29, 5, 0.55], [2423, 29, 4, 1.16], [12345, 1, 4, 0.61], [60, 3, 5, 2.26], [950, 1, 4, 0.39], [6494, 1, 4, 0.46], [11490, 1, 4, 0.48], [2424, 80, 4, 0.43], [13023, 3, 6, 1.51], [12373, 1, 5, 0.45], [13034, 3, 5, 1.37], [201, 3, 4, 1.1], [1519, 3, 9, 0.4], [11489, 1, 4, 0.37], [345, 3, 4, 0.76], [5208, 3, 5, 0.54], [11770, 1, 4, 0.48], [159, 1, 4, 0.73], [3, 2, 4, 3.1], [6952, 1, 4, 1.09], [3430, 15, 4, 1.23], [20927, 1, 4, 0.48], [11954, 1, 4, 0.42], [7886, 4, 5, 0.44], [432, 3, 4, 2.04], [3429, 15, 4, 0.46], [13928, 1, 4, 0.45], [11504, 2, 4, 0.2], [11811, 1, 4, 0.38], [566, 2, 4, 0.5], [5584, 3, 4, 1.36], [114, 3, 4, 1.64], [2331, 1, 4, 0.79], [10407, 10, 6, 1.18], [1492, 1, 4, 0.62], [105, 3, 4, 1.64], [1490, 1, 4, 1.38], [7004, 1, 4, 0.99], [11089, 1, 4, 0.39], [2703, 3, 4, 2.13], [6098, 80, 4, 1.16], [8274, 3, 4, 2.3], [11674, 1, 4, 0.36], [1886, 2, 4, 0.44], [12348, 1, 4, 0.61], [94, 4, 4, 1.77], [10410, 10, 6, 1.18], [3891, 1, 4, 2.39], [11953, 1, 4, 0.46], [22317, 3, 5, 0.52], [6097, 80, 4, 1.86], [141, 2, 156, 2.73], [2328, 2, 76, 3.53], [8650, 2, 114, 4.44], [362, 2, 72, 2.98], [5491, 2, 108, 2.9], [5493, 2, 55, 2.79], [130, 1, 30, 2.98], [589, 2, 153, 2.73], [2327, 2, 76, 3.26], [326, 2, 35, 3.64], [11685, 2, 138, 6.0], [8672, 2, 144, 3.33], [417, 2, 156, 2.81], [6935, 2, 141, 5.82], [205, 2, 109, 2.53], [11681, 2, 138, 5.84], [206, 2, 42, 2.64], [8648, 2, 114, 4.32], [6936, 2, 141, 5.23], [142, 2, 78, 3.03], [11837, 2, 269, 2.79], [12721, 2, 144, 3.19], [11838, 2, 134, 3.09], [2049, 3, 276, 3.27], [1446, 2, 76, 3.25], [523, 2, 156, 2.81], [615, 2, 107, 4.63], [8676, 2, 287, 4.22], [11737, 2, 57, 3.69], [305, 2, 74, 3.08], [616, 2, 107, 4.15], [413, 1, 44, 3.05], [412, 1, 42, 3.02], [411, 2, 109, 2.64], [11739, 2, 57, 3.69], [10574, 3, 501, 4.43], [11835, 2, 269, 2.79], [145, 2, 76, 2.84], [21793, 1, 238, 5.81], [2775, 2, 157, 2.56], [1429, 2, 153, 2.68], [76, 2, 109, 3.83], [8675, 2, 287, 3.21], [8673, 2, 284, 5.17], [143, 2, 148, 2.98], [11836, 2, 134, 2.89], [8674, 2, 287, 3.25], [8938, 2, 190, 3.57], [146, 2, 151, 2.93], [6158, 2, 260, 4.44], [151, 1, 33, 2.79], [12720, 2, 284, 3.48], [10149, 3, 872, 3.26], [2776, 2, 157, 3.16], [3495, 3, 965, 3.31], [2055, 3, 158, 4.31], [75, 2, 144, 3.94], [2057, 3, 158, 4.31], [11738, 2, 57, 3.69], [144, 2, 151, 2.74], [8939, 2, 63, 4.3], [416, 1, 86, 3.13], [7885, 4, 36, 2.38], [22316, 3, 159, 2.96], [88, 10, 561, 4.69], [159, 3, 709, 3.16], [2859, 15, 69, 2.6]]</t>
-  </si>
-  <si>
-    <t>[[326, 2, 4, 1.08], [6935, 2, 8, 0.99], [2049, 3, 8, 0.41], [362, 2, 4, 0.89], [589, 2, 5, 0.37], [75, 2, 4, 0.39], [141, 2, 4, 0.66], [1776, 1, 4, 0.2], [205, 2, 4, 0.38], [8915, 2, 5, 0.4], [2778, 2, 4, 0.2], [8672, 2, 6, 0.51], [6936, 2, 5, 1.05], [593, 2, 5, 0.44], [7886, 4, 4, 0.57], [305, 2, 4, 0.5], [206, 2, 4, 0.2], [151, 1, 5, 0.47], [8648, 2, 4, 1.08], [1777, 1, 4, 0.8], [2328, 2, 5, 0.35], [88, 10, 9, 0.55], [11681, 2, 5, 1.87], [990, 2, 4, 0.26], [8650, 2, 5, 1.09], [412, 1, 4, 0.62], [5151, 2, 4, 0.75], [2050, 3, 4, 0.8], [76, 2, 4, 0.56], [144, 2, 4, 0.49], [10149, 3, 17, 1.82], [345, 3, 5, 0.44], [2991, 3, 4, 1.6], [22247, 2, 4, 0.54], [57, 1, 4, 0.38], [3478, 2, 4, 0.89], [146, 2, 4, 1.0], [7004, 1, 5, 0.36], [45, 2, 4, 0.56], [2054, 3, 4, 0.51], [143, 2, 4, 0.46], [417, 2, 4, 0.46], [413, 1, 4, 0.81], [21793, 1, 5, 0.45], [167, 3, 5, 0.49], [201, 3, 5, 0.2], [74, 1, 4, 1.75], [1446, 2, 4, 0.54], [346, 1, 4, 0.2], [2055, 3, 5, 0.5], [168, 3, 4, 0.32], [10, 2, 4, 0.45], [7084, 3, 4, 0.36], [11234, 2, 4, 0.2], [1429, 2, 4, 0.2], [7036, 1, 4, 1.8], [12721, 2, 6, 0.49], [3495, 3, 13, 0.52], [5081, 2, 4, 0.44], [8649, 2, 4, 1.29], [308, 1, 5, 0.73], [13028, 3, 4, 0.47], [12870, 1, 4, 1.54], [10825, 21, 8, 1.34], [79, 1, 4, 0.38], [1492, 1, 4, 0.58], [96, 11, 14, 0.38], [23, 1, 4, 0.2], [1006, 2, 4, 0.55], [3893, 1, 5, 0.2], [418, 2, 4, 0.43], [1504, 2, 4, 0.2], [145, 2, 4, 0.43], [5208, 3, 6, 0.19], [9827, 3, 4, 0.2], [3891, 1, 4, 0.2], [432, 3, 5, 0.41], [7005, 1, 5, 0.36], [1490, 1, 5, 0.2], [8853, 2, 5, 1.01], [94, 4, 4, 1.24], [13260, 29, 4, 0.4], [5812, 3, 5, 2.01], [416, 1, 4, 0.81], [8651, 2, 4, 0.8], [12353, 1, 4, 1.55], [20256, 2, 4, 0.2], [8939, 2, 5, 0.2], [21269, 3, 4, 0.95], [13280, 1, 4, 0.81], [950, 1, 4, 0.46], [33, 1, 4, 0.53], [5086, 1, 5, 1.08], [998, 2, 5, 0.73], [9069, 1, 4, 0.97], [1243, 2, 4, 0.89], [229, 1, 4, 1.05], [2878, 1, 4, 0.74], [140, 2, 4, 0.63], [7567, 3, 4, 1.11], [2049, 1, 4, 0.2], [20927, 1, 4, 0.2], [126, 2, 5, 0.93], [346, 3, 5, 0.19], [1703, 2, 4, 0.41], [3980, 4, 4, 1.31], [8121, 3, 4, 0.53], [8274, 3, 4, 0.39], [35, 1, 4, 0.48], [9691, 1, 4, 1.09], [5209, 3, 4, 0.19], [997, 2, 4, 1.03], [11811, 1, 4, 1.0], [5584, 3, 4, 1.74], [1070, 7, 10, 0.2], [11914, 1, 5, 0.5], [1519, 3, 10, 0.4], [856, 1, 4, 0.38], [5660, 2, 5, 0.9], [8898, 3, 4, 2.43], [1091, 1, 4, 0.2], [5513, 2, 4, 0.43], [523, 2, 4, 0.63], [8926, 1, 4, 1.35], [11767, 1, 4, 0.48], [2775, 2, 4, 0.2], [9372, 1, 4, 0.39], [13034, 3, 5, 0.66], [9081, 3, 7, 1.8], [307, 2, 4, 1.14], [20255, 2, 5, 0.2], [12661, 1, 4, 0.97], [11808, 1, 5, 0.2], [326, 2, 84, 3.42], [6935, 2, 129, 4.09], [2049, 3, 192, 1.94], [362, 2, 131, 2.79], [589, 2, 142, 1.93], [75, 2, 51, 1.98], [141, 2, 143, 3.4], [1776, 1, 52, 1.74], [205, 2, 101, 1.85], [8915, 2, 179, 1.9], [2778, 2, 55, 2.06], [8672, 2, 100, 2.17], [6936, 2, 97, 4.51], [593, 2, 211, 2.16], [7886, 4, 132, 2.19], [305, 2, 51, 2.18], [206, 2, 39, 1.99], [151, 1, 31, 1.63], [8648, 2, 79, 3.41], [1777, 1, 39, 3.67], [2328, 2, 53, 1.92], [88, 10, 197, 2.3], [11681, 2, 95, 5.43], [990, 2, 30, 2.16], [8650, 2, 79, 3.43], [412, 1, 30, 2.41], [5151, 2, 14, 3.62], [2050, 3, 432, 3.55], [76, 2, 39, 2.3], [144, 2, 139, 2.06], [10149, 3, 300, 4.79], [345, 3, 106, 2.01], [2991, 3, 57, 4.91], [22247, 2, 99, 2.54], [57, 1, 79, 1.85], [3478, 2, 69, 3.31], [146, 2, 53, 2.18], [7004, 1, 28, 1.93], [45, 2, 39, 4.21], [2054, 3, 166, 2.21], [143, 2, 51, 2.11], [417, 2, 143, 2.0], [413, 1, 79, 3.28], [21793, 1, 85, 2.1], [167, 3, 80, 2.16], [201, 3, 106, 1.94], [74, 1, 71, 3.73], [1446, 2, 53, 3.18], [346, 1, 55, 2.05], [2055, 3, 166, 2.18], [168, 3, 141, 2.77], [10, 2, 97, 2.76], [7084, 3, 46, 1.93], [11234, 2, 65, 2.04], [1429, 2, 53, 2.47], [7036, 1, 45, 3.84], [12721, 2, 99, 2.13], [3495, 3, 336, 2.2], [5081, 2, 177, 1.96], [8649, 2, 79, 3.64], [308, 1, 58, 3.98], [13028, 3, 51, 2.14], [12870, 1, 49, 3.19], [10825, 21, 575, 3.62], [79, 1, 44, 1.85], [1492, 1, 13, 3.25], [96, 11, 784, 1.8]]</t>
-  </si>
-  <si>
-    <t>[[88, 10, 10, 0.93], [2327, 2, 4, 0.52], [8915, 2, 5, 1.08], [589, 2, 5, 0.2], [2778, 2, 4, 0.2], [6935, 2, 6, 1.77], [2328, 2, 4, 0.58], [5493, 2, 4, 1.23], [130, 1, 4, 0.98], [305, 2, 4, 0.45], [615, 2, 4, 0.2], [616, 2, 5, 0.2], [6936, 2, 5, 1.74], [326, 2, 5, 1.15], [8650, 2, 4, 0.39], [8648, 2, 4, 1.05], [1446, 2, 4, 0.2], [2049, 3, 5, 0.42], [10, 2, 4, 0.2], [143, 2, 5, 0.58], [159, 3, 5, 0.67], [593, 2, 4, 0.37], [205, 2, 4, 0.43], [5491, 2, 4, 0.58], [2775, 2, 4, 0.2], [7036, 1, 4, 0.94], [144, 2, 5, 0.53], [151, 1, 4, 0.59], [3840, 1, 5, 0.29], [94, 4, 4, 1.91], [434, 2, 5, 0.2], [8938, 2, 4, 0.52], [990, 2, 4, 0.2], [3893, 1, 4, 0.2], [8853, 2, 4, 1.79], [146, 2, 4, 1.07], [1504, 2, 4, 0.93], [624, 2, 4, 1.1], [12224, 1, 4, 0.46], [1429, 2, 4, 0.2], [3891, 1, 4, 0.2], [2776, 2, 4, 0.2], [206, 2, 4, 0.37], [2055, 3, 4, 0.46], [362, 2, 4, 0.5], [141, 2, 4, 0.39], [11681, 2, 5, 1.33], [11404, 2, 4, 0.2], [378, 2, 4, 1.16], [5208, 3, 5, 0.19], [3889, 1, 4, 0.35], [8649, 2, 4, 1.53], [1007, 2, 4, 0.46], [10574, 3, 5, 1.86], [10993, 2, 4, 0.7], [11234, 2, 4, 0.75], [7886, 4, 4, 0.46], [12870, 1, 5, 0.72], [21793, 1, 4, 0.5], [10149, 3, 15, 0.39], [3980, 4, 4, 0.73], [2050, 3, 4, 0.46], [12353, 1, 4, 0.66], [145, 2, 4, 1.01], [7084, 3, 4, 0.86], [11811, 1, 4, 0.44], [8672, 2, 4, 1.48], [20927, 1, 4, 0.95], [5165, 1, 4, 0.56], [998, 2, 4, 1.5], [9760, 29, 4, 0.37], [997, 2, 4, 1.42], [2436, 4, 4, 0.2], [1006, 2, 5, 0.54], [972, 3, 5, 0.51], [2424, 80, 4, 0.99], [346, 3, 5, 0.19], [3, 2, 4, 0.62], [229, 1, 4, 0.54], [6158, 2, 5, 0.48], [3495, 3, 11, 0.56], [12346, 1, 4, 0.66], [5165, 2, 5, 1.02], [7887, 4, 4, 0.47], [5076, 1, 4, 0.71], [126, 2, 4, 1.27], [20252, 2, 4, 0.38], [11953, 1, 4, 0.46], [9372, 1, 4, 1.42], [11770, 1, 4, 0.88], [140, 2, 4, 1.27], [12344, 1, 4, 0.66], [8939, 2, 4, 0.2], [11954, 1, 4, 0.38], [1492, 1, 4, 0.2], [11685, 2, 5, 1.33], [12352, 1, 4, 0.66], [996, 2, 4, 1.16], [12721, 2, 4, 2.31], [20256, 2, 4, 0.2], [2774, 2, 4, 0.63], [12350, 1, 4, 0.66], [3981, 3, 11, 0.23], [9491, 21, 12, 0.22], [5434, 1, 4, 1.0], [2423, 80, 5, 0.75], [12343, 1, 4, 0.66], [6497, 1, 4, 0.63], [5584, 3, 4, 1.75], [2438, 2, 6, 0.49], [10388, 2, 4, 0.37], [12351, 1, 4, 0.66], [10407, 10, 6, 1.18], [11179, 1, 4, 0.45], [6496, 1, 4, 1.73], [22317, 3, 4, 0.35], [7573, 1, 8, 2.02], [823, 1, 4, 0.55], [5209, 3, 5, 0.19], [8898, 3, 5, 1.44], [2805, 137, 4, 0.93], [3900, 3, 4, 1.76], [12526, 2, 4, 0.71], [2424, 29, 4, 0.55], [11812, 1, 4, 0.2], [4253, 1, 4, 0.54], [3975, 4, 5, 1.21], [11490, 1, 4, 0.35], [336, 15, 4, 0.97], [1622, 1, 4, 0.45], [12764, 2, 5, 0.54], [412, 1, 4, 0.44], [972, 1, 4, 1.02], [88, 10, 276, 3.94], [2327, 2, 74, 2.93], [8915, 2, 93, 2.96], [589, 2, 75, 2.97], [2778, 2, 77, 2.92], [6935, 2, 135, 6.0], [2328, 2, 74, 3.05], [5493, 2, 104, 3.91], [305, 2, 72, 2.8], [615, 2, 54, 3.01], [616, 2, 54, 2.64], [6936, 2, 135, 5.39], [326, 2, 44, 4.1], [8650, 2, 110, 3.45], [8648, 2, 110, 3.91], [1446, 2, 74, 3.2], [2049, 3, 360, 2.34], [10, 2, 52, 2.65], [143, 2, 72, 3.03], [159, 3, 690, 2.82], [593, 2, 223, 2.53], [205, 2, 54, 2.77], [5491, 2, 53, 3.05], [2775, 2, 77, 2.92], [7036, 1, 63, 4.28], [151, 1, 32, 2.68], [3840, 1, 84, 3.43], [94, 4, 60, 4.77], [434, 2, 53, 2.69], [8938, 2, 125, 2.43], [990, 2, 26, 2.69], [3893, 1, 61, 2.96], [8853, 2, 272, 5.15], [146, 2, 73, 3.02], [1504, 2, 99, 3.69], [624, 2, 104, 3.83], [12224, 1, 162, 2.49], [1429, 2, 74, 2.89], [3891, 1, 61, 2.96], [2776, 2, 77, 3.16], [206, 2, 106, 2.39], [2055, 3, 314, 2.32], [362, 2, 69, 2.89], [141, 2, 76, 2.69], [11681, 2, 131, 5.43], [11404, 2, 51, 3.15], [378, 2, 110, 4.11], [5208, 3, 273, 2.87], [3889, 1, 122, 2.29], [8649, 2, 218, 4.79], [1007, 2, 264, 2.49], [10993, 2, 54, 2.93], [11234, 2, 148, 3.27], [7886, 4, 70, 2.16], [12870, 1, 69, 3.3], [21793, 1, 119, 2.89], [10149, 3, 435, 3.88], [3980, 4, 234, 4.41], [2050, 3, 314, 2.32], [12353, 1, 612, 2.87], [145, 2, 73, 2.92], [7084, 3, 127, 3.22], [11811, 1, 447, 2.44], [8672, 2, 140, 4.92], [20927, 1, 30, 2.64], [5165, 1, 38, 3.97], [998, 2, 115, 4.81]]</t>
-  </si>
-  <si>
-    <t>[[6935, 2, 8, 1.31], [141, 2, 4, 0.4], [589, 2, 5, 0.2], [2778, 2, 4, 0.2], [6936, 2, 5, 0.71], [8648, 2, 4, 1.13], [362, 2, 4, 0.46], [2327, 2, 4, 0.39], [11681, 2, 9, 1.29], [8650, 2, 5, 0.84], [326, 2, 4, 0.77], [205, 2, 4, 0.2], [2328, 2, 4, 0.57], [1446, 2, 4, 0.28], [305, 2, 5, 0.88], [130, 1, 4, 0.2], [8649, 2, 5, 0.39], [2775, 2, 4, 0.2], [8853, 2, 5, 1.21], [361, 2, 4, 0.5], [2776, 2, 4, 0.2], [593, 2, 5, 0.48], [143, 2, 4, 1.13], [140, 2, 4, 0.77], [1429, 2, 4, 0.28], [206, 2, 4, 0.2], [5493, 2, 4, 0.51], [523, 2, 4, 0.4], [7004, 1, 4, 0.71], [413, 1, 4, 1.02], [7036, 1, 4, 1.58], [5491, 2, 4, 0.5], [412, 1, 4, 0.57], [21793, 1, 4, 1.03], [12350, 1, 4, 0.19], [1124, 2, 4, 0.64], [990, 2, 4, 0.2], [12353, 1, 5, 0.19], [5165, 1, 4, 0.42], [8915, 2, 5, 0.86], [615, 2, 4, 1.1], [583, 2, 4, 0.77], [417, 2, 4, 0.43], [21798, 1, 4, 0.36], [146, 2, 4, 0.64], [248, 1, 4, 0.2], [8089, 1, 4, 1.2], [434, 2, 5, 0.2], [201, 3, 5, 0.47], [142, 2, 4, 0.45], [6097, 80, 4, 0.38], [11770, 1, 4, 0.43], [6952, 1, 4, 1.71], [2055, 3, 4, 0.81], [345, 3, 4, 0.47], [3891, 1, 4, 0.98], [9372, 1, 4, 0.58], [2057, 3, 4, 0.81], [616, 2, 4, 0.86], [7084, 3, 4, 1.0], [3670, 2, 4, 1.47], [3893, 1, 4, 0.64], [5165, 2, 7, 1.41], [12346, 1, 4, 0.19], [12870, 1, 4, 1.18], [12343, 1, 4, 0.49], [10574, 3, 5, 1.39], [1886, 2, 4, 0.36], [2424, 80, 4, 0.43], [346, 3, 4, 0.2], [3334, 5, 5, 1.7], [20927, 1, 4, 0.38], [12351, 1, 4, 0.38], [7885, 4, 4, 0.53], [6098, 80, 4, 1.46], [6097, 29, 4, 0.88], [11089, 1, 4, 0.44], [12345, 1, 4, 0.47], [10149, 3, 13, 0.91], [20256, 2, 4, 0.2], [147, 1, 4, 0.53], [22316, 3, 4, 0.36], [1492, 1, 4, 0.58], [11953, 1, 4, 0.44], [432, 3, 5, 0.62], [11491, 2, 4, 0.51], [20252, 2, 4, 0.2], [418, 2, 4, 0.72], [4032, 29, 4, 0.47], [1490, 1, 4, 0.42], [1519, 3, 10, 0.4], [2423, 80, 4, 1.66], [11952, 1, 4, 0.46], [411, 2, 4, 0.5], [5151, 2, 4, 0.62], [229, 1, 4, 2.07], [12304, 1, 4, 0.64], [972, 3, 5, 0.46], [11769, 1, 4, 0.48], [3576, 25, 4, 0.91], [2331, 1, 4, 1.19], [346, 1, 4, 0.2], [13034, 3, 5, 1.29], [995, 2, 4, 0.41], [416, 1, 4, 0.99], [2424, 29, 4, 0.41], [3, 2, 4, 0.55], [11426, 25, 4, 0.58], [11737, 2, 4, 0.5], [11767, 1, 4, 0.48], [5076, 1, 4, 0.64], [439, 1, 4, 1.47], [11490, 1, 4, 0.56], [2805, 137, 4, 0.98], [2160, 68, 4, 0.56], [6494, 1, 4, 1.59], [950, 1, 4, 0.36], [414, 1, 4, 0.66], [3575, 25, 4, 0.98], [12764, 2, 5, 0.51], [8677, 3, 5, 1.11], [1701, 2, 4, 1.97], [11180, 1, 4, 0.54], [11586, 1, 7, 1.42], [75, 2, 4, 0.37], [3577, 25, 4, 0.42], [3478, 2, 4, 0.9], [11585, 29, 4, 1.12], [9998, 80, 4, 0.42], [11813, 1, 4, 1.11], [13023, 3, 5, 1.01], [2438, 2, 5, 1.05], [9784, 1, 4, 0.88], [6935, 2, 108, 5.03], [141, 2, 60, 2.71], [589, 2, 60, 2.6], [2778, 2, 60, 2.86], [6936, 2, 108, 5.43], [8648, 2, 88, 3.75], [362, 2, 55, 2.52], [2327, 2, 129, 3.02], [11681, 2, 105, 4.91], [8650, 2, 88, 3.23], [326, 2, 78, 2.83], [205, 2, 70, 2.22], [2328, 2, 59, 2.74], [1446, 2, 59, 3.11], [305, 2, 57, 3.31], [130, 1, 38, 1.55], [8649, 2, 88, 3.7], [2775, 2, 60, 2.86], [8853, 2, 108, 4.93], [361, 2, 60, 2.6], [2776, 2, 60, 2.86], [593, 2, 89, 2.55], [143, 2, 57, 3.07], [140, 2, 78, 2.83], [1429, 2, 59, 3.41], [206, 2, 42, 2.51], [5493, 2, 93, 2.36], [523, 2, 60, 2.68], [7004, 1, 68, 2.72], [413, 1, 33, 2.92], [7036, 1, 50, 3.67], [5491, 2, 93, 2.34], [412, 1, 72, 2.66], [21793, 1, 208, 5.07], [12350, 1, 243, 2.38], [1124, 2, 161, 2.69], [990, 2, 21, 2.5], [12353, 1, 243, 2.43], [5165, 1, 30, 3.83], [8915, 2, 163, 2.9], [615, 2, 92, 3.67], [583, 2, 78, 2.83], [417, 2, 60, 2.48], [21798, 1, 120, 2.36], [146, 2, 129, 4.34], [248, 1, 15, 2.08], [8089, 1, 61, 3.62], [434, 2, 42, 2.58], [201, 3, 119, 2.55], [142, 2, 133, 2.61], [6097, 80, 27, 5.58], [11770, 1, 189, 2.22], [6952, 1, 74, 4.06], [2055, 3, 410, 2.91], [345, 3, 119, 2.55], [3891, 1, 107, 3.22], [9372, 1, 195, 2.96], [2057, 3, 410, 2.91], [616, 2, 92, 3.0], [7084, 3, 51, 3.51], [3670, 2, 212, 4.13], [3893, 1, 107, 3.22], [12346, 1, 243, 2.38], [12870, 1, 119, 3.63], [12343, 1, 536, 2.3], [10574, 3, 198, 3.24], [1886, 2, 135, 2.08]]</t>
-  </si>
-  <si>
-    <t>[[6935, 2, 5, 1.18], [615, 2, 4, 1.69], [2778, 2, 5, 0.2], [305, 2, 4, 0.48], [5493, 2, 4, 1.52], [6936, 2, 4, 1.18], [130, 1, 4, 0.47], [205, 2, 4, 0.53], [616, 2, 4, 1.5], [1504, 2, 5, 0.57], [144, 2, 4, 0.53], [8648, 2, 4, 0.7], [2049, 3, 7, 0.41], [88, 10, 8, 0.37], [8915, 2, 5, 1.45], [326, 2, 4, 1.12], [7036, 1, 4, 1.57], [8650, 2, 5, 0.57], [593, 2, 5, 0.45], [2327, 2, 5, 0.47], [11681, 2, 4, 1.35], [8853, 2, 4, 1.18], [141, 2, 4, 0.48], [2775, 2, 5, 0.2], [206, 2, 4, 0.2], [151, 1, 4, 0.59], [7004, 1, 5, 0.35], [248, 1, 4, 0.43], [11685, 2, 4, 1.88], [3891, 1, 5, 0.2], [3840, 1, 4, 0.39], [2328, 2, 4, 0.5], [2050, 3, 5, 0.34], [5491, 2, 4, 0.54], [2497, 2, 4, 0.83], [2055, 3, 4, 1.73], [143, 2, 4, 0.58], [434, 2, 4, 0.47], [3980, 4, 4, 1.2], [2054, 3, 4, 0.34], [624, 2, 4, 1.35], [8672, 2, 4, 0.48], [362, 2, 4, 0.85], [8649, 2, 4, 1.53], [2776, 2, 4, 0.67], [12870, 1, 4, 0.92], [2057, 3, 5, 0.34], [12350, 1, 4, 0.66], [7886, 4, 5, 0.45], [10574, 3, 5, 1.86], [5165, 1, 4, 0.58], [1006, 2, 4, 0.58], [1446, 2, 4, 0.39], [94, 4, 4, 0.84], [75, 2, 4, 1.49], [523, 2, 4, 1.0], [2991, 3, 5, 1.1], [3495, 3, 13, 0.85], [7084, 3, 4, 0.58], [7005, 1, 4, 0.94], [3975, 4, 4, 1.26], [21793, 1, 4, 2.3], [10149, 3, 13, 0.39], [9760, 29, 4, 0.2], [11404, 2, 5, 0.2], [142, 2, 4, 0.51], [12346, 1, 4, 0.66], [6158, 2, 5, 0.2], [20927, 1, 4, 0.67], [3981, 3, 15, 1.15], [417, 2, 4, 0.66], [5165, 2, 5, 1.11], [2912, 1, 4, 0.2], [3982, 3, 10, 1.18], [8939, 2, 4, 0.2], [1007, 2, 4, 0.51], [11953, 1, 4, 0.45], [2774, 2, 4, 1.06], [33, 1, 4, 1.06], [956, 2, 4, 0.47], [11772, 1, 5, 1.35], [286, 3, 5, 1.06], [7887, 4, 5, 0.44], [6497, 1, 4, 0.93], [1492, 1, 4, 0.7], [11767, 1, 4, 0.2], [432, 3, 4, 0.47], [336, 15, 4, 1.12], [972, 3, 4, 1.07], [11769, 1, 4, 0.2], [11490, 1, 4, 1.04], [11770, 1, 4, 0.48], [410, 1, 5, 0.54], [389, 4, 5, 0.38], [2912, 2, 5, 0.47], [74, 1, 4, 1.16], [6496, 1, 4, 0.47], [7567, 3, 4, 1.65], [1413, 15, 4, 0.2], [35, 1, 5, 0.57], [411, 2, 4, 0.5], [4253, 1, 4, 0.82], [22317, 3, 4, 0.51], [140, 2, 4, 0.93], [8673, 2, 4, 0.47], [8121, 3, 5, 0.2], [1126, 2, 4, 0.58], [4176, 4, 4, 1.31], [2436, 4, 4, 0.2], [9372, 1, 4, 1.7], [8676, 2, 4, 1.7], [21269, 3, 4, 2.24], [8677, 3, 5, 0.4], [22247, 2, 4, 1.38], [10388, 2, 4, 1.08], [10936, 2, 4, 1.7], [12343, 1, 4, 0.66], [12526, 2, 4, 1.08], [11085, 2, 5, 1.27], [9784, 1, 4, 0.55], [12269, 2, 4, 1.03], [37, 1, 4, 0.66], [6494, 1, 5, 0.29], [1274, 1, 4, 0.23], [13023, 3, 4, 1.26], [1429, 2, 4, 0.5], [7573, 1, 5, 1.35], [12225, 1, 4, 0.69], [345, 3, 4, 1.31], [12271, 2, 4, 1.01], [3, 2, 4, 0.38], [3577, 25, 4, 0.48], [96, 11, 12, 0.38], [6935, 2, 108, 5.9], [615, 2, 91, 4.78], [2778, 2, 61, 2.77], [305, 2, 57, 2.58], [5493, 2, 91, 4.44], [6936, 2, 108, 5.92], [130, 1, 24, 2.58], [205, 2, 42, 2.69], [616, 2, 91, 4.41], [1504, 2, 80, 2.75], [144, 2, 59, 4.4], [8648, 2, 89, 2.99], [2049, 3, 144, 2.25], [88, 10, 220, 3.45], [8915, 2, 65, 4.29], [326, 2, 36, 3.57], [7036, 1, 50, 3.83], [8650, 2, 89, 2.75], [593, 2, 89, 2.78], [2327, 2, 59, 2.57], [11681, 2, 106, 5.01], [8853, 2, 108, 5.93], [141, 2, 61, 2.6], [2775, 2, 61, 2.77], [206, 2, 42, 2.55], [151, 1, 58, 2.7], [7004, 1, 31, 2.36], [248, 1, 47, 2.25], [11685, 2, 106, 5.4], [3891, 1, 49, 2.88], [3840, 1, 150, 2.17], [2328, 2, 59, 2.62], [2050, 3, 188, 2.34], [5491, 2, 91, 3.06], [2497, 2, 174, 4.13], [2055, 3, 396, 4.86], [143, 2, 58, 2.77], [434, 2, 56, 2.07], [3980, 4, 186, 4.07], [2054, 3, 188, 2.34], [624, 2, 91, 5.38], [8672, 2, 112, 4.65], [362, 2, 55, 3.27], [8649, 2, 194, 4.25], [2776, 2, 61, 3.86], [12870, 1, 117, 5.16], [2057, 3, 188, 2.34], [12350, 1, 543, 2.67], [7886, 4, 38, 2.23], [10574, 3, 196, 4.07], [5165, 1, 30, 3.74], [1006, 2, 197, 2.83], [1446, 2, 60, 2.62], [94, 4, 47, 5.25], [75, 2, 57, 3.52], [523, 2, 60, 2.64], [2991, 3, 63, 5.99], [3495, 3, 832, 2.92], [7084, 3, 51, 2.79], [7005, 1, 68, 3.18], [3975, 4, 186, 4.2], [21793, 1, 90, 5.26], [10149, 3, 752, 2.93], [9760, 29, 28, 2.5], [11404, 2, 41, 2.88], [142, 2, 133, 2.39], [12346, 1, 543, 2.67]]</t>
-  </si>
-  <si>
-    <t>[[6935, 2, 7, 1.38], [305, 2, 4, 0.53], [2328, 2, 4, 0.78], [130, 1, 4, 0.2], [141, 2, 5, 0.2], [2778, 2, 5, 0.47], [8650, 2, 4, 1.17], [5491, 2, 4, 0.63], [2327, 2, 4, 0.63], [8672, 2, 6, 0.58], [6936, 2, 4, 1.4], [143, 2, 4, 1.14], [11681, 2, 5, 1.41], [248, 1, 4, 0.46], [145, 2, 4, 0.4], [205, 2, 4, 0.56], [5493, 2, 4, 1.24], [146, 2, 4, 0.56], [417, 2, 4, 0.52], [589, 2, 4, 0.2], [75, 2, 4, 0.37], [11838, 2, 4, 0.57], [11737, 2, 4, 0.38], [1124, 2, 6, 0.2], [523, 2, 5, 0.2], [8648, 2, 4, 1.54], [8853, 2, 4, 1.38], [12721, 2, 6, 0.47], [615, 2, 4, 1.28], [1005, 2, 4, 0.2], [326, 2, 5, 0.47], [206, 2, 5, 0.2], [8915, 2, 4, 0.2], [8673, 2, 4, 0.74], [144, 2, 5, 0.44], [11739, 2, 4, 0.38], [434, 2, 4, 0.73], [88, 10, 9, 0.82], [2776, 2, 4, 0.41], [435, 2, 5, 0.49], [142, 2, 4, 0.2], [151, 1, 4, 0.57], [8676, 2, 4, 0.47], [6158, 2, 5, 0.2], [2424, 29, 4, 0.2], [8649, 2, 4, 1.19], [2423, 29, 4, 1.81], [11738, 2, 4, 0.38], [2497, 2, 4, 0.55], [7704, 2, 4, 1.08], [2424, 80, 4, 0.49], [1413, 15, 4, 0.77], [10574, 3, 6, 1.26], [2423, 80, 4, 1.75], [3670, 2, 4, 0.97], [11836, 2, 5, 0.2], [7705, 2, 4, 1.15], [2054, 3, 4, 0.4], [3, 2, 4, 0.43], [2859, 15, 4, 1.25], [412, 1, 4, 0.58], [7706, 2, 4, 1.08], [378, 2, 4, 2.48], [12720, 2, 4, 0.98], [22316, 3, 4, 0.46], [2055, 3, 4, 0.47], [12344, 1, 4, 0.48], [3478, 2, 4, 1.07], [10149, 3, 13, 1.12], [74, 1, 5, 1.47], [3429, 15, 4, 0.46], [2774, 2, 4, 0.55], [307, 2, 4, 1.5], [6497, 1, 4, 0.44], [60, 3, 5, 0.41], [12526, 2, 4, 1.43], [418, 2, 4, 0.81], [7004, 1, 4, 1.02], [13928, 1, 4, 0.2], [411, 2, 4, 0.49], [11089, 1, 4, 0.39], [413, 1, 4, 0.54], [2057, 3, 4, 0.4], [14037, 3, 4, 0.96], [11844, 2, 5, 0.2], [2050, 3, 4, 0.4], [7036, 1, 4, 0.43], [20252, 2, 4, 0.58], [13260, 29, 4, 0.67], [3893, 1, 5, 0.44], [8274, 3, 4, 0.88], [6097, 80, 4, 0.64], [439, 1, 4, 0.37], [6952, 1, 4, 1.09], [3891, 1, 4, 2.08], [94, 4, 5, 1.09], [159, 3, 5, 0.72], [6494, 1, 4, 0.46], [9784, 1, 4, 0.55], [1050, 2, 4, 0.36], [7707, 2, 4, 0.72], [1490, 1, 4, 1.02], [1413, 16, 4, 0.39], [11490, 1, 4, 0.47], [1243, 2, 5, 0.2], [7708, 2, 4, 1.15], [414, 1, 4, 0.66], [3889, 1, 5, 0.37], [1492, 1, 4, 0.62], [5208, 3, 5, 0.97], [565, 2, 4, 0.46], [22317, 3, 5, 0.52], [7703, 2, 4, 1.15], [21793, 1, 4, 0.95], [11491, 2, 4, 0.81], [3495, 3, 13, 0.85], [229, 1, 4, 2.0], [345, 3, 4, 1.26], [2422, 80, 4, 1.75], [6098, 80, 4, 1.14], [410, 1, 4, 0.4], [11504, 2, 4, 0.72], [149, 2, 4, 0.52], [947, 15, 4, 0.39], [6630, 3, 4, 1.31], [3674, 2, 4, 0.52], [147, 1, 4, 0.52], [3430, 15, 4, 1.23], [416, 1, 4, 1.59], [2805, 137, 6, 1.85], [2331, 1, 4, 0.73], [247, 1, 4, 1.18], [9126, 1, 4, 0.47], [6935, 2, 141, 6.0], [305, 2, 74, 3.08], [2328, 2, 76, 3.53], [130, 1, 49, 2.48], [141, 2, 78, 2.84], [2778, 2, 156, 3.07], [8650, 2, 114, 4.87], [5491, 2, 106, 4.31], [2327, 2, 76, 3.26], [8672, 2, 144, 3.33], [6936, 2, 141, 5.42], [11681, 2, 276, 5.75], [248, 1, 37, 2.46], [145, 2, 76, 2.84], [205, 2, 109, 2.81], [5493, 2, 106, 4.23], [146, 2, 76, 3.13], [417, 2, 78, 3.05], [589, 2, 77, 2.91], [75, 2, 145, 3.58], [11838, 2, 269, 2.83], [11737, 2, 57, 2.97], [1124, 2, 95, 2.98], [523, 2, 78, 3.36], [8648, 2, 114, 4.01], [8853, 2, 141, 4.82], [12721, 2, 144, 3.19], [615, 2, 108, 4.14], [326, 2, 35, 3.64], [206, 2, 42, 2.64], [8915, 2, 96, 2.87], [8673, 2, 144, 5.05], [144, 2, 76, 2.91], [11739, 2, 57, 2.97], [434, 2, 107, 3.23], [88, 10, 285, 3.62], [2776, 2, 78, 3.77], [435, 2, 54, 3.01], [142, 2, 78, 3.16], [151, 1, 33, 2.79], [8676, 2, 144, 2.97], [6158, 2, 133, 2.82], [2424, 29, 17, 3.17], [8649, 2, 114, 3.38], [2423, 29, 18, 4.52], [11738, 2, 57, 2.97], [2497, 2, 105, 3.11], [7704, 2, 90, 3.18], [2424, 80, 84, 3.11], [10574, 3, 249, 4.6], [2423, 80, 92, 4.41], [3670, 2, 236, 5.41], [11836, 2, 134, 2.89], [7705, 2, 176, 4.07], [2054, 3, 473, 3.89], [3, 2, 61, 2.9], [2859, 15, 35, 3.48], [412, 1, 42, 3.17], [7706, 2, 90, 3.18], [378, 2, 224, 6.0], [12720, 2, 144, 2.99], [22316, 3, 318, 2.64], [2055, 3, 181, 2.76], [12344, 1, 620, 2.67], [3478, 2, 38, 4.08], [10149, 3, 866, 4.0], [74, 1, 102, 5.0]]</t>
-  </si>
-  <si>
-    <t>[[8672, 2, 6, 0.26], [305, 2, 4, 0.56], [3, 2, 4, 0.53], [6935, 2, 8, 1.37], [205, 2, 4, 0.47], [143, 2, 4, 0.43], [144, 2, 4, 0.26], [75, 2, 4, 0.49], [12721, 2, 6, 0.56], [145, 2, 4, 0.26], [8915, 2, 6, 0.2], [2778, 2, 4, 0.2], [1776, 1, 4, 0.45], [146, 2, 4, 0.26], [206, 2, 4, 0.56], [20252, 2, 4, 0.48], [6936, 2, 5, 1.3], [1777, 1, 4, 1.16], [8648, 2, 4, 0.89], [151, 1, 4, 0.35], [2328, 2, 4, 0.73], [8650, 2, 4, 1.0], [5151, 2, 4, 0.9], [2050, 3, 4, 0.73], [248, 1, 4, 0.44], [7886, 4, 5, 0.39], [88, 10, 8, 1.09], [9507, 3, 4, 0.36], [74, 1, 4, 0.8], [1446, 2, 4, 0.59], [2991, 3, 4, 1.1], [362, 2, 4, 0.43], [7004, 1, 4, 0.54], [2057, 3, 4, 0.56], [1492, 1, 4, 0.51], [1007, 2, 5, 0.2], [2055, 3, 4, 0.57], [147, 1, 4, 1.02], [76, 2, 4, 0.74], [8649, 2, 4, 1.05], [3889, 1, 4, 0.44], [11234, 2, 6, 0.2], [410, 1, 4, 0.38], [7005, 1, 4, 0.5], [345, 3, 4, 0.47], [10, 2, 5, 0.41], [1429, 2, 4, 0.28], [307, 2, 4, 1.75], [10825, 21, 8, 0.55], [5081, 2, 4, 0.54], [12870, 1, 4, 0.65], [57, 1, 4, 0.43], [10149, 3, 13, 0.71], [7036, 1, 4, 0.94], [3478, 2, 4, 0.54], [7084, 3, 4, 0.87], [1006, 2, 4, 0.56], [1504, 2, 4, 0.2], [3891, 1, 4, 0.2], [21793, 1, 4, 0.89], [94, 4, 4, 1.55], [167, 3, 4, 0.75], [411, 2, 4, 0.47], [9827, 3, 4, 0.2], [3893, 1, 4, 0.2], [79, 1, 4, 0.57], [33, 1, 4, 0.76], [432, 3, 5, 0.62], [8677, 3, 5, 0.4], [11681, 2, 6, 0.82], [148, 1, 4, 1.5], [96, 11, 15, 0.38], [1490, 1, 5, 0.2], [12225, 1, 4, 0.43], [1124, 2, 5, 0.2], [11737, 2, 4, 0.2], [1243, 2, 4, 0.5], [22247, 2, 6, 0.89], [6158, 2, 5, 0.8], [5812, 3, 5, 1.51], [8853, 2, 5, 1.32], [201, 3, 4, 0.47], [412, 1, 4, 1.28], [9760, 29, 4, 0.24], [10574, 3, 6, 1.33], [8651, 2, 5, 0.61], [20927, 1, 4, 0.43], [5208, 3, 5, 0.54], [8676, 2, 6, 0.56], [229, 1, 4, 1.2], [1767, 25, 4, 0.59], [25, 1, 4, 0.76], [45, 2, 4, 1.37], [9069, 1, 4, 0.41], [413, 1, 4, 1.19], [11490, 1, 4, 0.36], [149, 2, 4, 1.7], [159, 3, 5, 0.63], [3495, 3, 15, 0.92], [998, 2, 4, 0.97], [21269, 3, 4, 1.0], [140, 2, 4, 0.78], [95, 3, 10, 0.93], [3980, 4, 5, 1.25], [950, 1, 4, 0.71], [5946, 1, 4, 0.95], [9372, 1, 4, 2.03], [1126, 2, 5, 0.47], [1766, 25, 4, 0.56], [2775, 2, 5, 0.2], [1413, 15, 5, 0.78], [490, 1, 4, 0.4], [506, 1, 4, 1.21], [8674, 2, 5, 0.54], [11489, 1, 4, 0.56], [8898, 3, 4, 0.75], [997, 2, 4, 1.82], [3670, 2, 4, 1.87], [1070, 7, 9, 0.46], [9691, 1, 4, 0.98], [107, 2, 4, 0.52], [974, 3, 5, 0.38], [20498, 1, 4, 0.94], [11954, 1, 4, 0.47], [14037, 3, 5, 0.44], [823, 1, 4, 0.84], [14017, 3, 4, 0.44], [34, 1, 4, 1.26], [972, 3, 5, 0.85], [5209, 3, 4, 0.54], [9784, 1, 5, 0.55], [11739, 2, 4, 0.2], [20498, 3, 6, 0.36], [8672, 2, 229, 4.11], [305, 2, 115, 3.11], [3, 2, 97, 3.34], [6935, 2, 136, 4.9], [205, 2, 53, 2.52], [143, 2, 117, 3.77], [144, 2, 119, 4.38], [75, 2, 71, 2.56], [12721, 2, 138, 2.64], [145, 2, 119, 3.97], [8915, 2, 93, 2.53], [2778, 2, 75, 2.63], [1776, 1, 72, 1.98], [146, 2, 119, 3.97], [206, 2, 93, 2.33], [20252, 2, 79, 2.19], [6936, 2, 136, 4.39], [1777, 1, 54, 3.8], [8648, 2, 109, 3.3], [151, 1, 54, 1.81], [2328, 2, 72, 3.01], [8650, 2, 109, 3.51], [5151, 2, 12, 4.59], [2050, 3, 204, 2.91], [248, 1, 46, 2.11], [7886, 4, 69, 2.38], [88, 10, 273, 4.1], [9507, 3, 86, 1.53], [74, 1, 98, 3.13], [1446, 2, 73, 3.67], [2991, 3, 78, 5.3], [362, 2, 69, 2.45], [7004, 1, 51, 2.45], [2057, 3, 408, 2.32], [1492, 1, 30, 2.52], [1007, 2, 130, 2.48], [2055, 3, 408, 2.35], [147, 1, 74, 5.47], [76, 2, 53, 3.03], [8649, 2, 109, 3.59], [3889, 1, 106, 2.11], [11234, 2, 88, 2.92], [410, 1, 90, 2.0], [7005, 1, 68, 2.22], [345, 3, 147, 2.53], [10, 2, 51, 3.33], [1429, 2, 73, 3.12], [307, 2, 70, 3.95], [10825, 21, 303, 2.64], [5081, 2, 91, 2.66], [12870, 1, 68, 2.86], [57, 1, 73, 2.09], [10149, 3, 431, 2.87], [7036, 1, 62, 3.26], [3478, 2, 64, 2.3], [7084, 3, 63, 3.26], [1006, 2, 110, 2.7], [1504, 2, 99, 2.66], [3891, 1, 60, 3.37], [21793, 1, 202, 4.74], [94, 4, 58, 4.72], [167, 3, 110, 3.03], [411, 2, 53, 2.52], [9827, 3, 42, 2.54], [3893, 1, 60, 2.31], [79, 1, 41, 2.38], [33, 1, 54, 3.19]]</t>
-  </si>
-  <si>
-    <t>[[8672, 2, 6, 0.55], [305, 2, 4, 0.57], [2049, 3, 10, 0.2], [6935, 2, 8, 1.1], [326, 2, 4, 1.08], [141, 2, 4, 0.66], [144, 2, 5, 0.36], [589, 2, 5, 0.2], [362, 2, 4, 0.2], [151, 1, 5, 0.48], [12721, 2, 6, 0.56], [146, 2, 5, 0.41], [1776, 1, 4, 1.16], [145, 2, 4, 0.44], [206, 2, 4, 0.2], [2328, 2, 5, 0.73], [8915, 2, 6, 0.2], [143, 2, 4, 0.58], [990, 2, 5, 0.26], [6936, 2, 5, 1.55], [20252, 2, 4, 0.5], [8650, 2, 4, 1.18], [1777, 1, 4, 0.93], [1007, 2, 5, 0.39], [2778, 2, 5, 0.2], [248, 1, 4, 0.2], [22247, 2, 4, 0.78], [88, 10, 9, 1.09], [2050, 3, 5, 0.38], [76, 2, 4, 1.24], [8649, 2, 5, 1.22], [10149, 3, 17, 1.82], [2054, 3, 4, 1.44], [10, 2, 5, 0.91], [8677, 3, 6, 1.56], [412, 1, 4, 0.62], [2055, 3, 4, 1.36], [13028, 3, 4, 0.75], [413, 1, 4, 1.1], [7004, 1, 4, 0.36], [411, 2, 4, 0.48], [10825, 21, 8, 1.28], [11681, 2, 5, 1.87], [1446, 2, 4, 0.54], [7084, 3, 4, 0.86], [307, 2, 4, 0.47], [3478, 2, 4, 0.89], [1429, 2, 4, 0.2], [3495, 3, 15, 0.92], [1006, 2, 5, 0.47], [5081, 2, 4, 0.44], [1492, 1, 4, 0.58], [140, 2, 5, 0.63], [7005, 1, 4, 0.36], [167, 3, 4, 1.25], [7036, 1, 4, 1.11], [9827, 3, 5, 0.2], [45, 2, 5, 0.56], [8676, 2, 4, 0.51], [1124, 2, 6, 0.2], [2049, 1, 4, 0.93], [94, 4, 4, 1.74], [13280, 1, 4, 1.47], [5812, 3, 5, 2.01], [1504, 2, 4, 0.2], [12870, 1, 4, 0.54], [168, 3, 4, 0.29], [11234, 2, 4, 0.63], [415, 1, 4, 1.07], [8651, 2, 4, 0.78], [148, 1, 4, 0.52], [418, 2, 4, 0.38], [6097, 29, 4, 1.14], [8853, 2, 5, 1.07], [416, 1, 4, 1.21], [8939, 2, 4, 0.2], [6097, 80, 4, 1.14], [11737, 2, 5, 0.2], [20256, 2, 5, 0.2], [1490, 1, 5, 0.2], [95, 3, 16, 0.19], [20927, 1, 4, 0.36], [79, 1, 4, 0.38], [6098, 29, 4, 1.08], [14017, 3, 4, 0.52], [6098, 80, 4, 1.08], [414, 1, 4, 0.81], [9069, 1, 4, 0.99], [1070, 7, 10, 0.2], [8898, 3, 5, 1.36], [1126, 2, 5, 0.39], [13034, 3, 6, 0.66], [126, 2, 4, 1.43], [20498, 1, 5, 0.8], [9760, 29, 4, 0.45], [5086, 1, 4, 0.71], [20255, 2, 5, 0.2], [12924, 1, 5, 0.2], [5513, 2, 4, 0.46], [9784, 1, 4, 0.55], [336, 15, 4, 0.86], [13260, 29, 4, 0.54], [22317, 3, 6, 0.51], [7567, 3, 4, 1.66], [1413, 15, 4, 0.33], [229, 1, 4, 1.05], [11085, 2, 4, 0.45], [5811, 3, 5, 1.26], [5813, 3, 5, 1.08], [192, 3, 11, 1.1], [8557, 3, 4, 0.2], [9082, 3, 17, 1.28], [506, 1, 4, 0.52], [3049, 3, 5, 1.6], [20498, 3, 5, 0.86], [9691, 1, 4, 1.0], [14018, 3, 4, 0.52], [524, 1, 4, 1.12], [4076, 3, 4, 1.54], [470, 1, 5, 0.2], [8943, 3, 5, 0.7], [1622, 1, 5, 0.38], [9372, 1, 4, 0.39], [20486, 3, 6, 0.79], [2775, 2, 5, 0.2], [13023, 3, 6, 1.24], [1703, 2, 4, 0.41], [11454, 2, 6, 1.6], [2423, 80, 4, 1.41], [3900, 3, 4, 1.63], [5584, 3, 5, 1.22], [2424, 80, 4, 2.04], [2497, 2, 4, 0.43], [8672, 2, 100, 2.23], [305, 2, 51, 2.31], [2049, 3, 192, 1.94], [6935, 2, 129, 4.34], [326, 2, 84, 3.42], [141, 2, 143, 3.4], [144, 2, 53, 1.93], [589, 2, 53, 2.26], [362, 2, 50, 2.1], [151, 1, 24, 2.16], [12721, 2, 99, 2.25], [146, 2, 53, 2.03], [1776, 1, 100, 3.34], [145, 2, 139, 1.96], [206, 2, 39, 1.99], [2328, 2, 53, 2.62], [8915, 2, 67, 2.05], [143, 2, 51, 2.33], [990, 2, 18, 2.66], [6936, 2, 97, 4.51], [20252, 2, 86, 2.06], [8650, 2, 79, 3.42], [1777, 1, 100, 4.11], [1007, 2, 250, 1.96], [2778, 2, 55, 2.06], [22247, 2, 99, 3.12], [88, 10, 197, 3.28], [2050, 3, 166, 1.95], [76, 2, 39, 2.63], [8649, 2, 79, 3.51], [10149, 3, 300, 4.79], [2054, 3, 324, 5.02], [10, 2, 62, 2.92], [8677, 3, 102, 4.35], [412, 1, 30, 2.41], [2055, 3, 324, 5.02], [13028, 3, 135, 2.54], [413, 1, 30, 2.36], [7004, 1, 28, 1.93], [411, 2, 101, 2.04], [10825, 21, 575, 3.49], [11681, 2, 95, 5.53], [1446, 2, 53, 3.18], [7084, 3, 46, 1.93], [307, 2, 51, 2.12], [3478, 2, 69, 3.31], [1429, 2, 53, 2.47], [3495, 3, 336, 2.89], [1006, 2, 80, 2.13], [5081, 2, 177, 1.96], [1492, 1, 13, 3.25], [140, 2, 32, 2.75], [7005, 1, 28, 1.93], [167, 3, 80, 3.59], [7036, 1, 45, 2.39], [9827, 3, 30, 2.15], [45, 2, 39, 4.21], [8676, 2, 100, 2.21], [1124, 2, 65, 2.07], [2049, 1, 21, 2.85], [94, 4, 42, 4.73], [13280, 1, 111, 3.97], [5812, 3, 543, 4.52], [1504, 2, 72, 2.1], [12870, 1, 49, 2.27], [168, 3, 141, 2.73], [11234, 2, 170, 2.47]]</t>
-  </si>
-  <si>
-    <t>[[11685, 2, 4, 1.88], [6935, 2, 5, 1.18], [326, 2, 4, 1.12], [8648, 2, 4, 0.7], [144, 2, 4, 0.2], [593, 2, 5, 0.45], [2327, 2, 4, 0.47], [143, 2, 4, 0.58], [205, 2, 5, 0.53], [8915, 2, 5, 1.45], [2328, 2, 4, 0.5], [6936, 2, 4, 1.18], [11681, 2, 4, 1.35], [305, 2, 5, 0.48], [151, 1, 4, 0.59], [8650, 2, 4, 0.57], [141, 2, 4, 0.48], [206, 2, 5, 0.46], [2778, 2, 5, 0.2], [2049, 3, 8, 0.41], [88, 10, 10, 0.37], [615, 2, 4, 1.69], [7036, 1, 4, 1.57], [8853, 2, 4, 1.18], [8649, 2, 4, 0.97], [5491, 2, 4, 0.47], [434, 2, 4, 0.47], [1006, 2, 4, 1.0], [75, 2, 5, 0.99], [2055, 3, 4, 1.73], [11737, 2, 5, 0.2], [417, 2, 4, 0.66], [616, 2, 4, 1.5], [3840, 1, 4, 0.39], [2050, 3, 4, 0.34], [1007, 2, 5, 0.51], [12353, 1, 5, 0.19], [12870, 1, 4, 0.92], [523, 2, 4, 1.0], [1504, 2, 4, 1.07], [159, 3, 5, 0.37], [20927, 1, 4, 0.67], [2057, 3, 4, 0.34], [13280, 1, 4, 2.05], [3, 2, 5, 0.2], [10574, 3, 6, 1.36], [142, 2, 4, 0.51], [12346, 1, 4, 0.19], [7084, 3, 4, 0.58], [624, 2, 4, 1.35], [9760, 29, 4, 0.2], [2054, 3, 4, 0.34], [140, 2, 4, 0.93], [2775, 2, 4, 0.2], [3891, 1, 4, 0.53], [21793, 1, 4, 2.3], [8939, 2, 4, 0.2], [1429, 2, 5, 0.2], [6158, 2, 4, 0.2], [11739, 2, 4, 0.59], [96, 11, 13, 0.38], [950, 1, 4, 0.37], [5165, 2, 5, 1.61], [12269, 2, 4, 1.03], [84, 2, 4, 1.02], [9372, 1, 4, 1.7], [1126, 2, 4, 0.58], [10388, 2, 4, 1.08], [411, 2, 4, 0.5], [98, 11, 10, 0.54], [972, 3, 4, 1.07], [8672, 2, 5, 0.98], [5165, 1, 4, 0.58], [413, 1, 4, 1.01], [8898, 3, 4, 3.33], [2912, 1, 4, 0.2], [2776, 2, 4, 1.41], [410, 1, 4, 0.54], [12343, 1, 5, 0.19], [10386, 2, 4, 0.92], [995, 2, 4, 1.84], [956, 2, 4, 0.47], [1492, 1, 5, 0.7], [418, 2, 4, 0.42], [12345, 1, 5, 0.19], [13928, 1, 4, 0.48], [9784, 1, 4, 0.47], [22316, 3, 4, 0.51], [147, 1, 4, 0.53], [412, 1, 4, 0.5], [22247, 2, 4, 1.23], [957, 2, 4, 0.55], [336, 15, 4, 0.86], [8677, 3, 4, 0.9], [11490, 1, 4, 0.56], [7567, 3, 4, 1.65], [2912, 2, 5, 0.47], [432, 3, 5, 0.47], [308, 1, 4, 0.95], [307, 2, 5, 0.59], [11953, 1, 4, 0.45], [33, 1, 4, 1.06], [11770, 1, 4, 0.48], [10631, 2, 4, 0.92], [414, 1, 4, 0.66], [35, 1, 4, 0.66], [20256, 2, 4, 0.44], [22317, 3, 5, 0.51], [10407, 10, 6, 1.44], [148, 1, 4, 0.55], [1413, 15, 4, 0.45], [10780, 10, 4, 1.52], [10410, 10, 6, 1.64], [13286, 1, 4, 1.32], [439, 1, 4, 1.15], [7573, 1, 5, 1.45], [335, 3, 9, 1.35], [7886, 4, 4, 0.47], [9691, 1, 4, 0.55], [11767, 1, 4, 0.5], [972, 1, 4, 1.51], [12347, 1, 4, 0.19], [10387, 2, 4, 0.95], [6497, 1, 4, 0.52], [74, 1, 4, 1.16], [20686, 1, 5, 1.33], [3478, 2, 4, 1.63], [12271, 2, 4, 1.01], [9971, 2, 4, 1.44], [8897, 3, 4, 3.33], [2331, 1, 4, 1.08], [11769, 1, 4, 1.1], [9082, 3, 17, 0.77], [11685, 2, 106, 5.4], [6935, 2, 108, 5.9], [326, 2, 36, 3.57], [8648, 2, 89, 2.99], [144, 2, 59, 4.4], [593, 2, 89, 2.78], [2327, 2, 59, 2.57], [143, 2, 58, 2.77], [205, 2, 42, 2.69], [8915, 2, 65, 4.29], [2328, 2, 59, 2.62], [6936, 2, 108, 5.92], [11681, 2, 106, 5.01], [305, 2, 57, 2.58], [151, 1, 58, 2.7], [8650, 2, 89, 2.75], [141, 2, 61, 2.6], [206, 2, 42, 2.55], [2778, 2, 61, 2.77], [2049, 3, 144, 2.25], [88, 10, 220, 3.45], [615, 2, 91, 4.78], [7036, 1, 50, 3.83], [8853, 2, 108, 5.93], [8649, 2, 89, 2.58], [5491, 2, 42, 2.57], [434, 2, 56, 2.07], [1006, 2, 89, 2.63], [75, 2, 57, 3.52], [2055, 3, 396, 4.86], [11737, 2, 23, 2.79], [417, 2, 133, 2.95], [616, 2, 91, 4.41], [3840, 1, 150, 2.17], [2050, 3, 188, 2.34], [1007, 2, 105, 2.65], [12353, 1, 241, 4.47], [12870, 1, 117, 5.16], [523, 2, 60, 2.64], [1504, 2, 80, 2.75], [159, 3, 619, 2.07], [20927, 1, 68, 3.22], [2057, 3, 188, 2.34], [13280, 1, 123, 5.48], [3, 2, 48, 2.52], [10574, 3, 196, 4.07], [142, 2, 133, 2.39], [12346, 1, 241, 4.15], [7084, 3, 51, 2.79], [624, 2, 91, 5.38], [9760, 29, 28, 2.5], [2054, 3, 188, 2.34], [140, 2, 78, 3.15], [2775, 2, 61, 2.77], [3891, 1, 108, 2.43], [21793, 1, 90, 5.26], [8939, 2, 75, 2.61], [1429, 2, 60, 2.59], [6158, 2, 103, 2.54], [11739, 2, 23, 2.79], [96, 11, 330, 2.81], [950, 1, 41, 2.04], [12269, 2, 55, 3.35], [84, 2, 27, 2.67], [9372, 1, 196, 4.79], [1126, 2, 197, 2.71], [10388, 2, 186, 3.58]]</t>
-  </si>
-  <si>
-    <t>[[8672, 2, 5, 0.47], [141, 2, 4, 0.51], [362, 2, 5, 0.2], [361, 2, 5, 0.54], [6935, 2, 7, 1.06], [205, 2, 4, 0.35], [12721, 2, 5, 1.21], [11737, 2, 4, 0.43], [206, 2, 4, 0.2], [2049, 3, 10, 0.21], [8676, 2, 4, 0.49], [8675, 2, 4, 0.6], [417, 2, 4, 0.57], [3, 2, 4, 0.5], [6936, 2, 4, 1.58], [305, 2, 5, 0.53], [151, 1, 4, 0.57], [523, 2, 4, 0.53], [22247, 2, 4, 1.0], [8650, 2, 4, 0.89], [142, 2, 4, 0.49], [8648, 2, 4, 1.7], [2328, 2, 4, 0.78], [2776, 2, 4, 0.2], [8853, 2, 4, 1.54], [616, 2, 4, 1.12], [11739, 2, 4, 0.43], [2327, 2, 5, 0.63], [11837, 2, 4, 0.45], [12352, 1, 4, 1.38], [411, 2, 4, 0.47], [589, 2, 4, 0.2], [143, 2, 4, 0.87], [146, 2, 4, 0.62], [11835, 2, 4, 0.55], [412, 1, 4, 1.0], [12353, 1, 4, 1.38], [6497, 1, 5, 0.5], [583, 2, 4, 1.31], [8674, 2, 5, 0.63], [145, 2, 4, 0.49], [2805, 137, 8, 0.2], [326, 2, 4, 1.31], [10574, 3, 5, 1.26], [418, 2, 4, 0.54], [144, 2, 4, 0.52], [6097, 80, 4, 1.14], [11836, 2, 4, 0.53], [11738, 2, 4, 0.43], [9784, 1, 4, 0.99], [10149, 3, 13, 0.49], [413, 1, 4, 0.97], [6097, 29, 5, 0.64], [2057, 3, 4, 1.0], [75, 2, 4, 0.56], [11234, 2, 4, 0.63], [2055, 3, 4, 1.18], [1413, 15, 4, 0.2], [12344, 1, 4, 1.38], [20252, 2, 4, 0.47], [11504, 2, 4, 0.2], [12269, 2, 4, 0.57], [8915, 2, 4, 0.39], [414, 1, 4, 0.99], [1492, 1, 4, 0.62], [6098, 80, 4, 1.14], [12346, 1, 4, 1.38], [247, 1, 4, 0.8], [3429, 15, 4, 0.46], [22316, 3, 4, 0.46], [2774, 2, 4, 0.52], [1490, 1, 4, 0.36], [416, 1, 4, 1.16], [6098, 29, 4, 1.19], [9786, 1, 4, 1.55], [3934, 5, 5, 0.56], [2859, 15, 4, 0.57], [2049, 1, 4, 0.41], [201, 3, 4, 0.51], [3670, 2, 4, 0.97], [20555, 2, 4, 0.43], [6158, 2, 5, 0.44], [3478, 2, 4, 0.89], [7084, 3, 4, 0.94], [9785, 1, 4, 0.99], [12526, 2, 4, 0.74], [8599, 1, 4, 0.49], [3430, 15, 4, 0.35], [8938, 2, 4, 0.57], [1703, 2, 4, 0.75], [4253, 1, 4, 0.5], [9760, 29, 4, 0.95], [186, 3, 7, 0.5], [1413, 16, 4, 0.37], [229, 1, 4, 1.15], [11885, 2, 4, 0.39], [107, 2, 4, 1.2], [11887, 2, 5, 0.39], [1050, 2, 4, 0.37], [11811, 1, 4, 0.38], [94, 4, 4, 1.76], [4232, 80, 4, 1.65], [11490, 1, 4, 0.52], [436, 2, 4, 0.51], [107, 7, 5, 1.13], [947, 15, 4, 0.39], [2438, 2, 5, 1.38], [415, 1, 4, 1.16], [11770, 1, 4, 0.43], [3673, 2, 4, 2.08], [11767, 1, 4, 0.48], [2821, 3, 8, 0.45], [11769, 1, 4, 0.48], [5939, 3, 4, 0.5], [11671, 1, 4, 0.45], [11160, 1, 4, 1.87], [11844, 2, 4, 0.47], [9491, 21, 10, 0.51], [12347, 1, 4, 1.38], [5812, 3, 4, 2.0], [7036, 1, 4, 0.43], [9358, 1, 4, 0.44], [140, 2, 4, 1.31], [5813, 3, 5, 1.1], [3495, 3, 13, 0.85], [12764, 2, 5, 0.49], [11771, 1, 4, 1.61], [11954, 1, 4, 0.42], [23920, 2, 4, 0.46], [9690, 1, 4, 0.79], [410, 1, 4, 0.8], [5811, 3, 6, 1.16], [308, 1, 5, 0.79], [8672, 2, 145, 3.11], [141, 2, 156, 2.73], [362, 2, 72, 2.98], [361, 2, 78, 3.1], [6935, 2, 143, 5.12], [205, 2, 110, 2.44], [12721, 2, 285, 4.59], [11737, 2, 57, 3.01], [206, 2, 42, 2.62], [2049, 3, 276, 2.87], [8676, 2, 287, 4.22], [8675, 2, 287, 3.21], [417, 2, 78, 3.15], [3, 2, 61, 3.03], [6936, 2, 143, 4.65], [305, 2, 74, 3.08], [151, 1, 33, 2.79], [523, 2, 78, 3.23], [22247, 2, 285, 3.62], [8650, 2, 114, 4.44], [142, 2, 156, 2.68], [8648, 2, 114, 4.32], [2328, 2, 76, 3.53], [2776, 2, 79, 3.28], [8853, 2, 282, 4.82], [616, 2, 107, 4.01], [11739, 2, 57, 3.01], [2327, 2, 76, 3.26], [11837, 2, 268, 2.61], [12352, 1, 607, 4.89], [411, 2, 110, 2.65], [589, 2, 77, 2.91], [143, 2, 147, 3.39], [146, 2, 151, 2.93], [11835, 2, 134, 3.11], [412, 1, 42, 3.02], [12353, 1, 607, 4.89], [6497, 1, 19, 3.94], [583, 2, 30, 3.93], [8674, 2, 145, 3.28], [145, 2, 151, 2.69], [2805, 137, 92, 3.7], [326, 2, 30, 3.62], [10574, 3, 249, 4.6], [418, 2, 142, 2.79], [144, 2, 151, 2.74], [6097, 80, 35, 5.49], [11836, 2, 268, 2.76], [11738, 2, 57, 3.01], [9784, 1, 36, 3.01], [10149, 3, 906, 2.65], [413, 1, 44, 2.97], [6097, 29, 18, 5.49], [2057, 3, 158, 4.31], [75, 2, 144, 2.82], [11234, 2, 185, 3.11], [2055, 3, 158, 4.31], [1413, 15, 50, 3.0], [12344, 1, 607, 4.33], [20252, 2, 94, 2.66], [11504, 2, 72, 2.78], [12269, 2, 65, 2.84], [8915, 2, 97, 2.14], [414, 1, 44, 3.01], [1492, 1, 37, 2.92], [6098, 80, 38, 4.03], [12346, 1, 607, 4.89]]</t>
-  </si>
-  <si>
-    <t>[[2327, 2, 4, 0.52], [305, 2, 4, 0.45], [6935, 2, 5, 1.77], [2778, 2, 4, 0.2], [144, 2, 4, 0.53], [130, 1, 4, 0.48], [8915, 2, 5, 1.08], [589, 2, 5, 0.2], [143, 2, 4, 0.58], [2328, 2, 4, 0.39], [6936, 2, 4, 1.74], [8648, 2, 5, 1.05], [2775, 2, 4, 0.2], [205, 2, 4, 0.43], [8650, 2, 5, 0.39], [326, 2, 4, 0.65], [593, 2, 4, 0.37], [146, 2, 4, 0.57], [145, 2, 4, 0.51], [7036, 1, 4, 0.44], [3840, 1, 5, 0.29], [2049, 3, 5, 0.42], [2776, 2, 4, 0.2], [615, 2, 4, 0.2], [616, 2, 4, 0.2], [88, 10, 9, 0.93], [141, 2, 4, 0.2], [151, 1, 4, 0.59], [1124, 2, 4, 0.79], [11681, 2, 5, 0.83], [206, 2, 4, 0.37], [1446, 2, 4, 0.2], [9760, 29, 4, 0.37], [8853, 2, 4, 1.79], [990, 2, 5, 0.2], [5491, 2, 4, 0.58], [1007, 2, 4, 0.46], [362, 2, 4, 0.5], [8672, 2, 4, 1.48], [1504, 2, 4, 0.93], [2055, 3, 4, 0.46], [9372, 1, 4, 1.97], [2057, 3, 4, 0.46], [3893, 1, 4, 0.2], [8649, 2, 5, 0.39], [8938, 2, 4, 0.52], [434, 2, 4, 0.2], [12870, 1, 4, 1.22], [624, 2, 4, 1.1], [2050, 3, 4, 0.46], [417, 2, 4, 0.42], [3889, 1, 4, 0.35], [5165, 1, 4, 0.56], [1429, 2, 4, 0.2], [378, 2, 4, 2.29], [7084, 3, 4, 0.86], [10, 2, 4, 0.45], [2991, 3, 4, 1.1], [140, 2, 4, 1.27], [3891, 1, 4, 0.2], [1006, 2, 4, 0.54], [7886, 4, 5, 0.41], [10574, 3, 5, 1.36], [7573, 1, 8, 2.02], [10149, 3, 13, 0.39], [5208, 3, 4, 0.19], [1622, 1, 4, 0.45], [75, 2, 4, 0.39], [3, 2, 4, 0.46], [20927, 1, 4, 0.95], [5165, 2, 5, 1.02], [997, 2, 4, 1.42], [11234, 2, 4, 1.25], [12721, 2, 5, 0.49], [22247, 2, 4, 1.37], [147, 1, 4, 1.75], [346, 3, 4, 0.19], [996, 2, 4, 1.16], [11811, 1, 4, 0.2], [229, 1, 4, 0.54], [20252, 2, 4, 0.38], [11685, 2, 5, 0.83], [998, 2, 5, 1.0], [94, 4, 4, 1.91], [972, 3, 5, 0.51], [9491, 21, 10, 0.44], [76, 2, 4, 0.87], [35, 1, 4, 1.02], [439, 1, 4, 0.46], [6158, 2, 4, 2.61], [413, 1, 4, 1.08], [13028, 3, 5, 1.54], [13928, 1, 4, 0.2], [8104, 1, 4, 0.87], [5076, 1, 4, 0.43], [2805, 137, 4, 0.6], [5209, 3, 4, 0.19], [412, 1, 4, 0.43], [8676, 2, 4, 2.17], [33, 1, 4, 0.97], [83, 2, 4, 0.88], [418, 2, 4, 0.63], [148, 1, 4, 1.76], [2774, 2, 4, 0.63], [3495, 3, 10, 0.82], [8898, 3, 5, 1.44], [12212, 29, 4, 0.2], [7887, 4, 4, 0.94], [20256, 2, 5, 0.2], [38, 1, 4, 1.16], [11490, 1, 5, 0.43], [11770, 1, 4, 0.88], [34, 1, 4, 1.09], [10407, 10, 7, 1.55], [415, 1, 4, 0.52], [9784, 1, 4, 0.52], [84, 2, 4, 0.97], [126, 2, 4, 1.27], [411, 2, 4, 0.48], [13928, 2, 4, 0.7], [11739, 2, 4, 1.42], [9691, 1, 4, 0.57], [3048, 3, 4, 1.15], [9690, 1, 4, 0.37], [8939, 2, 4, 0.2], [5584, 3, 5, 1.25], [11953, 1, 4, 0.46], [39, 1, 4, 1.13], [12351, 1, 4, 0.66], [10410, 10, 9, 2.08], [11954, 1, 4, 0.38], [12764, 2, 5, 0.21], [7567, 3, 5, 1.16], [2327, 2, 74, 2.93], [305, 2, 72, 2.8], [6935, 2, 135, 6.0], [2778, 2, 77, 2.92], [144, 2, 55, 4.54], [130, 1, 29, 2.86], [8915, 2, 93, 2.96], [589, 2, 75, 2.97], [143, 2, 72, 3.03], [2328, 2, 147, 3.37], [6936, 2, 135, 5.39], [8648, 2, 110, 3.91], [2775, 2, 77, 2.92], [205, 2, 54, 2.77], [8650, 2, 110, 3.45], [326, 2, 44, 4.1], [593, 2, 223, 2.53], [146, 2, 73, 3.02], [145, 2, 73, 2.92], [7036, 1, 63, 4.28], [3840, 1, 84, 3.43], [2049, 3, 360, 2.34], [2776, 2, 77, 3.16], [615, 2, 54, 3.01], [616, 2, 54, 2.64], [88, 10, 276, 3.94], [141, 2, 76, 2.69], [151, 1, 32, 2.68], [1124, 2, 182, 3.1], [11681, 2, 131, 5.43], [206, 2, 106, 2.39], [1446, 2, 74, 3.2], [9760, 29, 35, 2.66], [8853, 2, 135, 5.48], [990, 2, 26, 2.69], [5491, 2, 53, 3.05], [1007, 2, 264, 2.49], [362, 2, 69, 2.89], [8672, 2, 140, 4.92], [1504, 2, 99, 3.69], [2055, 3, 314, 2.32], [9372, 1, 114, 5.58], [2057, 3, 314, 2.32], [3893, 1, 61, 2.96], [8649, 2, 110, 3.26], [8938, 2, 125, 2.43], [434, 2, 53, 2.69], [12870, 1, 69, 3.3], [624, 2, 104, 3.83], [2050, 3, 314, 2.32], [417, 2, 76, 2.76], [3889, 1, 122, 2.29], [5165, 1, 38, 3.97], [1429, 2, 74, 2.89], [378, 2, 218, 5.85], [7084, 3, 127, 3.22], [10, 2, 102, 3.24], [2991, 3, 79, 5.62], [140, 2, 86, 3.98], [3891, 1, 61, 2.96], [1006, 2, 111, 2.97], [7886, 4, 35, 2.24], [10574, 3, 246, 4.55], [7573, 1, 336, 6.0], [10149, 3, 848, 3.11], [5208, 3, 273, 2.87], [1622, 1, 105, 2.46]]</t>
-  </si>
-  <si>
-    <t>[[2778, 2, 11, 1.2], [6935, 2, 19, 4.42], [6936, 2, 9, 3.89], [305, 2, 7, 1.48], [8672, 2, 10, 1.28], [615, 2, 7, 1.37], [1504, 2, 9, 1.35], [2775, 2, 9, 1.03], [145, 2, 7, 1.24], [2776, 2, 9, 1.9], [8853, 2, 7, 3.02], [2327, 2, 7, 1.21], [12721, 2, 11, 1.7], [130, 1, 9, 0.78], [143, 2, 7, 1.94], [146, 2, 7, 1.53], [2328, 2, 7, 1.5], [11681, 2, 11, 3.38], [11737, 2, 7, 1.32], [616, 2, 7, 2.16], [5491, 2, 7, 1.03], [141, 2, 7, 2.37], [362, 2, 6, 0.85], [144, 2, 7, 1.3], [2497, 2, 7, 1.64], [205, 2, 7, 0.85], [8650, 2, 11, 2.33], [5493, 2, 9, 0.77], [417, 2, 7, 1.55], [8676, 2, 7, 0.9], [8673, 2, 9, 2.44], [3670, 2, 9, 4.0], [2774, 2, 9, 3.42], [8648, 2, 7, 3.5], [589, 2, 9, 0.8], [3, 2, 7, 0.98], [206, 2, 7, 0.71], [6097, 80, 7, 3.38], [2423, 29, 7, 3.02], [22247, 2, 7, 1.94], [11836, 2, 7, 0.9], [6497, 1, 7, 1.84], [8674, 2, 7, 1.97], [624, 2, 7, 2.32], [2055, 3, 7, 3.23], [12343, 1, 7, 2.59], [2423, 80, 7, 2.97], [523, 2, 7, 1.25], [12344, 1, 7, 1.6], [593, 2, 8, 0.79], [6097, 29, 7, 3.38], [6098, 80, 7, 2.36], [12720, 2, 7, 1.69], [12345, 1, 7, 2.59], [11739, 2, 7, 1.32], [8915, 2, 7, 0.75], [75, 2, 7, 2.15], [88, 10, 16, 2.9], [326, 2, 7, 2.83], [6494, 1, 7, 0.85], [60, 3, 10, 1.49], [13260, 29, 7, 1.16], [142, 2, 7, 2.37], [3429, 15, 7, 0.85], [1492, 1, 7, 1.13], [411, 2, 7, 0.81], [21712, 3, 21, 1.11], [412, 1, 7, 1.93], [1050, 2, 7, 0.7], [2422, 80, 7, 2.41], [10149, 3, 21, 2.21], [2422, 29, 7, 3.8], [6098, 29, 7, 2.08], [378, 2, 9, 2.87], [12346, 1, 7, 2.59], [7704, 2, 7, 2.28], [151, 1, 7, 1.36], [11738, 2, 7, 1.32], [22316, 3, 7, 0.85], [1243, 2, 7, 1.32], [229, 1, 7, 3.68], [1049, 2, 7, 0.7], [13264, 29, 7, 0.94], [20252, 2, 7, 1.06], [345, 3, 7, 2.32], [13258, 29, 9, 1.59], [1490, 1, 7, 0.87], [964, 15, 7, 0.66], [12269, 2, 7, 0.93], [2438, 1, 7, 2.08], [2821, 3, 12, 1.27], [5208, 3, 9, 1.41], [10407, 10, 10, 2.08], [2331, 1, 7, 1.02], [1163, 3, 7, 2.25], [416, 1, 7, 3.06], [201, 3, 7, 4.28], [307, 2, 7, 1.91], [186, 3, 12, 0.9], [7004, 1, 7, 1.03], [149, 2, 7, 1.95], [418, 2, 7, 0.99], [957, 2, 7, 1.05], [13259, 29, 7, 2.95], [1309, 1, 7, 0.82], [7705, 2, 7, 2.28], [12229, 2, 7, 0.96], [7706, 2, 7, 2.28], [10406, 10, 12, 2.42], [11687, 2, 7, 1.02], [410, 1, 7, 1.3], [7036, 1, 7, 0.87], [3478, 2, 9, 1.47], [20255, 2, 7, 1.14], [9784, 1, 7, 1.67], [21713, 3, 13, 0.88], [8938, 2, 7, 1.06], [10408, 10, 10, 1.81], [5490, 2, 7, 0.91], [12870, 1, 7, 4.46], [11402, 1, 7, 0.85], [10410, 10, 10, 2.08], [19687, 1, 7, 2.23], [2438, 2, 8, 2.38], [11490, 1, 7, 0.83], [107, 7, 8, 2.46], [2703, 3, 7, 3.92], [11161, 1, 10, 3.78], [956, 2, 7, 0.96], [1886, 2, 7, 0.65], [21781, 2, 7, 0.86], [11690, 2, 7, 0.66], [10411, 10, 10, 1.97], [412, 1, 42, 3.02], [1050, 2, 38, 1.78], [2422, 80, 187, 4.2], [10149, 3, 866, 4.0], [2422, 29, 18, 5.41], [6098, 29, 19, 3.97], [378, 2, 114, 4.24], [12346, 1, 610, 4.37], [7704, 2, 176, 4.07], [151, 1, 33, 2.79], [11738, 2, 56, 3.11], [22316, 3, 318, 2.64], [1243, 2, 99, 3.11], [229, 1, 81, 5.47], [1049, 2, 38, 1.78], [13264, 29, 73, 2.73], [20252, 2, 92, 2.85], [345, 3, 297, 4.1], [13258, 29, 39, 3.37], [1490, 1, 51, 2.66], [12269, 2, 65, 2.72], [2438, 1, 54, 3.87], [2821, 3, 658, 3.36], [5208, 3, 561, 3.2], [10407, 10, 1201, 3.88], [2331, 1, 119, 2.8], [1163, 3, 114, 3.33], [416, 1, 85, 4.84], [201, 3, 297, 6.0], [307, 2, 148, 3.7], [186, 3, 665, 2.69], [7004, 1, 80, 2.82], [149, 2, 88, 3.74], [418, 2, 143, 2.78], [957, 2, 107, 2.84], [13259, 29, 35, 4.73], [1309, 1, 58, 2.6], [7705, 2, 176, 4.07], [12229, 2, 152, 2.74], [7706, 2, 176, 4.07], [10406, 10, 1784, 4.24], [11687, 2, 303, 2.8], [410, 1, 105, 3.09], [7036, 1, 127, 2.65], [3478, 2, 38, 4.08], [20255, 2, 93, 2.93], [9784, 1, 72, 3.46], [21713, 3, 1121, 2.67], [8938, 2, 192, 2.85], [10408, 10, 785, 3.6], [5490, 2, 108, 2.69], [12870, 1, 137, 6.0], [11402, 1, 45, 2.64], [10410, 10, 1201, 3.88], [19687, 1, 30, 4.02], [2438, 2, 643, 4.17], [11490, 1, 55, 2.9], [107, 7, 239, 4.24], [2703, 3, 300, 5.7], [11161, 1, 490, 5.57], [956, 2, 107, 2.75], [1886, 2, 158, 2.44], [21781, 2, 104, 2.65], [11690, 2, 303, 2.44], [10411, 10, 785, 3.76]]</t>
-  </si>
-  <si>
-    <t>[[141, 2, 7, 0.94], [2328, 2, 7, 1.43], [8650, 2, 7, 2.83], [362, 2, 9, 0.78], [5491, 2, 7, 1.11], [5493, 2, 9, 0.67], [130, 1, 7, 1.38], [589, 2, 7, 0.95], [2327, 2, 7, 1.16], [326, 2, 7, 1.87], [11685, 2, 7, 4.19], [8672, 2, 10, 1.28], [417, 2, 7, 1.02], [6935, 2, 12, 4.21], [205, 2, 7, 0.74], [11681, 2, 11, 3.74], [206, 2, 7, 0.71], [8648, 2, 7, 3.27], [6936, 2, 8, 3.12], [142, 2, 9, 0.8], [8915, 2, 7, 1.26], [11837, 2, 7, 1.01], [12721, 2, 9, 1.92], [11838, 2, 9, 0.99], [2049, 3, 17, 1.18], [1446, 2, 7, 1.82], [523, 2, 7, 1.02], [615, 2, 7, 2.85], [8676, 2, 7, 2.44], [11737, 2, 7, 1.9], [305, 2, 7, 0.98], [616, 2, 7, 2.37], [413, 1, 7, 1.44], [412, 1, 7, 1.93], [411, 2, 7, 0.86], [11739, 2, 7, 1.9], [10574, 3, 10, 2.64], [11835, 2, 7, 1.01], [145, 2, 7, 1.24], [21793, 1, 8, 4.02], [2775, 2, 7, 0.78], [1429, 2, 7, 0.89], [76, 2, 7, 2.04], [8675, 2, 9, 1.42], [8673, 2, 7, 3.38], [143, 2, 7, 1.19], [11836, 2, 9, 0.79], [8674, 2, 7, 1.46], [8938, 2, 7, 1.78], [146, 2, 7, 1.14], [6158, 2, 9, 2.65], [151, 1, 7, 1.36], [12720, 2, 7, 1.69], [10149, 3, 21, 1.48], [2776, 2, 7, 1.37], [3495, 3, 21, 1.51], [2055, 3, 7, 3.23], [75, 2, 7, 2.15], [2057, 3, 7, 3.23], [11738, 2, 7, 1.9], [144, 2, 7, 0.96], [8939, 2, 7, 3.23], [416, 1, 7, 1.34], [7885, 4, 7, 0.81], [22316, 3, 9, 0.85], [88, 10, 16, 2.9], [159, 3, 9, 1.37], [2859, 15, 7, 0.81], [7084, 3, 7, 3.21], [418, 2, 9, 0.68], [10993, 2, 7, 0.94], [20252, 2, 7, 0.68], [9784, 1, 7, 1.61], [7705, 2, 7, 2.28], [5165, 1, 7, 1.09], [12526, 2, 7, 2.78], [410, 1, 7, 0.87], [11844, 2, 7, 1.16], [414, 1, 7, 1.34], [12351, 1, 7, 1.63], [2423, 80, 7, 2.8], [378, 2, 7, 2.23], [2424, 29, 9, 1.09], [2423, 29, 7, 3.02], [12345, 1, 7, 1.19], [60, 3, 10, 4.98], [950, 1, 7, 0.72], [6494, 1, 7, 0.85], [11490, 1, 7, 0.89], [2424, 80, 7, 2.28], [13023, 3, 10, 2.63], [12373, 1, 11, 1.47], [13034, 3, 8, 2.37], [201, 3, 7, 2.12], [1519, 3, 15, 0.69], [11489, 1, 7, 0.68], [345, 3, 7, 1.4], [5208, 3, 9, 1.01], [11770, 1, 7, 0.89], [159, 1, 7, 1.33], [3, 2, 7, 5.0], [6952, 1, 7, 2.01], [3430, 15, 7, 2.26], [20927, 1, 7, 0.87], [11954, 1, 7, 0.77], [7886, 4, 7, 0.8], [432, 3, 7, 3.74], [3429, 15, 7, 0.85], [13928, 1, 7, 0.82], [11504, 2, 7, 0.67], [11811, 1, 7, 1.93], [566, 2, 7, 0.92], [5584, 3, 7, 2.91], [114, 3, 7, 3.01], [2331, 1, 7, 2.78], [10407, 10, 10, 2.08], [1492, 1, 7, 1.13], [105, 3, 7, 3.01], [1490, 1, 7, 3.38], [7004, 1, 7, 1.91], [11089, 1, 7, 0.71], [2703, 3, 7, 3.92], [6098, 80, 7, 2.52], [8274, 3, 7, 4.22], [11674, 1, 7, 0.66], [1886, 2, 7, 0.82], [12348, 1, 7, 1.19], [94, 4, 7, 4.17], [10410, 10, 10, 2.08], [3891, 1, 7, 4.39], [11953, 1, 7, 0.85], [22317, 3, 8, 0.88], [6097, 80, 7, 3.42], [7084, 3, 129, 5.0], [418, 2, 72, 2.79], [10993, 2, 27, 3.0], [20252, 2, 93, 2.46], [9784, 1, 72, 3.4], [7705, 2, 176, 4.07], [5165, 1, 49, 2.88], [12526, 2, 272, 4.56], [410, 1, 53, 2.3], [11844, 2, 186, 2.77], [414, 1, 86, 3.13], [12351, 1, 315, 3.26], [2423, 80, 92, 4.41], [378, 2, 114, 4.24], [2424, 29, 17, 3.17], [2423, 29, 37, 4.81], [12345, 1, 315, 3.26], [950, 1, 30, 2.15], [6494, 1, 52, 2.64], [11490, 1, 109, 2.68], [2424, 80, 170, 4.07], [13023, 3, 592, 4.42], [12373, 1, 533, 3.26], [13034, 3, 592, 4.16], [201, 3, 151, 3.21], [1519, 3, 561, 1.77], [11489, 1, 109, 2.46], [345, 3, 298, 3.19], [5208, 3, 563, 2.79], [11770, 1, 221, 2.67], [159, 1, 39, 3.12], [3, 2, 118, 6.0], [6952, 1, 189, 3.79], [3430, 15, 69, 4.05], [20927, 1, 80, 2.66], [11954, 1, 203, 2.56], [7886, 4, 36, 2.38], [432, 3, 300, 5.53], [3429, 15, 53, 2.63], [13928, 1, 49, 2.61], [11504, 2, 72, 2.78], [11811, 1, 451, 3.72], [566, 2, 175, 2.7], [5584, 3, 229, 4.7], [114, 3, 241, 4.8], [2331, 1, 117, 4.57], [10407, 10, 1201, 3.88], [1492, 1, 37, 2.92], [105, 3, 201, 4.72], [1490, 1, 48, 5.17], [7004, 1, 40, 3.0], [11089, 1, 173, 2.5], [2703, 3, 300, 5.7], [6098, 80, 74, 4.31], [11674, 1, 205, 2.44], [1886, 2, 157, 2.61], [12348, 1, 315, 3.26], [94, 4, 116, 5.96], [10410, 10, 1201, 3.88], [3891, 1, 122, 6.0], [11953, 1, 203, 2.63], [22317, 3, 318, 2.66], [6097, 80, 68, 5.21]]</t>
-  </si>
-  <si>
-    <t>[[326, 2, 8, 2.27], [6935, 2, 17, 3.32], [2049, 3, 13, 0.72], [362, 2, 7, 1.64], [589, 2, 10, 0.77], [75, 2, 7, 0.75], [141, 2, 7, 2.25], [1776, 1, 9, 0.83], [205, 2, 7, 0.7], [8915, 2, 9, 0.75], [2778, 2, 7, 0.79], [8672, 2, 10, 0.94], [6936, 2, 10, 3.25], [593, 2, 11, 1.01], [7886, 4, 7, 1.04], [305, 2, 7, 0.96], [206, 2, 7, 0.72], [151, 1, 7, 0.87], [8648, 2, 7, 2.14], [1777, 1, 9, 1.98], [2328, 2, 7, 0.65], [88, 10, 14, 1.03], [11681, 2, 10, 4.17], [990, 2, 7, 1.06], [8650, 2, 7, 2.17], [412, 1, 7, 1.64], [5151, 2, 9, 2.35], [2050, 3, 7, 2.4], [76, 2, 9, 1.39], [144, 2, 7, 0.91], [10149, 3, 25, 4.03], [345, 3, 10, 0.97], [2991, 3, 7, 3.64], [22247, 2, 9, 1.34], [57, 1, 7, 0.7], [3478, 2, 7, 2.16], [146, 2, 7, 1.93], [7004, 1, 9, 0.71], [45, 2, 7, 2.94], [2054, 3, 6, 0.93], [143, 2, 6, 0.84], [417, 2, 7, 0.85], [413, 1, 7, 2.13], [21793, 1, 7, 0.83], [167, 3, 9, 0.97], [201, 3, 10, 0.7], [74, 1, 7, 3.37], [1446, 2, 7, 1.41], [346, 1, 9, 0.73], [2055, 3, 7, 0.9], [168, 3, 9, 1.11], [10, 2, 9, 1.61], [7084, 3, 7, 0.69], [11234, 2, 9, 0.72], [1429, 2, 7, 1.71], [7036, 1, 7, 3.47], [12721, 2, 10, 0.9], [3495, 3, 21, 0.95], [5081, 2, 7, 0.81], [8649, 2, 7, 2.48], [308, 1, 9, 2.22], [13028, 3, 7, 0.9], [12870, 1, 7, 2.96], [10825, 21, 14, 2.47], [79, 1, 7, 0.7], [1492, 1, 7, 1.98], [96, 11, 23, 0.64], [23, 1, 7, 1.24], [1006, 2, 7, 1.06], [3893, 1, 7, 1.48], [418, 2, 7, 0.79], [1504, 2, 7, 1.39], [145, 2, 7, 0.79], [5208, 3, 9, 1.57], [9827, 3, 7, 1.36], [3891, 1, 7, 0.98], [432, 3, 7, 0.75], [7005, 1, 7, 1.16], [1490, 1, 7, 1.46], [8853, 2, 11, 3.48], [94, 4, 7, 4.2], [13260, 29, 7, 0.77], [5812, 3, 8, 3.38], [416, 1, 7, 1.53], [8651, 2, 7, 1.54], [12353, 1, 7, 3.09], [20256, 2, 7, 0.92], [8939, 2, 7, 1.39], [21269, 3, 7, 4.99], [13280, 1, 7, 2.64], [950, 1, 7, 0.98], [33, 1, 7, 1.02], [5086, 1, 7, 2.64], [998, 2, 7, 1.84], [9069, 1, 7, 1.87], [1243, 2, 7, 1.64], [229, 1, 7, 2.92], [2878, 1, 6, 1.36], [140, 2, 7, 1.21], [7567, 3, 7, 2.54], [2049, 1, 7, 0.69], [20927, 1, 9, 0.66], [126, 2, 7, 2.22], [346, 3, 8, 0.74], [1703, 2, 7, 1.51], [3980, 4, 7, 2.59], [8121, 3, 7, 0.97], [8274, 3, 7, 1.24], [35, 1, 7, 0.88], [9691, 1, 7, 2.1], [5209, 3, 9, 0.67], [997, 2, 7, 1.98], [11811, 1, 7, 1.83], [5584, 3, 7, 3.35], [1070, 7, 13, 1.16], [11914, 1, 7, 1.42], [1519, 3, 17, 0.69], [856, 1, 7, 0.69], [5660, 2, 7, 1.66], [8898, 3, 7, 4.68], [1091, 1, 7, 1.15], [5513, 2, 7, 0.8], [523, 2, 7, 1.16], [8926, 1, 7, 2.6], [11767, 1, 7, 0.88], [2775, 2, 7, 0.79], [9372, 1, 7, 2.03], [13034, 3, 8, 3.38], [9081, 3, 12, 3.55], [307, 2, 7, 2.19], [20255, 2, 7, 1.43], [12661, 1, 7, 1.87], [11808, 1, 7, 1.16], [23, 1, 39, 2.51], [1006, 2, 80, 2.28], [3893, 1, 44, 2.25], [418, 2, 131, 1.94], [1504, 2, 72, 2.16], [145, 2, 139, 1.94], [5208, 3, 196, 2.33], [9827, 3, 30, 2.12], [3891, 1, 44, 2.25], [432, 3, 106, 2.02], [7005, 1, 28, 1.93], [1490, 1, 18, 2.23], [8853, 2, 97, 4.75], [94, 4, 42, 4.96], [13260, 29, 26, 2.0], [5812, 3, 543, 4.52], [416, 1, 79, 2.68], [8651, 2, 79, 2.73], [12353, 1, 557, 4.25], [20256, 2, 33, 2.19], [21269, 3, 270, 6.0], [13280, 1, 291, 3.8], [950, 1, 55, 2.13], [33, 1, 39, 2.24], [5086, 1, 63, 3.41], [998, 2, 83, 2.61], [9069, 1, 43, 2.12], [1243, 2, 90, 2.79], [229, 1, 75, 4.08], [2878, 1, 28, 2.63], [140, 2, 32, 2.75], [7567, 3, 24, 3.31], [2049, 1, 14, 1.46], [20927, 1, 28, 1.93], [126, 2, 32, 2.98], [346, 3, 219, 2.01], [1703, 2, 149, 2.66], [3980, 4, 443, 3.74], [8121, 3, 270, 2.12], [8274, 3, 159, 2.0], [35, 1, 103, 2.02], [9691, 1, 27, 2.36], [5209, 3, 196, 1.95], [997, 2, 83, 2.24], [11811, 1, 416, 2.98], [5584, 3, 86, 3.55], [1070, 7, 206, 1.93], [11914, 1, 30, 2.19], [1519, 3, 1545, 1.83], [856, 1, 32, 1.84], [5660, 2, 61, 2.93], [8898, 3, 102, 5.05], [1091, 1, 17, 2.42], [5513, 2, 70, 1.95], [523, 2, 143, 2.31], [8926, 1, 22, 2.84], [11767, 1, 151, 2.03], [2775, 2, 55, 2.06], [9372, 1, 210, 3.18], [13034, 3, 203, 4.14], [9081, 3, 161, 4.81], [307, 2, 51, 2.45], [20255, 2, 33, 2.2], [12661, 1, 28, 2.13], [11808, 1, 166, 1.93]]</t>
-  </si>
-  <si>
-    <t>[[88, 10, 16, 1.96], [2327, 2, 7, 1.0], [8915, 2, 8, 1.9], [589, 2, 8, 0.99], [2778, 2, 9, 0.94], [6935, 2, 11, 4.09], [2328, 2, 7, 1.12], [5493, 2, 7, 2.27], [130, 1, 9, 2.43], [305, 2, 6, 0.82], [615, 2, 9, 0.87], [616, 2, 9, 0.66], [6936, 2, 7, 3.42], [326, 2, 7, 2.62], [8650, 2, 7, 1.47], [8648, 2, 7, 2.02], [1446, 2, 7, 1.22], [2049, 3, 10, 0.87], [10, 2, 9, 0.67], [143, 2, 7, 1.55], [159, 3, 8, 1.18], [593, 2, 9, 0.88], [205, 2, 7, 0.83], [5491, 2, 7, 1.12], [2775, 2, 9, 0.94], [7036, 1, 7, 2.3], [144, 2, 7, 3.22], [151, 1, 7, 1.36], [3840, 1, 9, 1.09], [94, 4, 7, 3.68], [434, 2, 9, 0.71], [8938, 2, 7, 0.95], [990, 2, 7, 1.21], [3893, 1, 9, 0.98], [8853, 2, 7, 3.51], [146, 2, 7, 2.06], [1504, 2, 7, 1.79], [624, 2, 7, 2.19], [12224, 1, 7, 0.84], [1429, 2, 7, 0.91], [3891, 1, 7, 0.98], [2776, 2, 7, 1.18], [206, 2, 7, 0.74], [2055, 3, 7, 0.84], [362, 2, 7, 0.96], [141, 2, 7, 1.21], [11681, 2, 11, 3.45], [11404, 2, 9, 0.94], [378, 2, 7, 2.23], [5208, 3, 9, 0.78], [3889, 1, 7, 0.65], [8649, 2, 7, 3.15], [1007, 2, 7, 0.85], [10574, 3, 11, 4.5], [10993, 2, 7, 1.29], [11234, 2, 7, 1.8], [7886, 4, 7, 0.85], [12870, 1, 7, 1.83], [21793, 1, 7, 0.96], [10149, 3, 21, 2.43], [3980, 4, 6, 2.43], [2050, 3, 7, 0.84], [12353, 1, 7, 1.22], [145, 2, 7, 1.94], [7084, 3, 7, 1.58], [11811, 1, 7, 0.8], [8672, 2, 9, 3.66], [20927, 1, 7, 1.83], [5165, 1, 7, 2.49], [998, 2, 7, 2.89], [9760, 29, 7, 0.71], [997, 2, 7, 2.64], [2436, 4, 9, 0.85], [1006, 2, 7, 0.99], [972, 3, 8, 0.89], [2424, 80, 7, 1.91], [346, 3, 7, 1.21], [3, 2, 7, 1.14], [229, 1, 7, 1.0], [6158, 2, 7, 1.38], [3495, 3, 14, 0.98], [12346, 1, 7, 1.22], [5165, 2, 8, 2.84], [7887, 4, 7, 1.42], [5076, 1, 7, 1.3], [126, 2, 7, 2.34], [20252, 2, 7, 1.43], [11953, 1, 7, 0.84], [9372, 1, 7, 3.48], [11770, 1, 7, 2.76], [140, 2, 7, 2.34], [12344, 1, 7, 1.22], [8939, 2, 7, 0.92], [11954, 1, 7, 0.7], [1492, 1, 7, 0.95], [11685, 2, 11, 3.45], [12352, 1, 7, 1.22], [996, 2, 7, 2.83], [12721, 2, 7, 4.25], [20256, 2, 9, 0.82], [2774, 2, 7, 1.15], [12350, 1, 7, 1.22], [3981, 3, 22, 1.14], [9491, 21, 21, 0.8], [5434, 1, 7, 1.93], [2423, 80, 7, 1.88], [12343, 1, 7, 1.22], [6497, 1, 7, 3.31], [5584, 3, 7, 3.37], [2438, 2, 8, 1.33], [10388, 2, 7, 1.93], [12351, 1, 7, 1.22], [10407, 10, 10, 2.08], [11179, 1, 7, 1.6], [6496, 1, 7, 3.41], [22317, 3, 7, 0.66], [7573, 1, 22, 5.0], [823, 1, 7, 1.9], [5209, 3, 7, 1.38], [8898, 3, 7, 3.35], [2805, 137, 7, 2.91], [3900, 3, 7, 3.39], [12526, 2, 7, 2.21], [2424, 29, 7, 1.01], [11812, 1, 7, 0.87], [4253, 1, 7, 1.04], [3975, 4, 7, 2.86], [11490, 1, 7, 0.65], [336, 15, 7, 1.79], [1622, 1, 7, 0.87], [12764, 2, 8, 0.9], [412, 1, 7, 0.81], [972, 1, 7, 1.96], [9760, 29, 35, 2.66], [997, 2, 232, 4.28], [2436, 4, 57, 2.98], [1006, 2, 111, 2.97], [972, 3, 291, 2.82], [2424, 80, 82, 2.99], [346, 3, 308, 2.68], [3, 2, 118, 2.78], [229, 1, 81, 2.64], [6158, 2, 127, 2.86], [3495, 3, 471, 2.98], [12346, 1, 612, 2.87], [5165, 2, 180, 4.82], [7887, 4, 68, 2.73], [5076, 1, 127, 2.94], [126, 2, 86, 3.98], [20252, 2, 91, 3.07], [11953, 1, 195, 2.48], [9372, 1, 224, 5.12], [11770, 1, 206, 4.4], [140, 2, 86, 3.98], [12344, 1, 612, 2.87], [8939, 2, 93, 2.9], [11954, 1, 195, 2.34], [1492, 1, 18, 2.93], [11685, 2, 131, 5.43], [12352, 1, 612, 2.87], [996, 2, 115, 4.81], [12721, 2, 272, 5.89], [20256, 2, 49, 2.94], [2774, 2, 200, 2.79], [12350, 1, 612, 2.87], [3981, 3, 790, 3.14], [9491, 21, 1034, 2.76], [5434, 1, 24, 2.89], [2423, 80, 90, 3.36], [12343, 1, 612, 2.87], [6497, 1, 35, 4.95], [5584, 3, 120, 4.28], [2438, 2, 308, 2.82], [10388, 2, 211, 3.57], [12351, 1, 612, 2.87], [10407, 10, 1168, 3.71], [11179, 1, 85, 3.24], [6496, 1, 38, 5.05], [22317, 3, 308, 2.3], [7573, 1, 336, 6.0], [823, 1, 39, 3.54], [5209, 3, 273, 2.87], [8898, 3, 144, 4.83], [2805, 137, 175, 4.54], [3900, 3, 21, 4.29], [12526, 2, 135, 3.53], [2424, 29, 34, 2.65], [11812, 1, 116, 2.85], [4253, 1, 83, 2.97], [3975, 4, 234, 4.34], [11490, 1, 106, 2.29], [336, 15, 110, 3.43], [1622, 1, 52, 2.81], [12764, 2, 734, 2.54], [412, 1, 82, 2.45], [972, 1, 48, 2.93]]</t>
-  </si>
-  <si>
-    <t>[[6935, 2, 15, 3.35], [141, 2, 7, 1.02], [589, 2, 10, 0.69], [2778, 2, 9, 1.18], [6936, 2, 13, 3.74], [8648, 2, 7, 2.18], [362, 2, 7, 1.34], [2327, 2, 7, 1.6], [11681, 2, 22, 3.47], [8650, 2, 7, 2.04], [326, 2, 7, 1.42], [205, 2, 7, 1.04], [2328, 2, 9, 1.41], [1446, 2, 9, 1.08], [305, 2, 7, 2.13], [130, 1, 7, 0.87], [8649, 2, 9, 2.02], [2775, 2, 7, 1.18], [8853, 2, 11, 3.24], [361, 2, 7, 0.96], [2776, 2, 7, 1.18], [593, 2, 7, 1.38], [143, 2, 7, 2.18], [140, 2, 7, 1.42], [1429, 2, 9, 1.24], [206, 2, 9, 0.75], [5493, 2, 7, 0.94], [523, 2, 7, 1.0], [7004, 1, 7, 1.3], [413, 1, 7, 1.96], [7036, 1, 7, 3.04], [5491, 2, 7, 0.92], [412, 1, 7, 1.25], [21793, 1, 7, 3.65], [12350, 1, 7, 0.7], [1124, 2, 7, 1.27], [990, 2, 7, 0.82], [12353, 1, 7, 1.26], [5165, 1, 9, 2.64], [8915, 2, 8, 1.49], [615, 2, 7, 2.25], [583, 2, 7, 1.42], [417, 2, 7, 0.83], [21798, 1, 7, 0.95], [146, 2, 7, 2.92], [248, 1, 9, 0.68], [8089, 1, 7, 2.21], [434, 2, 9, 0.79], [201, 3, 7, 1.37], [142, 2, 7, 1.19], [6097, 80, 9, 3.4], [11770, 1, 7, 0.8], [6952, 1, 7, 3.29], [2055, 3, 7, 1.5], [345, 3, 7, 0.9], [3891, 1, 7, 1.8], [9372, 1, 7, 1.55], [2057, 3, 7, 1.5], [616, 2, 7, 1.58], [7084, 3, 7, 2.33], [3670, 2, 7, 2.71], [3893, 1, 7, 1.8], [5165, 2, 12, 3.15], [12346, 1, 7, 0.7], [12870, 1, 7, 2.21], [12343, 1, 7, 0.89], [10574, 3, 8, 2.44], [1886, 2, 7, 0.66], [2424, 80, 7, 2.28], [346, 3, 7, 0.72], [3334, 5, 7, 3.63], [20927, 1, 7, 0.95], [12351, 1, 7, 0.7], [7885, 4, 7, 0.98], [6098, 80, 7, 2.81], [6097, 29, 7, 3.9], [11089, 1, 7, 0.8], [12345, 1, 7, 0.85], [10149, 3, 21, 1.91], [20256, 2, 7, 0.87], [147, 1, 7, 2.36], [22316, 3, 7, 0.66], [1492, 1, 9, 1.48], [11953, 1, 7, 0.81], [432, 3, 7, 1.65], [11491, 2, 7, 0.94], [20252, 2, 7, 0.85], [418, 2, 7, 1.68], [4032, 29, 7, 0.9], [1490, 1, 7, 0.76], [1519, 3, 16, 0.69], [2423, 80, 7, 3.06], [11952, 1, 7, 0.85], [411, 2, 7, 0.96], [5151, 2, 7, 1.14], [229, 1, 7, 3.82], [12304, 1, 7, 1.18], [972, 3, 9, 0.93], [11769, 1, 7, 0.88], [3576, 25, 7, 1.68], [2331, 1, 7, 2.67], [346, 1, 7, 0.7], [13034, 3, 7, 4.02], [995, 2, 7, 2.14], [416, 1, 7, 1.91], [2424, 29, 7, 2.13], [3, 2, 7, 1.01], [11426, 25, 7, 1.07], [11737, 2, 7, 0.91], [11767, 1, 7, 0.88], [5076, 1, 7, 1.18], [439, 1, 7, 3.23], [11490, 1, 7, 1.08], [2805, 137, 7, 1.99], [2160, 68, 7, 2.19], [6494, 1, 7, 3.12], [950, 1, 7, 0.76], [414, 1, 7, 1.47], [3575, 25, 7, 1.81], [12764, 2, 8, 0.87], [8677, 3, 8, 1.86], [1701, 2, 7, 3.79], [11180, 1, 7, 1.04], [11586, 1, 14, 3.12], [75, 2, 7, 1.94], [3577, 25, 7, 0.77], [3478, 2, 7, 1.65], [11585, 29, 7, 2.06], [9998, 80, 7, 0.77], [11813, 1, 7, 3.17], [13023, 3, 8, 2.24], [2438, 2, 8, 1.84], [9784, 1, 7, 1.61], [2424, 80, 146, 3.69], [346, 3, 245, 2.39], [3334, 5, 70, 4.81], [20927, 1, 68, 2.36], [12351, 1, 536, 2.11], [7885, 4, 120, 2.4], [6098, 80, 30, 3.45], [6097, 29, 23, 5.08], [11089, 1, 149, 2.22], [12345, 1, 536, 2.26], [10149, 3, 346, 3.62], [20256, 2, 37, 2.55], [147, 1, 77, 3.78], [22316, 3, 273, 2.08], [1492, 1, 15, 3.66], [11953, 1, 172, 2.22], [432, 3, 118, 2.82], [11491, 2, 121, 2.36], [20252, 2, 36, 2.53], [418, 2, 121, 3.09], [4032, 29, 38, 2.55], [1490, 1, 44, 2.18], [1519, 3, 864, 1.89], [2423, 80, 155, 4.47], [11952, 1, 172, 2.27], [411, 2, 42, 2.61], [5151, 2, 21, 2.55], [229, 1, 70, 5.24], [12304, 1, 97, 2.59], [972, 3, 233, 2.55], [11769, 1, 140, 2.3], [3576, 25, 87, 3.09], [2331, 1, 100, 4.08], [346, 1, 62, 2.39], [13034, 3, 228, 5.21], [995, 2, 206, 3.55], [416, 1, 33, 2.59], [2424, 29, 29, 3.54], [3, 2, 105, 2.43], [11426, 25, 103, 2.49], [11737, 2, 49, 2.33], [11767, 1, 140, 2.3], [5076, 1, 112, 2.59], [439, 1, 74, 4.64], [11490, 1, 42, 2.71], [2805, 137, 154, 3.41], [2160, 68, 112, 3.61], [6494, 1, 42, 4.54], [950, 1, 51, 2.18], [414, 1, 74, 2.89], [3575, 25, 87, 3.22], [12764, 2, 646, 2.28], [8677, 3, 253, 3.28], [1701, 2, 63, 4.58], [11180, 1, 34, 2.67], [11586, 1, 147, 3.61], [75, 2, 124, 3.36], [3577, 25, 76, 2.18], [3478, 2, 65, 3.07], [11585, 29, 149, 3.47], [9998, 80, 107, 2.19], [11813, 1, 266, 4.58], [13023, 3, 509, 3.66], [2438, 2, 551, 3.26], [9784, 1, 61, 3.03]]</t>
-  </si>
-  <si>
-    <t>[[6935, 2, 12, 4.2], [615, 2, 7, 3.33], [2778, 2, 9, 1.07], [305, 2, 7, 0.92], [5493, 2, 7, 2.99], [6936, 2, 11, 4.22], [130, 1, 7, 1.37], [205, 2, 7, 1.02], [616, 2, 7, 2.96], [1504, 2, 7, 1.54], [144, 2, 9, 2.7], [8648, 2, 7, 1.35], [2049, 3, 17, 1.07], [88, 10, 18, 1.22], [8915, 2, 8, 3.38], [326, 2, 7, 2.16], [7036, 1, 7, 3.02], [8650, 2, 7, 1.54], [593, 2, 9, 1.07], [2327, 2, 7, 0.86], [11681, 2, 7, 3.3], [8853, 2, 9, 4.23], [141, 2, 9, 1.19], [2775, 2, 9, 1.07], [206, 2, 9, 0.85], [151, 1, 7, 1.25], [7004, 1, 7, 1.15], [248, 1, 7, 0.8], [11685, 2, 7, 3.69], [3891, 1, 7, 1.68], [3840, 1, 7, 0.72], [2328, 2, 7, 0.96], [2050, 3, 7, 0.64], [5491, 2, 7, 1.61], [2497, 2, 7, 2.68], [2055, 3, 7, 3.41], [143, 2, 7, 1.12], [434, 2, 7, 0.86], [3980, 4, 7, 2.36], [2054, 3, 7, 0.67], [624, 2, 7, 3.92], [8672, 2, 9, 2.44], [362, 2, 7, 1.64], [8649, 2, 7, 2.8], [2776, 2, 9, 1.66], [12870, 1, 7, 3.71], [2057, 3, 7, 0.64], [12350, 1, 7, 1.22], [7886, 4, 7, 1.32], [10574, 3, 8, 3.28], [5165, 1, 7, 2.53], [1006, 2, 7, 1.38], [1446, 2, 7, 0.91], [94, 4, 9, 3.04], [75, 2, 7, 2.87], [523, 2, 7, 1.93], [2991, 3, 7, 4.78], [3495, 3, 21, 1.48], [7084, 3, 7, 1.12], [7005, 1, 7, 1.73], [3975, 4, 7, 2.49], [21793, 1, 7, 4.43], [10149, 3, 21, 1.48], [9760, 29, 7, 0.8], [11404, 2, 7, 1.67], [142, 2, 7, 0.94], [12346, 1, 7, 1.22], [6158, 2, 7, 1.33], [20927, 1, 7, 1.77], [3981, 3, 22, 2.52], [417, 2, 7, 1.5], [5165, 2, 10, 2.64], [2912, 1, 7, 0.8], [3982, 3, 17, 2.34], [8939, 2, 7, 0.89], [1007, 2, 7, 0.98], [11953, 1, 7, 0.96], [2774, 2, 7, 1.95], [33, 1, 7, 2.04], [956, 2, 7, 0.86], [11772, 1, 7, 2.97], [286, 3, 7, 2.44], [7887, 4, 9, 0.87], [6497, 1, 7, 2.42], [1492, 1, 7, 2.27], [11767, 1, 7, 0.81], [432, 3, 7, 0.86], [336, 15, 7, 2.22], [972, 3, 7, 2.05], [11769, 1, 7, 1.46], [11490, 1, 7, 2.0], [11770, 1, 7, 1.8], [410, 1, 7, 1.49], [389, 4, 7, 2.13], [2912, 2, 8, 0.79], [74, 1, 7, 2.13], [6496, 1, 7, 0.85], [7567, 3, 7, 3.18], [1413, 15, 7, 1.04], [35, 1, 7, 1.54], [411, 2, 7, 1.02], [4253, 1, 7, 1.5], [22317, 3, 7, 0.92], [140, 2, 7, 1.7], [8673, 2, 7, 2.48], [8121, 3, 6, 0.85], [1126, 2, 7, 1.26], [4176, 4, 9, 3.25], [2436, 4, 9, 0.73], [9372, 1, 7, 3.34], [8676, 2, 7, 3.11], [21269, 3, 7, 4.87], [8677, 3, 7, 1.51], [22247, 2, 7, 2.66], [10388, 2, 7, 2.13], [10936, 2, 7, 3.12], [12343, 1, 7, 1.22], [12526, 2, 7, 2.15], [11085, 2, 8, 3.16], [9784, 1, 7, 1.01], [12269, 2, 7, 1.9], [37, 1, 7, 1.7], [6494, 1, 7, 2.34], [1274, 1, 9, 1.03], [13023, 3, 7, 2.32], [1429, 2, 7, 0.91], [7573, 1, 9, 2.67], [12225, 1, 7, 2.51], [345, 3, 7, 2.52], [12271, 2, 7, 1.86], [3, 2, 7, 0.7], [3577, 25, 7, 0.92], [96, 11, 22, 1.1], [6158, 2, 103, 2.54], [20927, 1, 68, 3.22], [3981, 3, 623, 3.73], [417, 2, 133, 2.95], [5165, 2, 144, 4.85], [2912, 1, 32, 1.51], [3982, 3, 306, 4.03], [8939, 2, 75, 2.61], [1007, 2, 105, 2.65], [11953, 1, 175, 2.42], [2774, 2, 174, 3.4], [33, 1, 44, 2.74], [956, 2, 93, 2.32], [11772, 1, 84, 4.18], [286, 3, 55, 3.65], [7887, 4, 54, 2.53], [6497, 1, 15, 4.13], [1492, 1, 15, 3.97], [11767, 1, 63, 2.52], [432, 3, 264, 2.32], [336, 15, 96, 3.67], [972, 3, 232, 2.73], [11769, 1, 63, 3.17], [11490, 1, 42, 2.71], [11770, 1, 84, 3.51], [410, 1, 41, 2.7], [389, 4, 81, 3.34], [2912, 2, 342, 2.25], [74, 1, 176, 3.58], [6496, 1, 35, 2.31], [7567, 3, 27, 3.83], [1413, 15, 39, 2.75], [35, 1, 44, 2.75], [411, 2, 42, 2.73], [4253, 1, 145, 2.95], [22317, 3, 273, 2.38], [140, 2, 78, 3.15], [8673, 2, 240, 3.93], [8121, 3, 114, 2.56], [1126, 2, 197, 2.71], [4176, 4, 186, 4.3], [2436, 4, 45, 2.5], [9372, 1, 196, 4.79], [8676, 2, 245, 4.57], [21269, 3, 254, 6.0], [8677, 3, 115, 2.72], [22247, 2, 111, 3.32], [10388, 2, 186, 3.58], [10936, 2, 115, 4.58], [12343, 1, 543, 2.67], [12526, 2, 235, 3.6], [11085, 2, 207, 4.36], [9784, 1, 63, 2.46], [12269, 2, 55, 3.35], [37, 1, 96, 3.15], [6494, 1, 20, 3.55], [1274, 1, 32, 3.06], [13023, 3, 507, 3.78], [1429, 2, 131, 2.36], [7573, 1, 144, 3.67], [12225, 1, 141, 3.96], [345, 3, 115, 3.19], [12271, 2, 55, 3.31], [3, 2, 106, 2.15], [3577, 25, 35, 2.59], [96, 11, 330, 2.81]]</t>
-  </si>
-  <si>
-    <t>[[6935, 2, 23, 4.99], [305, 2, 7, 1.02], [2328, 2, 7, 1.5], [130, 1, 7, 0.78], [141, 2, 9, 0.74], [2778, 2, 13, 1.27], [8650, 2, 9, 2.9], [5491, 2, 7, 2.52], [2327, 2, 7, 1.21], [8672, 2, 12, 1.28], [6936, 2, 9, 3.46], [143, 2, 7, 4.32], [11681, 2, 13, 3.96], [248, 1, 7, 0.85], [145, 2, 7, 0.77], [205, 2, 7, 1.02], [5493, 2, 7, 2.44], [146, 2, 7, 1.08], [417, 2, 7, 1.0], [589, 2, 9, 0.74], [75, 2, 7, 1.79], [11838, 2, 7, 1.04], [11737, 2, 7, 1.18], [1124, 2, 12, 0.72], [523, 2, 9, 0.96], [8648, 2, 7, 2.96], [8853, 2, 7, 2.71], [12721, 2, 9, 1.59], [615, 2, 7, 2.35], [1005, 2, 7, 1.22], [326, 2, 7, 2.21], [206, 2, 7, 1.21], [8915, 2, 9, 0.71], [8673, 2, 9, 2.44], [144, 2, 7, 1.3], [11739, 2, 7, 1.18], [434, 2, 7, 1.44], [88, 10, 14, 1.5], [2776, 2, 9, 1.21], [435, 2, 7, 1.4], [142, 2, 7, 1.05], [151, 1, 7, 1.36], [8676, 2, 7, 0.9], [6158, 2, 10, 0.73], [2424, 29, 9, 0.85], [8649, 2, 7, 2.29], [2423, 29, 7, 3.48], [11738, 2, 7, 1.18], [2497, 2, 7, 1.06], [7704, 2, 7, 2.08], [2424, 80, 9, 1.21], [1413, 15, 9, 1.91], [10574, 3, 9, 3.0], [2423, 80, 7, 3.37], [3670, 2, 9, 3.61], [11836, 2, 9, 0.79], [7705, 2, 7, 2.28], [2054, 3, 7, 2.1], [3, 2, 7, 0.83], [2859, 15, 7, 2.41], [412, 1, 9, 1.44], [7706, 2, 7, 2.08], [378, 2, 7, 4.55], [12720, 2, 7, 1.89], [22316, 3, 7, 0.85], [2055, 3, 7, 0.88], [12344, 1, 7, 0.88], [3478, 2, 9, 2.65], [10149, 3, 21, 2.21], [74, 1, 7, 3.39], [3429, 15, 7, 0.85], [2774, 2, 7, 1.06], [307, 2, 7, 2.95], [6497, 1, 7, 0.8], [60, 3, 8, 1.99], [12526, 2, 7, 2.76], [418, 2, 7, 1.49], [7004, 1, 7, 1.96], [13928, 1, 7, 0.74], [411, 2, 7, 0.9], [11089, 1, 7, 0.71], [413, 1, 9, 1.34], [2057, 3, 7, 2.1], [14037, 3, 7, 1.85], [11844, 2, 7, 1.79], [2050, 3, 7, 2.1], [7036, 1, 7, 1.74], [20252, 2, 7, 1.06], [13260, 29, 7, 1.29], [3893, 1, 7, 1.3], [8274, 3, 7, 1.68], [6097, 80, 7, 3.38], [439, 1, 9, 2.21], [6952, 1, 7, 2.01], [3891, 1, 7, 3.83], [94, 4, 7, 2.5], [159, 3, 9, 1.37], [6494, 1, 7, 0.85], [9784, 1, 7, 2.37], [1050, 2, 7, 0.66], [7707, 2, 7, 1.32], [1490, 1, 7, 1.88], [1413, 16, 7, 0.71], [11490, 1, 7, 0.86], [1243, 2, 7, 1.32], [7708, 2, 7, 2.28], [414, 1, 9, 1.63], [3889, 1, 7, 1.17], [1492, 1, 7, 1.13], [5208, 3, 9, 1.82], [565, 2, 7, 0.84], [22317, 3, 8, 0.88], [7703, 2, 7, 2.28], [21793, 1, 7, 1.83], [11491, 2, 7, 1.5], [3495, 3, 21, 1.51], [229, 1, 7, 3.68], [345, 3, 7, 2.32], [2422, 80, 9, 4.33], [6098, 80, 7, 2.19], [410, 1, 7, 0.74], [11504, 2, 7, 1.33], [149, 2, 7, 2.73], [947, 15, 7, 0.71], [6630, 3, 7, 3.21], [3674, 2, 7, 0.96], [147, 1, 7, 2.73], [3430, 15, 7, 2.26], [416, 1, 7, 2.93], [2805, 137, 11, 3.57], [2331, 1, 7, 1.34], [247, 1, 7, 2.33], [9126, 1, 7, 0.87], [3429, 15, 53, 2.63], [2774, 2, 105, 3.11], [307, 2, 72, 5.06], [6497, 1, 38, 2.59], [60, 3, 405, 4.08], [12526, 2, 138, 4.87], [418, 2, 141, 3.27], [7004, 1, 40, 3.07], [13928, 1, 24, 2.85], [411, 2, 109, 2.69], [11089, 1, 173, 2.5], [413, 1, 44, 3.1], [2057, 3, 473, 3.89], [2050, 3, 473, 3.89], [7036, 1, 128, 3.53], [20252, 2, 92, 2.85], [13260, 29, 36, 3.33], [3893, 1, 63, 2.9], [8274, 3, 115, 2.76], [6097, 80, 35, 5.49], [439, 1, 43, 4.81], [6952, 1, 189, 3.79], [3891, 1, 123, 5.62], [94, 4, 60, 4.11], [159, 3, 709, 3.16], [6494, 1, 52, 2.64], [9784, 1, 71, 4.16], [7707, 2, 176, 3.11], [1490, 1, 50, 3.67], [1413, 16, 50, 2.5], [11490, 1, 109, 2.65], [1243, 2, 50, 2.93], [7708, 2, 176, 4.07], [414, 1, 44, 3.31], [3889, 1, 63, 2.78], [1492, 1, 37, 2.92], [5208, 3, 558, 3.6], [565, 2, 176, 2.63], [22317, 3, 318, 2.66], [7703, 2, 176, 4.07], [21793, 1, 123, 2.94], [11491, 2, 141, 3.28], [3495, 3, 965, 3.31], [229, 1, 81, 5.47], [345, 3, 297, 4.1], [2422, 80, 92, 5.46], [6098, 80, 38, 4.03], [410, 1, 53, 2.17], [11504, 2, 141, 3.12], [149, 2, 87, 4.52], [947, 15, 41, 2.5], [6630, 3, 93, 5.0], [3674, 2, 260, 2.74], [147, 1, 87, 4.52], [3430, 15, 69, 4.05], [416, 1, 85, 4.71], [2805, 137, 182, 5.36], [2331, 1, 118, 3.13], [247, 1, 87, 4.12], [9126, 1, 71, 2.65]]</t>
-  </si>
-  <si>
-    <t>[[8672, 2, 12, 2.94], [305, 2, 7, 1.95], [3, 2, 9, 2.18], [6935, 2, 18, 3.39], [205, 2, 7, 1.36], [143, 2, 7, 3.11], [144, 2, 9, 3.22], [75, 2, 7, 0.94], [12721, 2, 10, 1.03], [145, 2, 9, 2.81], [8915, 2, 12, 0.71], [2778, 2, 9, 0.96], [1776, 1, 7, 0.87], [146, 2, 9, 3.31], [206, 2, 7, 1.02], [20252, 2, 7, 0.88], [6936, 2, 10, 2.86], [1777, 1, 9, 2.87], [8648, 2, 7, 1.71], [151, 1, 7, 0.67], [2328, 2, 7, 1.41], [8650, 2, 9, 2.48], [5151, 2, 7, 3.43], [2050, 3, 7, 2.04], [248, 1, 7, 0.8], [7886, 4, 7, 1.22], [88, 10, 21, 3.14], [9507, 3, 7, 0.66], [74, 1, 7, 1.54], [1446, 2, 7, 1.51], [2991, 3, 7, 3.64], [362, 2, 7, 0.83], [7004, 1, 7, 1.29], [2057, 3, 7, 1.01], [1492, 1, 9, 1.36], [1007, 2, 12, 0.69], [2055, 3, 7, 1.04], [147, 1, 7, 4.17], [76, 2, 7, 1.42], [8649, 2, 9, 2.6], [3889, 1, 7, 0.81], [11234, 2, 11, 0.93], [410, 1, 7, 0.7], [7005, 1, 7, 0.91], [345, 3, 7, 0.9], [10, 2, 9, 1.21], [1429, 2, 7, 1.46], [307, 2, 7, 3.37], [10825, 21, 13, 1.0], [5081, 2, 7, 1.04], [12870, 1, 7, 1.25], [57, 1, 7, 0.78], [10149, 3, 21, 1.27], [7036, 1, 7, 1.81], [3478, 2, 7, 1.0], [7084, 3, 7, 1.67], [1006, 2, 7, 1.53], [1504, 2, 9, 1.0], [3891, 1, 7, 1.71], [21793, 1, 7, 3.44], [94, 4, 7, 3.06], [167, 3, 7, 1.44], [411, 2, 7, 0.9], [9827, 3, 7, 1.38], [3893, 1, 7, 0.65], [79, 1, 7, 1.08], [33, 1, 9, 1.88], [432, 3, 9, 1.23], [8677, 3, 9, 1.51], [11681, 2, 11, 3.45], [148, 1, 7, 3.1], [96, 11, 24, 0.67], [1490, 1, 9, 0.82], [12225, 1, 7, 1.7], [1124, 2, 11, 0.74], [11737, 2, 7, 1.26], [1243, 2, 7, 0.92], [22247, 2, 11, 1.79], [6158, 2, 8, 1.39], [5812, 3, 8, 3.52], [8853, 2, 14, 4.07], [201, 3, 7, 0.9], [412, 1, 7, 2.46], [9760, 29, 9, 1.04], [10574, 3, 9, 2.6], [8651, 2, 7, 1.63], [20927, 1, 7, 0.83], [5208, 3, 11, 1.25], [8676, 2, 12, 1.23], [229, 1, 7, 2.31], [1767, 25, 9, 1.46], [25, 1, 7, 1.4], [45, 2, 7, 2.7], [9069, 1, 7, 0.79], [413, 1, 7, 2.29], [11490, 1, 7, 0.69], [149, 2, 7, 3.27], [159, 3, 9, 1.18], [3495, 3, 21, 1.61], [998, 2, 7, 1.87], [21269, 3, 7, 2.34], [140, 2, 7, 1.5], [95, 3, 17, 3.57], [3980, 4, 7, 2.46], [950, 1, 7, 1.3], [5946, 1, 7, 1.83], [9372, 1, 7, 3.91], [1126, 2, 7, 1.36], [1766, 25, 7, 1.08], [2775, 2, 7, 1.46], [1413, 15, 9, 1.85], [490, 1, 9, 0.99], [506, 1, 7, 4.76], [8674, 2, 7, 0.99], [11489, 1, 7, 1.21], [8898, 3, 7, 3.23], [997, 2, 7, 3.34], [3670, 2, 7, 3.6], [1070, 7, 15, 0.85], [9691, 1, 7, 1.89], [107, 2, 7, 1.46], [974, 3, 7, 1.64], [20498, 1, 7, 1.81], [11954, 1, 7, 0.87], [14037, 3, 7, 1.3], [823, 1, 7, 1.62], [14017, 3, 9, 1.09], [34, 1, 7, 2.43], [972, 3, 8, 1.49], [5209, 3, 7, 0.98], [9784, 1, 7, 1.51], [11739, 2, 7, 1.26], [20498, 3, 10, 1.16], [432, 3, 146, 2.81], [8677, 3, 142, 2.67], [11681, 2, 129, 5.11], [148, 1, 43, 4.77], [96, 11, 409, 2.32], [1490, 1, 24, 2.48], [12225, 1, 71, 2.57], [1124, 2, 90, 2.7], [11737, 2, 28, 2.92], [1243, 2, 83, 2.22], [22247, 2, 138, 3.38], [6158, 2, 221, 2.69], [5812, 3, 502, 4.82], [8853, 2, 136, 4.71], [201, 3, 147, 2.53], [412, 1, 40, 3.1], [9760, 29, 35, 3.01], [10574, 3, 239, 4.26], [8651, 2, 109, 2.79], [20927, 1, 39, 2.46], [5208, 3, 480, 2.56], [8676, 2, 138, 2.65], [229, 1, 40, 2.95], [1767, 25, 83, 2.76], [25, 1, 95, 2.71], [45, 2, 53, 4.36], [9069, 1, 60, 2.41], [413, 1, 42, 2.94], [11490, 1, 53, 2.32], [149, 2, 43, 4.03], [159, 3, 602, 2.48], [3495, 3, 463, 3.28], [998, 2, 117, 2.54], [21269, 3, 141, 3.5], [140, 2, 44, 3.09], [95, 3, 892, 4.89], [3980, 4, 230, 4.11], [950, 1, 25, 2.17], [5946, 1, 60, 2.48], [9372, 1, 112, 4.69], [1126, 2, 110, 2.52], [1766, 25, 90, 2.69], [2775, 2, 75, 2.63], [1413, 15, 47, 4.01], [490, 1, 29, 2.39], [506, 1, 74, 6.0], [8674, 2, 138, 2.66], [11489, 1, 53, 2.87], [8898, 3, 141, 4.39], [997, 2, 202, 4.64], [3670, 2, 117, 4.37], [1070, 7, 283, 2.51], [9691, 1, 36, 2.54], [107, 2, 31, 2.12], [974, 3, 72, 2.8], [20498, 1, 47, 3.4], [11954, 1, 171, 2.17], [823, 1, 20, 3.2], [14017, 3, 95, 2.47], [34, 1, 54, 3.19], [972, 3, 286, 2.26], [5209, 3, 480, 2.29], [9784, 1, 35, 2.67], [11739, 2, 28, 2.92], [20498, 3, 282, 3.16]]</t>
-  </si>
-  <si>
-    <t>[[8672, 2, 10, 1.01], [305, 2, 7, 1.1], [2049, 3, 13, 0.7], [6935, 2, 21, 3.58], [326, 2, 8, 2.27], [141, 2, 7, 2.25], [144, 2, 7, 1.17], [589, 2, 12, 0.77], [362, 2, 9, 0.83], [151, 1, 7, 0.89], [12721, 2, 10, 1.03], [146, 2, 7, 1.26], [1776, 1, 7, 2.19], [145, 2, 7, 0.8], [206, 2, 7, 0.69], [2328, 2, 7, 1.35], [8915, 2, 11, 0.71], [143, 2, 7, 1.12], [990, 2, 7, 1.06], [6936, 2, 10, 3.41], [20252, 2, 7, 0.91], [8650, 2, 7, 2.27], [1777, 1, 7, 2.96], [1007, 2, 10, 0.81], [2778, 2, 7, 0.79], [248, 1, 7, 1.2], [22247, 2, 9, 1.93], [88, 10, 14, 2.0], [2050, 3, 7, 0.69], [76, 2, 7, 2.39], [8649, 2, 7, 2.74], [10149, 3, 25, 3.53], [2054, 3, 7, 4.0], [10, 2, 11, 2.2], [8677, 3, 8, 3.58], [412, 1, 7, 1.64], [2055, 3, 7, 4.0], [13028, 3, 7, 1.38], [413, 1, 7, 2.12], [7004, 1, 9, 0.89], [411, 2, 7, 0.89], [10825, 21, 14, 2.34], [11681, 2, 10, 4.26], [1446, 2, 7, 1.91], [7084, 3, 7, 1.66], [307, 2, 7, 1.35], [3478, 2, 7, 2.16], [1429, 2, 7, 1.21], [3495, 3, 26, 1.77], [1006, 2, 7, 1.36], [5081, 2, 7, 0.81], [1492, 1, 6, 1.98], [140, 2, 7, 1.98], [7005, 1, 9, 0.89], [167, 3, 9, 3.09], [7036, 1, 7, 2.14], [9827, 3, 7, 1.38], [45, 2, 7, 2.95], [8676, 2, 7, 0.98], [1124, 2, 11, 0.72], [2049, 1, 7, 1.7], [94, 4, 7, 3.47], [13280, 1, 9, 3.64], [5812, 3, 8, 3.38], [1504, 2, 7, 1.33], [12870, 1, 7, 1.5], [168, 3, 9, 1.46], [11234, 2, 8, 1.32], [415, 1, 7, 2.06], [8651, 2, 7, 1.94], [148, 1, 7, 1.56], [418, 2, 7, 0.7], [6097, 29, 7, 3.38], [8853, 2, 14, 3.62], [416, 1, 7, 2.33], [8939, 2, 7, 0.84], [6097, 80, 7, 3.38], [11737, 2, 7, 2.34], [20256, 2, 7, 1.42], [1490, 1, 7, 1.27], [95, 3, 26, 0.85], [20927, 1, 9, 0.89], [79, 1, 7, 0.7], [6098, 29, 7, 2.08], [14017, 3, 7, 1.0], [6098, 80, 7, 2.08], [414, 1, 7, 1.49], [9069, 1, 7, 1.91], [1070, 7, 16, 0.73], [8898, 3, 7, 2.67], [1126, 2, 7, 1.22], [13034, 3, 8, 3.38], [126, 2, 7, 2.75], [20498, 1, 7, 1.96], [9760, 29, 7, 0.87], [5086, 1, 9, 1.76], [20255, 2, 7, 1.43], [12924, 1, 9, 0.86], [5513, 2, 7, 0.84], [9784, 1, 7, 1.06], [336, 15, 7, 1.66], [13260, 29, 7, 1.0], [22317, 3, 8, 1.35], [7567, 3, 7, 3.2], [1413, 15, 7, 1.52], [229, 1, 7, 2.92], [11085, 2, 7, 0.83], [5811, 3, 7, 2.82], [5813, 3, 9, 2.14], [192, 3, 22, 4.76], [8557, 3, 7, 1.01], [9082, 3, 20, 2.38], [506, 1, 7, 2.73], [3049, 3, 7, 3.65], [20498, 3, 8, 2.02], [9691, 1, 9, 2.48], [14018, 3, 7, 1.0], [524, 1, 7, 2.16], [4076, 3, 7, 2.96], [470, 1, 7, 1.35], [8943, 3, 7, 3.03], [1622, 1, 10, 0.79], [9372, 1, 7, 2.03], [20486, 3, 8, 1.86], [2775, 2, 9, 0.73], [13023, 3, 8, 2.94], [1703, 2, 7, 1.51], [11454, 2, 9, 3.65], [2423, 80, 7, 3.68], [3900, 3, 7, 3.14], [5584, 3, 7, 2.74], [2424, 80, 7, 3.75], [2497, 2, 7, 0.78], [415, 1, 30, 2.31], [8651, 2, 79, 2.71], [148, 1, 80, 2.71], [418, 2, 131, 1.85], [6097, 29, 12, 4.65], [8853, 2, 97, 4.88], [416, 1, 30, 2.57], [8939, 2, 67, 2.11], [6097, 80, 24, 4.65], [11737, 2, 20, 3.11], [20256, 2, 33, 2.19], [1490, 1, 18, 2.03], [95, 3, 390, 2.19], [20927, 1, 28, 1.93], [79, 1, 44, 1.85], [6098, 29, 13, 3.21], [14017, 3, 69, 2.22], [6098, 80, 27, 3.2], [414, 1, 79, 2.64], [9069, 1, 43, 2.17], [1070, 7, 206, 2.01], [8898, 3, 102, 3.94], [1126, 2, 80, 1.99], [13034, 3, 203, 4.14], [126, 2, 32, 2.98], [20498, 1, 34, 2.73], [9760, 29, 25, 2.09], [5086, 1, 63, 3.49], [20255, 2, 33, 2.2], [12924, 1, 19, 2.3], [5513, 2, 70, 1.99], [9784, 1, 25, 2.28], [336, 15, 40, 1.92], [13260, 29, 67, 2.15], [22317, 3, 109, 2.11], [7567, 3, 24, 3.41], [1413, 15, 34, 2.79], [229, 1, 75, 4.08], [11085, 2, 508, 1.97], [5811, 3, 203, 3.58], [5813, 3, 203, 3.24], [192, 3, 1287, 5.9], [8557, 3, 70, 2.28], [9082, 3, 845, 3.66], [506, 1, 80, 3.88], [3049, 3, 48, 4.42], [20498, 3, 204, 2.76], [9691, 1, 27, 2.98], [14018, 3, 69, 2.22], [524, 1, 30, 2.41], [4076, 3, 71, 3.19], [470, 1, 12, 2.12], [8943, 3, 137, 4.31], [1622, 1, 50, 1.56], [9372, 1, 210, 3.18], [20486, 3, 208, 2.61], [2775, 2, 55, 2.06], [13023, 3, 203, 3.7], [1703, 2, 149, 2.66], [11454, 2, 114, 4.42], [2423, 80, 169, 4.83], [3900, 3, 15, 3.35], [5584, 3, 86, 3.51], [2424, 80, 153, 4.9], [2497, 2, 189, 1.94]]</t>
-  </si>
-  <si>
-    <t>[[11685, 2, 7, 3.69], [6935, 2, 10, 4.2], [326, 2, 9, 2.77], [8648, 2, 7, 1.35], [144, 2, 9, 2.2], [593, 2, 7, 1.57], [2327, 2, 7, 0.9], [143, 2, 7, 1.57], [205, 2, 7, 1.48], [8915, 2, 8, 3.38], [2328, 2, 7, 1.41], [6936, 2, 9, 4.22], [11681, 2, 7, 3.3], [305, 2, 7, 1.38], [151, 1, 7, 1.25], [8650, 2, 7, 1.1], [141, 2, 7, 0.92], [206, 2, 7, 1.35], [2778, 2, 9, 1.07], [2049, 3, 14, 0.83], [88, 10, 18, 1.22], [615, 2, 7, 3.33], [7036, 1, 7, 3.02], [8853, 2, 7, 4.23], [8649, 2, 7, 1.87], [5491, 2, 7, 0.9], [434, 2, 7, 0.86], [1006, 2, 7, 1.93], [75, 2, 7, 2.32], [2055, 3, 7, 3.41], [11737, 2, 7, 1.58], [417, 2, 7, 1.5], [616, 2, 7, 2.96], [3840, 1, 7, 0.72], [2050, 3, 7, 0.67], [1007, 2, 7, 1.44], [12353, 1, 9, 2.27], [12870, 1, 7, 3.71], [523, 2, 7, 1.93], [1504, 2, 7, 2.06], [159, 3, 8, 0.61], [20927, 1, 7, 1.77], [2057, 3, 9, 0.88], [13280, 1, 9, 5.0], [3, 2, 9, 0.74], [10574, 3, 8, 2.36], [142, 2, 7, 0.94], [12346, 1, 9, 1.93], [7084, 3, 7, 1.12], [624, 2, 7, 3.92], [9760, 29, 7, 1.3], [2054, 3, 9, 0.88], [140, 2, 7, 1.7], [2775, 2, 7, 1.07], [3891, 1, 7, 0.98], [21793, 1, 7, 4.43], [8939, 2, 7, 0.89], [1429, 2, 7, 1.38], [6158, 2, 9, 0.75], [11739, 2, 7, 1.14], [96, 11, 22, 1.59], [950, 1, 7, 0.68], [5165, 2, 8, 3.15], [12269, 2, 7, 1.9], [84, 2, 7, 1.96], [9372, 1, 7, 3.34], [1126, 2, 7, 1.26], [10388, 2, 7, 2.13], [411, 2, 7, 1.02], [98, 11, 16, 0.91], [972, 3, 7, 2.05], [8672, 2, 9, 2.94], [5165, 1, 7, 3.03], [413, 1, 7, 1.94], [8898, 3, 7, 5.0], [2912, 1, 7, 0.8], [2776, 2, 7, 2.59], [410, 1, 7, 1.04], [12343, 1, 7, 3.27], [10386, 2, 7, 1.68], [995, 2, 7, 3.38], [956, 2, 7, 0.86], [1492, 1, 7, 2.77], [418, 2, 7, 0.81], [12345, 1, 7, 2.72], [13928, 1, 7, 0.87], [9784, 1, 7, 0.9], [22316, 3, 7, 0.92], [147, 1, 7, 0.98], [412, 1, 7, 0.92], [22247, 2, 7, 2.43], [957, 2, 7, 1.01], [336, 15, 7, 1.66], [8677, 3, 7, 1.73], [11490, 1, 7, 1.02], [7567, 3, 7, 3.18], [2912, 2, 8, 0.79], [432, 3, 7, 0.86], [308, 1, 7, 3.28], [307, 2, 7, 1.58], [11953, 1, 7, 0.96], [33, 1, 7, 2.04], [11770, 1, 9, 1.3], [10631, 2, 7, 2.7], [414, 1, 7, 1.24], [35, 1, 7, 1.7], [20256, 2, 7, 0.81], [22317, 3, 7, 1.42], [10407, 10, 10, 2.88], [148, 1, 7, 1.0], [1413, 15, 7, 1.17], [10780, 10, 7, 3.0], [10410, 10, 10, 3.2], [13286, 1, 7, 2.52], [439, 1, 7, 2.12], [7573, 1, 11, 3.36], [335, 3, 15, 3.35], [7886, 4, 7, 0.86], [9691, 1, 7, 1.0], [11767, 1, 7, 0.92], [972, 1, 7, 2.77], [12347, 1, 7, 3.27], [10387, 2, 7, 1.75], [6497, 1, 7, 0.95], [74, 1, 7, 2.13], [20686, 1, 7, 2.96], [3478, 2, 7, 3.14], [12271, 2, 7, 1.86], [9971, 2, 7, 2.77], [8897, 3, 7, 5.0], [2331, 1, 7, 2.08], [11769, 1, 7, 2.06], [9082, 3, 34, 1.7], [411, 2, 42, 2.73], [98, 11, 720, 2.35], [972, 3, 232, 2.73], [8672, 2, 112, 4.65], [413, 1, 34, 2.64], [8898, 3, 242, 6.0], [2912, 1, 32, 1.51], [2776, 2, 135, 4.04], [410, 1, 41, 2.7], [12343, 1, 241, 4.47], [10386, 2, 186, 3.14], [995, 2, 208, 4.83], [956, 2, 93, 2.32], [1492, 1, 15, 3.97], [418, 2, 55, 2.48], [12345, 1, 241, 3.94], [13928, 1, 42, 2.32], [9784, 1, 29, 2.57], [22316, 3, 273, 2.38], [147, 1, 79, 2.43], [412, 1, 73, 2.37], [22247, 2, 243, 3.88], [957, 2, 93, 2.46], [336, 15, 45, 2.36], [8677, 3, 115, 2.72], [11490, 1, 94, 2.47], [7567, 3, 27, 3.83], [2912, 2, 342, 2.25], [432, 3, 118, 2.57], [308, 1, 139, 4.73], [307, 2, 58, 2.78], [11953, 1, 175, 2.42], [33, 1, 44, 2.74], [11770, 1, 84, 3.51], [10631, 2, 183, 4.15], [414, 1, 74, 2.69], [35, 1, 96, 3.15], [20256, 2, 81, 2.26], [22317, 3, 123, 2.63], [10407, 10, 1015, 4.32], [148, 1, 79, 2.46], [1413, 15, 86, 2.63], [10780, 10, 316, 4.46], [10410, 10, 1015, 4.64], [13286, 1, 123, 3.2], [439, 1, 75, 3.57], [7573, 1, 288, 4.82], [335, 3, 1103, 4.78], [7886, 4, 99, 2.22], [9691, 1, 66, 2.45], [11767, 1, 139, 2.37], [972, 1, 85, 4.22], [12347, 1, 241, 4.47], [10387, 2, 186, 3.2], [6497, 1, 33, 2.4], [74, 1, 176, 3.58], [20686, 1, 237, 4.17], [3478, 2, 30, 3.79], [12271, 2, 55, 3.31], [9971, 2, 108, 3.59], [8897, 3, 242, 6.0], [2331, 1, 47, 2.78], [11769, 1, 139, 3.51], [9082, 3, 948, 3.83]]</t>
-  </si>
-  <si>
-    <t>[[8672, 2, 10, 1.03], [141, 2, 7, 0.94], [362, 2, 7, 0.88], [361, 2, 6, 0.99], [6935, 2, 23, 3.83], [205, 2, 7, 0.65], [12721, 2, 11, 2.8], [11737, 2, 7, 1.23], [206, 2, 7, 0.7], [2049, 3, 17, 0.72], [8676, 2, 7, 2.44], [8675, 2, 9, 1.42], [417, 2, 7, 1.55], [3, 2, 7, 0.96], [6936, 2, 7, 3.04], [305, 2, 7, 1.48], [151, 1, 7, 1.36], [523, 2, 7, 1.13], [22247, 2, 7, 1.83], [8650, 2, 7, 2.33], [142, 2, 7, 0.9], [8648, 2, 7, 3.27], [2328, 2, 7, 1.5], [2776, 2, 7, 1.18], [8853, 2, 7, 3.03], [616, 2, 7, 2.22], [11739, 2, 7, 1.23], [2327, 2, 7, 1.66], [11837, 2, 7, 0.82], [12352, 1, 7, 3.09], [411, 2, 7, 0.86], [589, 2, 7, 0.8], [143, 2, 7, 1.6], [146, 2, 7, 1.14], [11835, 2, 7, 1.06], [412, 1, 7, 1.93], [12353, 1, 7, 3.09], [6497, 1, 9, 1.34], [583, 2, 7, 2.85], [8674, 2, 7, 1.17], [145, 2, 7, 0.9], [2805, 137, 14, 1.1], [326, 2, 7, 2.54], [10574, 3, 9, 2.49], [418, 2, 7, 1.0], [144, 2, 7, 0.96], [6097, 80, 7, 3.38], [11836, 2, 7, 0.97], [11738, 2, 7, 1.23], [9784, 1, 7, 1.91], [10149, 3, 21, 0.86], [413, 1, 7, 1.87], [6097, 29, 7, 3.88], [2057, 3, 7, 3.23], [75, 2, 7, 1.04], [11234, 2, 8, 1.32], [2055, 3, 7, 3.23], [1413, 15, 7, 0.89], [12344, 1, 7, 2.54], [20252, 2, 7, 0.87], [11504, 2, 7, 0.67], [12269, 2, 7, 1.05], [8915, 2, 7, 0.71], [414, 1, 7, 1.91], [1492, 1, 7, 1.13], [6098, 80, 7, 2.19], [12346, 1, 7, 3.09], [247, 1, 7, 3.32], [3429, 15, 7, 0.85], [22316, 3, 7, 0.85], [2774, 2, 7, 2.72], [1490, 1, 7, 0.66], [416, 1, 7, 2.14], [6098, 29, 7, 2.55], [9786, 1, 7, 2.84], [3934, 5, 8, 0.94], [2859, 15, 7, 1.05], [2049, 1, 7, 0.75], [201, 3, 7, 2.66], [3670, 2, 9, 3.61], [20555, 2, 7, 1.23], [6158, 2, 9, 1.76], [3478, 2, 7, 2.16], [7084, 3, 7, 1.81], [9785, 1, 7, 1.91], [12526, 2, 7, 2.78], [8599, 1, 7, 2.59], [3430, 15, 7, 0.65], [8938, 2, 7, 1.06], [1703, 2, 7, 1.53], [4253, 1, 7, 0.92], [9760, 29, 7, 1.83], [186, 3, 12, 0.9], [1413, 16, 7, 0.68], [229, 1, 7, 2.94], [11885, 2, 7, 0.71], [107, 2, 7, 2.38], [11887, 2, 8, 0.65], [1050, 2, 7, 0.68], [11811, 1, 7, 1.93], [94, 4, 7, 4.01], [4232, 80, 7, 3.23], [11490, 1, 7, 0.95], [436, 2, 7, 0.94], [107, 7, 8, 1.99], [947, 15, 7, 0.71], [2438, 2, 8, 2.38], [415, 1, 7, 2.14], [11770, 1, 7, 0.8], [3673, 2, 7, 3.82], [11767, 1, 7, 0.88], [2821, 3, 13, 0.77], [11769, 1, 7, 0.88], [5939, 3, 7, 0.91], [11671, 1, 7, 0.83], [11160, 1, 7, 3.67], [11844, 2, 7, 1.16], [9491, 21, 16, 0.87], [12347, 1, 7, 3.55], [5812, 3, 7, 4.0], [7036, 1, 7, 0.87], [9358, 1, 7, 0.81], [140, 2, 7, 2.41], [5813, 3, 8, 1.92], [3495, 3, 21, 1.51], [12764, 2, 8, 0.82], [11771, 1, 7, 3.17], [11954, 1, 7, 0.77], [23920, 2, 7, 0.85], [9690, 1, 7, 1.45], [410, 1, 7, 2.74], [5811, 3, 8, 3.52], [308, 1, 11, 1.83], [247, 1, 86, 5.11], [3429, 15, 53, 2.63], [22316, 3, 318, 2.64], [2774, 2, 205, 4.5], [1490, 1, 51, 2.45], [416, 1, 86, 3.92], [6098, 29, 37, 4.34], [9786, 1, 48, 4.45], [3934, 5, 586, 2.73], [2859, 15, 69, 2.84], [2049, 1, 15, 2.36], [201, 3, 299, 4.45], [3670, 2, 236, 5.41], [20555, 2, 57, 3.01], [6158, 2, 259, 3.55], [3478, 2, 75, 3.95], [7084, 3, 65, 3.92], [9785, 1, 36, 3.01], [12526, 2, 272, 4.56], [8599, 1, 145, 4.37], [3430, 15, 71, 2.44], [8938, 2, 192, 2.85], [1703, 2, 164, 3.32], [4253, 1, 171, 2.71], [9760, 29, 36, 2.93], [186, 3, 665, 2.69], [1413, 16, 50, 2.47], [229, 1, 80, 4.73], [11885, 2, 97, 2.14], [107, 2, 48, 4.16], [11887, 2, 130, 2.26], [11811, 1, 451, 3.72], [94, 4, 119, 5.8], [4232, 80, 153, 5.02], [11490, 1, 110, 2.74], [436, 2, 107, 2.72], [107, 7, 122, 3.2], [947, 15, 41, 2.5], [2438, 2, 643, 4.17], [415, 1, 86, 3.92], [11770, 1, 220, 2.59], [3673, 2, 236, 5.61], [11767, 1, 164, 2.67], [2821, 3, 1338, 2.55], [11769, 1, 164, 2.67], [5939, 3, 266, 2.71], [11671, 1, 310, 2.62], [11160, 1, 490, 5.45], [11844, 2, 186, 2.77], [9491, 21, 1065, 2.98], [12347, 1, 607, 5.34], [5812, 3, 589, 5.78], [7036, 1, 127, 2.65], [9358, 1, 59, 2.6], [140, 2, 45, 3.84], [5813, 3, 589, 3.7], [3495, 3, 965, 3.31], [12764, 2, 755, 2.62], [11771, 1, 213, 4.96], [11954, 1, 203, 2.56], [23920, 2, 106, 2.63], [9690, 1, 75, 3.24], [410, 1, 35, 3.81], [5811, 3, 296, 5.12], [308, 1, 173, 3.62]]</t>
-  </si>
-  <si>
-    <t>[[2327, 2, 7, 1.0], [305, 2, 7, 1.32], [6935, 2, 11, 4.28], [2778, 2, 9, 0.81], [144, 2, 9, 2.22], [130, 1, 7, 1.38], [8915, 2, 8, 1.9], [589, 2, 10, 0.99], [143, 2, 7, 1.12], [2328, 2, 7, 1.73], [6936, 2, 7, 3.42], [8648, 2, 7, 1.93], [2775, 2, 9, 0.94], [205, 2, 7, 0.83], [8650, 2, 7, 1.47], [326, 2, 9, 1.62], [593, 2, 9, 0.88], [146, 2, 7, 1.55], [145, 2, 7, 0.98], [7036, 1, 9, 2.3], [3840, 1, 7, 1.09], [2049, 3, 10, 0.87], [2776, 2, 9, 0.94], [615, 2, 9, 0.87], [616, 2, 9, 0.66], [88, 10, 16, 2.46], [141, 2, 7, 0.71], [151, 1, 7, 1.36], [1124, 2, 7, 1.46], [11681, 2, 11, 3.45], [206, 2, 7, 0.74], [1446, 2, 7, 1.22], [9760, 29, 7, 1.18], [8853, 2, 7, 3.51], [990, 2, 7, 0.66], [5491, 2, 9, 1.44], [1007, 2, 7, 0.85], [362, 2, 9, 1.24], [8672, 2, 7, 2.94], [1504, 2, 7, 1.79], [2055, 3, 7, 0.84], [9372, 1, 7, 3.79], [2057, 3, 7, 0.84], [3893, 1, 7, 1.48], [8649, 2, 7, 1.29], [8938, 2, 7, 0.95], [434, 2, 9, 0.71], [12870, 1, 7, 2.35], [624, 2, 7, 2.19], [2050, 3, 7, 0.84], [417, 2, 9, 1.04], [3889, 1, 7, 0.65], [5165, 1, 7, 2.49], [1429, 2, 7, 0.91], [378, 2, 7, 4.21], [7084, 3, 7, 1.58], [10, 2, 7, 1.6], [2991, 3, 7, 3.64], [140, 2, 7, 2.34], [3891, 1, 7, 0.98], [1006, 2, 7, 1.04], [7886, 4, 7, 0.75], [10574, 3, 11, 3.29], [7573, 1, 22, 5.0], [10149, 3, 21, 1.48], [5208, 3, 9, 0.88], [1622, 1, 7, 0.82], [75, 2, 7, 0.75], [3, 2, 7, 0.89], [20927, 1, 7, 1.83], [5165, 2, 10, 2.34], [997, 2, 7, 2.64], [11234, 2, 7, 2.3], [12721, 2, 7, 1.26], [22247, 2, 7, 2.64], [147, 1, 7, 3.37], [346, 3, 9, 0.69], [996, 2, 7, 2.83], [11811, 1, 7, 0.8], [229, 1, 7, 1.0], [20252, 2, 7, 1.43], [11685, 2, 11, 3.45], [998, 2, 7, 3.33], [94, 4, 7, 3.68], [972, 3, 8, 1.36], [9491, 21, 17, 0.8], [76, 2, 7, 1.67], [35, 1, 7, 1.96], [439, 1, 9, 2.21], [6158, 2, 7, 4.79], [413, 1, 7, 2.08], [13028, 3, 7, 4.24], [13928, 1, 7, 1.28], [8104, 1, 7, 1.67], [5076, 1, 7, 0.83], [2805, 137, 7, 1.16], [5209, 3, 9, 0.78], [412, 1, 7, 1.85], [8676, 2, 7, 4.08], [33, 1, 7, 1.87], [83, 2, 7, 1.69], [418, 2, 7, 1.21], [148, 1, 7, 3.39], [2774, 2, 7, 1.15], [3495, 3, 16, 1.41], [8898, 3, 7, 3.35], [12212, 29, 7, 0.98], [7887, 4, 7, 1.81], [20256, 2, 9, 0.82], [38, 1, 7, 2.23], [11490, 1, 7, 1.29], [11770, 1, 7, 2.76], [34, 1, 7, 2.1], [10407, 10, 10, 3.59], [415, 1, 7, 1.0], [9784, 1, 7, 0.96], [84, 2, 7, 1.87], [126, 2, 7, 2.34], [411, 2, 7, 0.89], [13928, 2, 7, 1.35], [11739, 2, 7, 2.61], [9691, 1, 7, 1.05], [3048, 3, 7, 4.58], [9690, 1, 7, 0.69], [8939, 2, 7, 0.92], [5584, 3, 7, 2.81], [11953, 1, 7, 0.84], [39, 1, 7, 2.18], [12351, 1, 7, 1.22], [10410, 10, 15, 3.84], [11954, 1, 7, 0.7], [12764, 2, 8, 0.64], [7567, 3, 7, 2.64], [75, 2, 72, 2.69], [3, 2, 59, 2.81], [20927, 1, 30, 2.64], [5165, 2, 180, 4.82], [997, 2, 232, 4.28], [11234, 2, 179, 3.94], [12721, 2, 139, 3.23], [22247, 2, 139, 3.57], [147, 1, 43, 4.28], [346, 3, 308, 2.68], [996, 2, 115, 4.81], [11811, 1, 222, 2.78], [229, 1, 81, 2.64], [20252, 2, 91, 3.07], [11685, 2, 131, 5.43], [998, 2, 115, 4.81], [94, 4, 60, 4.77], [972, 3, 291, 2.82], [9491, 21, 1034, 2.76], [76, 2, 54, 2.65], [35, 1, 54, 2.93], [439, 1, 42, 4.69], [6158, 2, 249, 6.0], [413, 1, 42, 3.04], [13028, 3, 72, 5.72], [13928, 1, 24, 3.26], [8104, 1, 99, 3.59], [5076, 1, 64, 2.77], [2805, 137, 90, 3.08], [5209, 3, 273, 2.87], [412, 1, 41, 3.83], [8676, 2, 274, 5.72], [33, 1, 54, 3.76], [418, 2, 69, 3.13], [148, 1, 43, 4.3], [2774, 2, 200, 2.79], [3495, 3, 938, 3.05], [8898, 3, 144, 4.83], [12212, 29, 58, 2.95], [7887, 4, 34, 2.3], [20256, 2, 46, 2.94], [38, 1, 54, 3.19], [11490, 1, 54, 2.77], [11770, 1, 206, 4.4], [34, 1, 54, 3.07], [10407, 10, 569, 5.06], [415, 1, 42, 2.92], [9784, 1, 71, 2.6], [84, 2, 33, 2.85], [126, 2, 86, 3.98], [411, 2, 106, 2.53], [13928, 2, 12, 3.26], [11739, 2, 55, 4.25], [9691, 1, 74, 2.7], [3048, 3, 137, 6.0], [9690, 1, 25, 1.68], [8939, 2, 93, 2.9], [5584, 3, 120, 4.28], [11953, 1, 195, 2.48], [39, 1, 54, 3.13], [12351, 1, 612, 2.87], [10410, 10, 569, 5.1], [11954, 1, 195, 2.34], [12764, 2, 358, 2.62], [7567, 3, 34, 4.12]]</t>
+    <t>[[2778, 2, 5, 0.2], [6935, 2, 7, 1.05], [6936, 2, 4, 1.57], [305, 2, 4, 0.53], [8672, 2, 5, 0.58], [615, 2, 4, 0.71], [1504, 2, 5, 0.37], [2775, 2, 5, 0.2], [145, 2, 5, 0.4], [2776, 2, 4, 0.8], [8853, 2, 4, 1.54], [2327, 2, 4, 0.63], [12721, 2, 5, 0.73], [130, 1, 4, 0.2], [143, 2, 4, 1.01], [146, 2, 4, 0.56], [2328, 2, 4, 0.78], [11681, 2, 5, 0.94], [11737, 2, 4, 0.53], [616, 2, 4, 1.09], [5491, 2, 4, 0.56], [141, 2, 4, 0.79], [362, 2, 5, 0.2], [144, 2, 4, 0.44], [2497, 2, 4, 0.45], [205, 2, 4, 0.46], [8650, 2, 4, 0.39], [5493, 2, 4, 0.2], [417, 2, 5, 0.57], [8676, 2, 4, 0.47], [8673, 2, 4, 0.24], [3670, 2, 4, 1.02], [2774, 2, 5, 0.33], [8648, 2, 4, 1.91], [589, 2, 5, 0.2], [3, 2, 5, 0.53], [206, 2, 4, 0.2], [6097, 80, 4, 1.14], [2423, 29, 4, 1.16], [22247, 2, 4, 1.01], [11836, 2, 4, 0.49], [6497, 1, 4, 0.5], [8674, 2, 5, 0.49], [624, 2, 4, 1.26], [12343, 1, 4, 0.87], [2055, 3, 4, 1.18], [2423, 80, 4, 1.1], [523, 2, 4, 0.68], [12344, 1, 4, 0.87], [593, 2, 5, 0.45], [6097, 29, 4, 1.14], [6098, 80, 5, 0.58], [12720, 2, 4, 0.82], [12345, 1, 4, 0.87], [11739, 2, 4, 0.53], [75, 2, 4, 1.17], [8915, 2, 4, 0.41], [88, 10, 9, 0.82], [326, 2, 4, 1.54], [6494, 1, 4, 0.46], [60, 3, 6, 0.19], [13260, 29, 4, 0.36], [142, 2, 4, 0.79], [3429, 15, 4, 0.46], [1492, 1, 4, 0.62], [411, 2, 4, 0.57], [21712, 3, 13, 0.67], [412, 1, 4, 1.0], [2422, 80, 4, 1.31], [1050, 2, 4, 0.38], [10149, 3, 13, 1.12], [2422, 29, 5, 1.19], [378, 2, 4, 1.16], [6098, 29, 4, 1.08], [12346, 1, 4, 0.87], [151, 1, 4, 0.75], [7704, 2, 4, 1.15], [11738, 2, 4, 0.53], [229, 1, 4, 2.0], [22316, 3, 4, 0.46], [1243, 2, 4, 0.72], [1049, 2, 4, 0.38], [20252, 2, 4, 0.58], [13264, 29, 4, 0.52], [345, 3, 4, 1.26], [13258, 29, 4, 1.26], [1490, 1, 4, 0.47], [12269, 2, 4, 0.51], [964, 15, 4, 0.36], [2438, 1, 4, 1.05], [10407, 10, 6, 1.27], [1163, 3, 5, 0.58], [5208, 3, 5, 0.74], [2331, 1, 4, 0.55], [2821, 3, 10, 0.23], [416, 1, 4, 1.66], [201, 3, 4, 1.26], [307, 2, 4, 1.04], [186, 3, 7, 0.5], [7004, 1, 4, 0.56], [149, 2, 4, 0.37], [13259, 29, 4, 1.13], [418, 2, 4, 0.54], [957, 2, 4, 0.57], [7705, 2, 4, 1.15], [12229, 2, 4, 0.52], [7706, 2, 4, 1.15], [11687, 2, 4, 0.56], [10406, 10, 7, 1.21], [410, 1, 4, 0.71], [3478, 2, 4, 0.57], [7036, 1, 4, 0.43], [9784, 1, 4, 0.91], [20255, 2, 4, 0.4], [8938, 2, 4, 0.58], [21713, 3, 7, 0.46], [12870, 1, 4, 2.33], [10408, 10, 6, 1.04], [5490, 2, 4, 0.49], [11402, 1, 4, 0.46], [11404, 2, 4, 0.45], [10410, 10, 6, 1.18], [11161, 1, 5, 1.8], [956, 2, 4, 0.53], [2438, 2, 5, 1.38], [2703, 3, 4, 2.2], [1886, 2, 4, 0.35], [19687, 1, 4, 1.21], [11490, 1, 4, 0.43], [107, 7, 5, 1.24], [21781, 2, 4, 0.47], [22125, 2, 4, 0.36], [11690, 2, 4, 0.36], [2778, 2, 140, 2.81], [6935, 2, 252, 6.0], [6936, 2, 252, 5.81], [305, 2, 132, 3.08], [8672, 2, 259, 3.33], [615, 2, 96, 3.4], [1504, 2, 183, 2.95], [2775, 2, 140, 3.13], [145, 2, 135, 2.84], [2776, 2, 140, 4.5], [8853, 2, 252, 5.13], [2327, 2, 135, 3.26], [12721, 2, 284, 3.49], [130, 1, 53, 2.98], [143, 2, 133, 3.04], [146, 2, 135, 3.13], [2328, 2, 135, 3.53], [11681, 2, 248, 5.48], [11737, 2, 56, 3.11], [616, 2, 107, 3.95], [5491, 2, 109, 2.82], [141, 2, 155, 4.16], [362, 2, 128, 2.96], [144, 2, 135, 2.91], [2497, 2, 183, 3.25], [205, 2, 109, 2.64], [8650, 2, 202, 4.44], [5493, 2, 98, 2.97], [417, 2, 139, 3.15], [8676, 2, 259, 2.97], [8673, 2, 260, 5.05], [3670, 2, 235, 5.79], [2774, 2, 183, 6.0], [8648, 2, 225, 5.29], [589, 2, 137, 2.91], [3, 2, 108, 3.09], [206, 2, 98, 2.64], [6097, 80, 61, 5.49], [2423, 29, 37, 4.87], [22247, 2, 255, 3.05], [11836, 2, 269, 2.69], [6497, 1, 27, 2.94], [8674, 2, 259, 3.57], [624, 2, 107, 4.11], [12343, 1, 610, 4.37], [2055, 3, 158, 4.31], [2423, 80, 185, 4.81], [523, 2, 155, 3.04], [12344, 1, 610, 3.38], [593, 2, 207, 2.86], [6097, 29, 30, 5.49], [6098, 80, 66, 3.97], [12720, 2, 284, 3.48], [12345, 1, 610, 4.37], [11739, 2, 56, 3.11], [75, 2, 144, 3.94], [8915, 2, 129, 2.36], [88, 10, 504, 3.62], [326, 2, 30, 3.9], [6494, 1, 52, 2.64], [60, 3, 730, 4.08], [13260, 29, 65, 2.76], [142, 2, 155, 4.16], [3429, 15, 53, 2.63], [1492, 1, 37, 2.92], [411, 2, 109, 2.83], [21712, 3, 2180, 2.89]]</t>
+  </si>
+  <si>
+    <t>[[141, 2, 4, 0.66], [2328, 2, 4, 0.28], [8650, 2, 5, 0.39], [362, 2, 4, 0.2], [5491, 2, 4, 0.6], [5493, 2, 4, 0.2], [130, 1, 5, 0.48], [589, 2, 4, 0.44], [2327, 2, 4, 0.2], [326, 2, 4, 0.97], [11685, 2, 4, 1.41], [8672, 2, 5, 0.58], [417, 2, 4, 0.56], [6935, 2, 8, 1.3], [205, 2, 4, 0.37], [11681, 2, 5, 1.41], [206, 2, 4, 0.2], [8648, 2, 4, 1.7], [6936, 2, 5, 1.32], [142, 2, 4, 0.2], [8915, 2, 5, 0.2], [11837, 2, 4, 0.55], [12721, 2, 5, 0.97], [11838, 2, 4, 0.2], [2049, 3, 9, 0.47], [1446, 2, 4, 0.78], [523, 2, 4, 0.56], [615, 2, 4, 1.55], [8676, 2, 4, 0.49], [11737, 2, 4, 1.04], [305, 2, 5, 0.53], [616, 2, 4, 1.29], [413, 1, 5, 0.51], [412, 1, 4, 1.0], [411, 2, 4, 0.52], [11739, 2, 4, 1.04], [10574, 3, 5, 1.26], [11835, 2, 4, 0.55], [145, 2, 5, 0.4], [8675, 2, 4, 0.6], [2775, 2, 4, 0.42], [1429, 2, 4, 0.48], [76, 2, 4, 1.11], [8673, 2, 4, 1.45], [143, 2, 4, 0.65], [8674, 2, 4, 0.49], [11836, 2, 4, 0.2], [6158, 2, 5, 1.33], [8938, 2, 4, 0.97], [146, 2, 4, 0.62], [151, 1, 4, 0.75], [12720, 2, 4, 0.82], [2776, 2, 4, 0.75], [10149, 3, 13, 0.39], [3495, 3, 13, 0.85], [2055, 3, 4, 1.18], [75, 2, 4, 1.17], [2057, 3, 4, 1.0], [11738, 2, 4, 1.04], [144, 2, 4, 0.52], [8939, 2, 4, 0.94], [416, 1, 4, 0.73], [7885, 4, 5, 0.44], [22316, 3, 5, 0.19], [88, 10, 8, 0.95], [159, 3, 5, 0.72], [2859, 15, 4, 0.44], [7084, 3, 4, 0.94], [418, 2, 4, 0.2], [10993, 2, 4, 0.49], [20252, 2, 4, 0.37], [9784, 1, 4, 0.88], [7705, 2, 4, 1.15], [5165, 1, 4, 1.11], [410, 1, 4, 0.47], [12526, 2, 4, 0.73], [11844, 2, 4, 0.47], [414, 1, 4, 0.73], [2423, 80, 5, 1.25], [12351, 1, 5, 0.61], [2424, 29, 5, 0.55], [378, 2, 4, 1.16], [2423, 29, 4, 1.16], [12345, 1, 4, 0.61], [60, 3, 5, 2.26], [950, 1, 4, 0.39], [6494, 1, 4, 0.46], [11490, 1, 4, 0.48], [2424, 80, 4, 0.43], [12373, 1, 5, 0.45], [13023, 3, 6, 1.51], [201, 3, 4, 1.1], [13034, 3, 5, 1.37], [1519, 3, 9, 0.4], [11489, 1, 4, 0.37], [5208, 3, 5, 0.54], [345, 3, 4, 0.76], [11770, 1, 4, 0.48], [3, 2, 4, 3.1], [159, 1, 4, 0.73], [6952, 1, 4, 1.09], [3430, 15, 4, 1.23], [20927, 1, 4, 0.48], [11954, 1, 4, 0.42], [7886, 4, 5, 0.44], [432, 3, 4, 2.04], [3429, 15, 4, 0.46], [11504, 2, 4, 0.2], [566, 2, 4, 0.5], [13928, 1, 4, 0.45], [11811, 1, 4, 0.38], [5584, 3, 4, 1.36], [114, 3, 4, 1.64], [2331, 1, 4, 0.79], [10407, 10, 6, 1.27], [1492, 1, 4, 0.62], [105, 3, 4, 1.64], [7004, 1, 4, 0.99], [1490, 1, 4, 1.38], [11089, 1, 4, 0.39], [2703, 3, 4, 2.2], [6098, 80, 4, 1.16], [8274, 3, 4, 2.3], [11674, 1, 4, 0.36], [1886, 2, 4, 0.44], [12348, 1, 4, 0.61], [10410, 10, 6, 1.18], [94, 4, 4, 1.77], [3891, 1, 4, 2.39], [11953, 1, 4, 0.46], [6097, 80, 4, 1.86], [22317, 3, 5, 0.52], [9082, 3, 15, 1.25], [141, 2, 156, 3.01], [2328, 2, 135, 3.53], [8650, 2, 201, 4.44], [362, 2, 128, 2.98], [5491, 2, 108, 2.9], [5493, 2, 97, 2.79], [130, 1, 34, 2.98], [589, 2, 137, 2.91], [2327, 2, 135, 3.26], [326, 2, 81, 3.64], [11685, 2, 247, 6.0], [8672, 2, 258, 3.33], [417, 2, 156, 2.82], [6935, 2, 254, 5.82], [205, 2, 109, 2.53], [11681, 2, 247, 5.84], [206, 2, 81, 2.64], [8648, 2, 201, 4.32], [6936, 2, 254, 5.23], [142, 2, 140, 3.03], [11837, 2, 269, 2.79], [12721, 2, 255, 3.19], [11838, 2, 242, 3.09], [2049, 3, 495, 3.27], [1446, 2, 76, 3.25], [523, 2, 156, 2.81], [615, 2, 107, 4.63], [8676, 2, 287, 4.22], [11737, 2, 57, 3.69], [305, 2, 132, 3.08], [616, 2, 107, 4.15], [413, 1, 77, 3.05], [412, 1, 75, 3.02], [411, 2, 109, 2.74], [11739, 2, 57, 3.69], [10574, 3, 450, 4.6], [11835, 2, 269, 2.79], [145, 2, 135, 2.84], [8675, 2, 287, 3.21], [2775, 2, 157, 2.56], [1429, 2, 153, 2.68], [76, 2, 109, 3.83], [8673, 2, 284, 5.17], [143, 2, 148, 2.98], [8674, 2, 287, 3.25], [11836, 2, 242, 2.89], [6158, 2, 260, 4.44], [8938, 2, 190, 3.57], [146, 2, 151, 2.93], [151, 1, 33, 2.81], [12720, 2, 284, 3.48], [2776, 2, 157, 3.16], [10149, 3, 872, 3.26], [3495, 3, 965, 3.31], [2055, 3, 158, 4.31], [75, 2, 144, 3.94], [2057, 3, 158, 4.31], [11738, 2, 57, 3.69], [144, 2, 151, 2.74], [8939, 2, 63, 4.3], [416, 1, 86, 3.13], [7885, 4, 40, 2.38], [22316, 3, 286, 2.96], [88, 10, 561, 4.69], [159, 3, 709, 3.16], [2859, 15, 69, 2.6], [7084, 3, 116, 3.92]]</t>
+  </si>
+  <si>
+    <t>[[326, 2, 4, 1.08], [6935, 2, 8, 0.99], [2049, 3, 8, 0.41], [362, 2, 4, 0.92], [589, 2, 5, 0.37], [75, 2, 4, 0.39], [141, 2, 4, 0.66], [1776, 1, 4, 0.2], [205, 2, 4, 0.38], [8915, 2, 5, 0.4], [2778, 2, 4, 0.2], [8672, 2, 6, 0.51], [6936, 2, 5, 1.05], [593, 2, 5, 0.44], [7886, 4, 4, 0.57], [305, 2, 4, 0.5], [206, 2, 4, 0.2], [151, 1, 5, 0.47], [8648, 2, 4, 1.08], [1777, 1, 4, 0.8], [2328, 2, 5, 0.35], [88, 10, 9, 0.55], [11681, 2, 5, 1.87], [990, 2, 4, 0.26], [8650, 2, 5, 1.09], [412, 1, 4, 0.62], [5151, 2, 4, 0.75], [2050, 3, 4, 0.8], [76, 2, 4, 1.06], [144, 2, 4, 0.49], [345, 3, 5, 0.44], [10149, 3, 17, 1.82], [2991, 3, 4, 1.6], [22247, 2, 4, 0.54], [57, 1, 4, 0.38], [3478, 2, 4, 0.89], [146, 2, 4, 1.0], [7004, 1, 5, 0.36], [45, 2, 4, 0.56], [2054, 3, 4, 0.51], [143, 2, 4, 0.46], [417, 2, 4, 0.45], [413, 1, 4, 0.81], [21793, 1, 5, 0.45], [167, 3, 5, 0.49], [201, 3, 5, 0.2], [74, 1, 4, 1.75], [1446, 2, 4, 0.54], [346, 1, 4, 0.2], [2055, 3, 4, 0.5], [168, 3, 4, 0.32], [10, 2, 4, 0.45], [11234, 2, 4, 0.2], [7084, 3, 4, 0.36], [1429, 2, 4, 0.2], [7036, 1, 4, 1.8], [12721, 2, 6, 0.49], [3495, 3, 13, 0.52], [5081, 2, 4, 0.44], [8649, 2, 4, 1.29], [308, 1, 5, 0.73], [13028, 3, 4, 0.47], [10825, 21, 8, 1.34], [12870, 1, 4, 1.54], [79, 1, 4, 0.38], [1492, 1, 4, 0.58], [96, 11, 14, 0.46], [23, 1, 4, 0.2], [1006, 2, 4, 0.55], [3893, 1, 5, 0.2], [418, 2, 4, 0.43], [1504, 2, 4, 0.2], [145, 2, 4, 0.43], [5208, 3, 6, 0.19], [9827, 3, 4, 0.2], [3891, 1, 4, 0.2], [432, 3, 5, 0.41], [7005, 1, 5, 0.36], [94, 4, 4, 1.24], [1490, 1, 5, 0.2], [8853, 2, 5, 1.01], [13260, 29, 4, 0.4], [5812, 3, 5, 2.01], [416, 1, 4, 0.81], [8651, 2, 4, 0.8], [12353, 1, 4, 1.55], [20256, 2, 4, 0.2], [8939, 2, 5, 0.2], [21269, 3, 4, 0.95], [13280, 1, 4, 0.81], [12349, 1, 4, 1.63], [950, 1, 4, 0.46], [33, 1, 4, 0.53], [5086, 1, 5, 1.08], [998, 2, 5, 0.73], [12350, 1, 4, 0.62], [9069, 1, 4, 0.97], [1243, 2, 4, 0.89], [229, 1, 4, 1.05], [2878, 1, 4, 0.74], [140, 2, 4, 0.63], [2049, 1, 4, 0.2], [7567, 3, 4, 1.11], [20927, 1, 4, 0.2], [126, 2, 4, 0.93], [346, 3, 5, 0.19], [3980, 4, 4, 1.31], [1703, 2, 4, 0.41], [8274, 3, 4, 0.39], [9691, 1, 4, 1.09], [35, 1, 4, 0.48], [5209, 3, 4, 0.19], [1070, 7, 10, 0.2], [997, 2, 4, 1.03], [5584, 3, 4, 1.74], [11811, 1, 4, 1.0], [1519, 3, 10, 0.4], [11914, 1, 5, 0.5], [5660, 2, 5, 0.9], [856, 1, 4, 0.38], [8898, 3, 4, 2.43], [1091, 1, 4, 0.2], [5513, 2, 4, 0.44], [8926, 1, 4, 1.35], [523, 2, 4, 0.63], [11767, 1, 4, 0.48], [2775, 2, 4, 0.2], [9372, 1, 4, 0.39], [9081, 3, 7, 1.8], [13034, 3, 5, 0.66], [20255, 2, 5, 0.2], [307, 2, 4, 1.14], [11808, 1, 5, 0.2], [326, 2, 84, 3.42], [6935, 2, 235, 4.09], [2049, 3, 450, 1.94], [362, 2, 131, 2.84], [589, 2, 142, 1.93], [75, 2, 121, 1.98], [141, 2, 143, 3.4], [1776, 1, 90, 1.74], [205, 2, 101, 1.85], [8915, 2, 179, 1.9], [2778, 2, 130, 2.06], [8672, 2, 235, 2.17], [6936, 2, 235, 4.51], [593, 2, 211, 2.16], [7886, 4, 132, 2.19], [305, 2, 121, 2.18], [206, 2, 90, 1.99], [151, 1, 54, 1.63], [8648, 2, 186, 3.41], [1777, 1, 90, 3.67], [2328, 2, 126, 1.92], [88, 10, 463, 2.3], [11681, 2, 227, 5.43], [990, 2, 43, 2.16], [8650, 2, 186, 3.43], [412, 1, 69, 2.41], [5151, 2, 19, 3.62], [2050, 3, 433, 3.55], [76, 2, 90, 3.12], [144, 2, 139, 2.06], [345, 3, 248, 2.01], [10149, 3, 715, 4.79], [2991, 3, 133, 4.91], [22247, 2, 234, 2.54], [57, 1, 79, 1.85], [3478, 2, 69, 3.31], [146, 2, 125, 2.18], [7004, 1, 65, 1.93], [45, 2, 90, 4.21], [2054, 3, 389, 2.21], [143, 2, 122, 2.11], [417, 2, 143, 3.4], [413, 1, 79, 3.28], [21793, 1, 196, 2.1], [167, 3, 188, 2.16], [201, 3, 248, 1.94], [74, 1, 163, 3.73], [1446, 2, 126, 3.18], [346, 1, 131, 2.05], [2055, 3, 389, 2.18], [168, 3, 339, 2.77], [10, 2, 97, 2.76], [11234, 2, 153, 2.04], [7084, 3, 107, 1.93], [1429, 2, 126, 2.47], [7036, 1, 105, 3.84], [12721, 2, 234, 2.13], [3495, 3, 797, 2.2], [5081, 2, 177, 1.96], [8649, 2, 186, 3.64], [308, 1, 139, 3.98], [13028, 3, 122, 2.14], [10825, 21, 575, 3.62], [12870, 1, 113, 3.19], [79, 1, 44, 1.85], [1492, 1, 30, 3.25], [96, 11, 784, 1.97]]</t>
+  </si>
+  <si>
+    <t>[[88, 10, 10, 0.93], [2327, 2, 4, 0.52], [8915, 2, 5, 1.08], [589, 2, 5, 0.2], [2778, 2, 4, 0.2], [6935, 2, 6, 1.77], [2328, 2, 4, 0.58], [5493, 2, 4, 1.23], [130, 1, 4, 0.98], [305, 2, 4, 0.45], [615, 2, 4, 0.2], [616, 2, 5, 0.2], [6936, 2, 5, 1.74], [326, 2, 5, 1.15], [8650, 2, 4, 0.39], [8648, 2, 4, 1.05], [1446, 2, 4, 0.2], [2049, 3, 5, 0.42], [10, 2, 4, 0.2], [143, 2, 5, 0.58], [159, 3, 5, 0.67], [593, 2, 4, 0.37], [205, 2, 4, 0.43], [5491, 2, 4, 0.58], [2775, 2, 4, 0.2], [7036, 1, 4, 0.94], [144, 2, 5, 0.53], [3840, 1, 5, 0.29], [151, 1, 4, 0.75], [94, 4, 4, 1.91], [434, 2, 5, 0.2], [8938, 2, 4, 0.52], [990, 2, 4, 0.2], [3893, 1, 4, 0.2], [146, 2, 4, 1.07], [8853, 2, 4, 1.79], [1504, 2, 4, 0.93], [12224, 1, 4, 0.46], [624, 2, 4, 1.1], [1429, 2, 4, 0.2], [3891, 1, 4, 0.2], [2776, 2, 4, 0.2], [206, 2, 4, 0.37], [2055, 3, 4, 0.46], [362, 2, 4, 0.5], [141, 2, 4, 0.39], [2057, 3, 4, 0.46], [75, 2, 4, 0.39], [11681, 2, 5, 1.33], [11404, 2, 4, 0.2], [5208, 3, 5, 0.19], [8649, 2, 4, 1.53], [3889, 1, 4, 0.35], [1007, 2, 4, 0.46], [10574, 3, 5, 1.86], [11234, 2, 4, 0.75], [10993, 2, 4, 0.7], [7886, 4, 4, 0.46], [12870, 1, 5, 0.72], [21793, 1, 4, 0.5], [10149, 3, 15, 0.39], [3980, 4, 4, 0.73], [2050, 3, 4, 0.46], [12353, 1, 4, 0.66], [145, 2, 4, 1.01], [7084, 3, 4, 0.86], [11811, 1, 4, 0.2], [8672, 2, 4, 1.48], [20927, 1, 4, 0.95], [998, 2, 4, 1.0], [9760, 29, 4, 0.37], [997, 2, 4, 1.42], [2436, 4, 4, 0.2], [1006, 2, 5, 0.54], [1886, 2, 4, 0.2], [972, 3, 5, 0.51], [2424, 80, 4, 0.99], [3, 2, 4, 0.62], [346, 3, 5, 0.19], [229, 1, 4, 0.47], [6158, 2, 5, 0.48], [3495, 3, 11, 0.56], [12346, 1, 4, 0.66], [5076, 1, 4, 0.71], [7887, 4, 4, 0.47], [12345, 1, 4, 0.66], [20252, 2, 4, 0.38], [126, 2, 4, 1.27], [11953, 1, 4, 0.46], [74, 1, 4, 1.97], [9372, 1, 4, 1.42], [11770, 1, 4, 0.88], [140, 2, 4, 1.27], [12344, 1, 4, 0.66], [8939, 2, 4, 0.2], [11954, 1, 4, 0.38], [11685, 2, 5, 1.33], [1492, 1, 4, 0.2], [12352, 1, 4, 0.66], [996, 2, 4, 1.16], [12721, 2, 4, 2.31], [2774, 2, 4, 0.63], [20256, 2, 4, 0.2], [12350, 1, 4, 0.66], [3981, 3, 11, 0.23], [9081, 3, 7, 0.48], [9491, 21, 12, 0.22], [5434, 1, 4, 1.0], [2423, 80, 4, 0.75], [6497, 1, 4, 0.63], [12343, 1, 4, 0.66], [12229, 2, 4, 0.47], [5584, 3, 4, 1.75], [2438, 2, 6, 0.49], [10388, 2, 4, 0.37], [12351, 1, 4, 0.66], [10407, 10, 7, 1.55], [11179, 1, 4, 0.45], [6496, 1, 4, 1.89], [22317, 3, 4, 0.6], [7573, 1, 8, 2.02], [823, 1, 4, 0.55], [5209, 3, 5, 0.19], [3900, 3, 4, 1.76], [2805, 137, 4, 0.89], [8898, 3, 5, 1.44], [12526, 2, 4, 0.71], [11812, 1, 4, 0.2], [2424, 29, 4, 0.55], [3975, 4, 5, 1.21], [4253, 1, 4, 0.54], [11490, 1, 4, 0.35], [336, 15, 4, 0.97], [88, 10, 490, 3.94], [2327, 2, 132, 2.93], [8915, 2, 165, 2.96], [589, 2, 134, 2.97], [2778, 2, 137, 2.92], [6935, 2, 244, 6.0], [2328, 2, 132, 3.05], [5493, 2, 104, 3.91], [305, 2, 128, 2.8], [615, 2, 93, 3.01], [616, 2, 93, 2.64], [6936, 2, 244, 5.39], [326, 2, 77, 4.1], [8650, 2, 196, 3.45], [8648, 2, 196, 3.91], [1446, 2, 134, 3.2], [2049, 3, 360, 2.34], [10, 2, 91, 2.65], [143, 2, 130, 3.03], [159, 3, 690, 2.82], [593, 2, 223, 2.53], [205, 2, 95, 2.77], [5491, 2, 93, 3.05], [2775, 2, 137, 2.92], [7036, 1, 113, 4.28], [3840, 1, 150, 3.43], [151, 1, 32, 2.69], [94, 4, 105, 4.77], [434, 2, 93, 2.69], [8938, 2, 125, 2.43], [990, 2, 19, 2.69], [3893, 1, 109, 2.96], [146, 2, 132, 3.02], [8853, 2, 272, 5.15], [1504, 2, 180, 3.69], [12224, 1, 162, 2.49], [624, 2, 104, 3.83], [1429, 2, 134, 2.89], [3891, 1, 109, 2.96], [2776, 2, 137, 3.16], [206, 2, 106, 2.39], [2055, 3, 314, 2.32], [362, 2, 124, 2.89], [141, 2, 136, 2.69], [2057, 3, 314, 2.32], [75, 2, 126, 2.69], [11681, 2, 234, 5.43], [11404, 2, 92, 3.15], [5208, 3, 493, 2.87], [8649, 2, 218, 4.79], [3889, 1, 122, 2.29], [1007, 2, 264, 2.49], [11234, 2, 161, 3.27], [10993, 2, 54, 2.93], [7886, 4, 70, 2.16], [12870, 1, 121, 3.3], [21793, 1, 208, 2.89], [10149, 3, 763, 3.88], [3980, 4, 365, 4.41], [2050, 3, 314, 2.32], [12353, 1, 612, 2.87], [145, 2, 132, 2.92], [7084, 3, 127, 3.22], [11811, 1, 402, 2.78], [8672, 2, 247, 4.92], [20927, 1, 34, 2.64], [998, 2, 208, 4.81]]</t>
+  </si>
+  <si>
+    <t>[[6935, 2, 8, 1.31], [141, 2, 4, 0.4], [589, 2, 5, 0.2], [2778, 2, 4, 0.2], [6936, 2, 5, 0.71], [8648, 2, 4, 1.13], [362, 2, 4, 0.46], [2327, 2, 4, 0.39], [11681, 2, 9, 1.29], [8650, 2, 5, 0.84], [326, 2, 4, 0.77], [205, 2, 4, 0.2], [2328, 2, 4, 0.57], [1446, 2, 4, 0.28], [305, 2, 5, 0.88], [130, 1, 4, 0.2], [8649, 2, 5, 0.39], [2775, 2, 4, 0.2], [8853, 2, 5, 1.21], [361, 2, 4, 0.5], [2776, 2, 4, 0.2], [593, 2, 5, 0.48], [143, 2, 4, 1.13], [140, 2, 4, 0.77], [1429, 2, 4, 0.28], [206, 2, 4, 0.2], [5493, 2, 4, 0.2], [523, 2, 4, 0.4], [7004, 1, 4, 0.71], [413, 1, 4, 1.02], [7036, 1, 4, 1.58], [5491, 2, 4, 0.5], [412, 1, 4, 0.57], [21793, 1, 4, 1.03], [12350, 1, 4, 0.19], [151, 1, 4, 0.46], [1124, 2, 4, 0.64], [990, 2, 4, 0.2], [12353, 1, 5, 0.19], [5165, 1, 4, 0.42], [8915, 2, 5, 0.86], [615, 2, 4, 1.1], [583, 2, 4, 0.77], [417, 2, 4, 0.43], [21798, 1, 4, 0.36], [146, 2, 4, 0.64], [248, 1, 4, 0.2], [434, 2, 5, 0.2], [201, 3, 5, 0.47], [142, 2, 4, 0.48], [6097, 80, 4, 0.38], [11770, 1, 4, 0.43], [6952, 1, 4, 1.71], [2055, 3, 4, 0.81], [345, 3, 4, 0.47], [3891, 1, 4, 0.98], [9372, 1, 4, 0.58], [2057, 3, 4, 0.81], [616, 2, 4, 0.86], [7084, 3, 4, 1.0], [3670, 2, 4, 1.47], [3893, 1, 4, 0.64], [5165, 2, 7, 1.41], [12346, 1, 5, 0.19], [12870, 1, 4, 1.18], [12343, 1, 4, 0.49], [10574, 3, 5, 1.39], [1886, 2, 4, 0.36], [2424, 80, 4, 0.43], [346, 3, 4, 0.2], [3334, 5, 5, 1.7], [20927, 1, 4, 0.38], [12351, 1, 4, 0.38], [7885, 4, 4, 0.49], [6098, 80, 4, 1.46], [6097, 29, 4, 0.88], [11089, 1, 4, 0.44], [12345, 1, 4, 0.47], [10149, 3, 13, 0.91], [20256, 2, 4, 0.2], [147, 1, 4, 0.53], [22316, 3, 4, 0.36], [1492, 1, 4, 0.58], [11953, 1, 4, 0.44], [432, 3, 5, 0.62], [11491, 2, 4, 0.51], [20252, 2, 4, 0.2], [4032, 29, 4, 0.47], [418, 2, 4, 0.72], [1490, 1, 4, 0.42], [1519, 3, 10, 0.4], [2423, 80, 4, 1.66], [11952, 1, 4, 0.46], [411, 2, 4, 0.5], [12304, 1, 4, 0.2], [5151, 2, 4, 0.62], [229, 1, 4, 2.07], [11769, 1, 4, 0.48], [3576, 25, 4, 0.91], [972, 3, 5, 0.46], [2331, 1, 4, 1.19], [346, 1, 4, 0.2], [995, 2, 4, 0.41], [416, 1, 4, 0.99], [13034, 3, 4, 1.31], [2424, 29, 4, 0.41], [11426, 25, 4, 0.58], [3, 2, 4, 0.55], [11737, 2, 4, 0.5], [5076, 1, 4, 0.63], [11767, 1, 4, 0.48], [439, 1, 4, 1.47], [11490, 1, 4, 0.56], [2805, 137, 4, 0.98], [2160, 68, 4, 0.56], [6494, 1, 4, 1.59], [950, 1, 4, 0.36], [414, 1, 4, 0.66], [3575, 25, 4, 0.98], [12764, 2, 5, 0.51], [1701, 2, 4, 1.97], [11180, 1, 4, 0.54], [8677, 3, 5, 1.11], [75, 2, 4, 0.37], [11586, 1, 7, 1.42], [3577, 25, 4, 0.42], [3478, 2, 4, 0.9], [11585, 29, 4, 1.12], [11813, 1, 4, 1.11], [13023, 3, 5, 1.01], [9998, 80, 4, 0.81], [2438, 2, 5, 1.05], [12526, 2, 4, 0.48], [6935, 2, 212, 5.03], [141, 2, 119, 2.71], [589, 2, 118, 2.6], [2778, 2, 119, 2.86], [6936, 2, 212, 5.43], [8648, 2, 171, 3.75], [362, 2, 108, 2.52], [2327, 2, 129, 3.24], [11681, 2, 208, 4.91], [8650, 2, 171, 3.23], [326, 2, 78, 2.83], [205, 2, 84, 2.22], [2328, 2, 116, 2.74], [1446, 2, 118, 3.11], [305, 2, 113, 3.31], [130, 1, 45, 1.55], [8649, 2, 171, 3.7], [2775, 2, 119, 2.86], [8853, 2, 212, 4.93], [361, 2, 119, 2.6], [2776, 2, 119, 2.86], [593, 2, 177, 2.55], [143, 2, 114, 3.07], [140, 2, 78, 2.83], [1429, 2, 118, 3.41], [206, 2, 84, 2.51], [5493, 2, 83, 2.55], [523, 2, 119, 2.68], [7004, 1, 68, 2.72], [413, 1, 66, 2.92], [7036, 1, 99, 3.67], [5491, 2, 93, 2.34], [412, 1, 72, 2.66], [21793, 1, 208, 5.07], [12350, 1, 482, 2.38], [151, 1, 57, 2.33], [1124, 2, 161, 2.69], [990, 2, 40, 2.5], [12353, 1, 482, 2.43], [5165, 1, 26, 3.83], [8915, 2, 163, 2.9], [615, 2, 92, 3.67], [583, 2, 78, 2.83], [417, 2, 119, 2.48], [21798, 1, 120, 2.36], [146, 2, 129, 4.34], [248, 1, 42, 2.08], [434, 2, 82, 2.58], [201, 3, 231, 2.55], [142, 2, 119, 2.56], [6097, 80, 54, 5.58], [11770, 1, 189, 2.22], [6952, 1, 145, 4.06], [2055, 3, 410, 2.91], [345, 3, 231, 2.55], [3891, 1, 107, 3.22], [9372, 1, 195, 2.96], [2057, 3, 410, 2.91], [616, 2, 92, 3.0], [7084, 3, 99, 3.51], [3670, 2, 212, 4.13], [3893, 1, 107, 3.22], [12346, 1, 482, 2.38], [12870, 1, 119, 3.63], [12343, 1, 536, 2.32], [10574, 3, 392, 3.24], [1886, 2, 135, 2.08]]</t>
+  </si>
+  <si>
+    <t>[[6935, 2, 5, 1.18], [615, 2, 4, 1.69], [2778, 2, 5, 0.2], [305, 2, 4, 0.48], [5493, 2, 4, 1.52], [6936, 2, 4, 1.18], [130, 1, 4, 0.97], [205, 2, 4, 0.53], [616, 2, 4, 1.5], [1504, 2, 5, 0.57], [144, 2, 4, 0.53], [8648, 2, 4, 0.7], [2049, 3, 9, 0.41], [88, 10, 8, 0.37], [8915, 2, 5, 1.45], [326, 2, 4, 1.12], [7036, 1, 4, 1.57], [8650, 2, 5, 0.57], [593, 2, 5, 0.45], [2327, 2, 5, 0.47], [11681, 2, 4, 1.35], [8853, 2, 4, 1.18], [141, 2, 4, 0.48], [2775, 2, 5, 0.2], [206, 2, 4, 0.2], [151, 1, 4, 0.59], [7004, 1, 5, 0.35], [248, 1, 4, 0.43], [11685, 2, 4, 1.88], [3840, 1, 4, 0.39], [3891, 1, 5, 0.2], [2328, 2, 4, 0.5], [2050, 3, 5, 0.34], [5491, 2, 4, 0.54], [2497, 2, 4, 0.83], [2055, 3, 4, 1.75], [143, 2, 4, 0.58], [434, 2, 4, 0.47], [3980, 4, 4, 1.2], [990, 2, 4, 0.2], [2054, 3, 4, 0.34], [624, 2, 4, 1.35], [8649, 2, 4, 1.53], [362, 2, 4, 0.85], [2776, 2, 4, 0.67], [12870, 1, 4, 0.92], [2057, 3, 5, 0.34], [12350, 1, 4, 0.66], [7886, 4, 5, 0.45], [10574, 3, 5, 1.86], [5165, 1, 4, 0.58], [1006, 2, 4, 0.58], [1446, 2, 4, 0.39], [3495, 3, 13, 0.85], [94, 4, 4, 0.84], [75, 2, 4, 1.49], [523, 2, 4, 1.0], [7084, 3, 4, 0.58], [2991, 3, 4, 1.1], [7005, 1, 4, 0.94], [10149, 3, 13, 0.39], [3975, 4, 4, 1.26], [21793, 1, 4, 2.3], [9760, 29, 4, 0.2], [11404, 2, 5, 0.2], [142, 2, 4, 0.51], [12346, 1, 4, 0.66], [6158, 2, 5, 0.2], [20927, 1, 4, 0.67], [3981, 3, 15, 1.15], [5165, 2, 5, 1.11], [417, 2, 4, 0.54], [2912, 1, 4, 0.2], [3982, 3, 11, 1.18], [8939, 2, 4, 0.2], [1007, 2, 4, 0.51], [11953, 1, 4, 0.45], [2774, 2, 4, 1.06], [33, 1, 4, 1.06], [956, 2, 4, 0.47], [11772, 1, 5, 1.35], [286, 3, 5, 1.06], [1492, 1, 4, 0.7], [11767, 1, 4, 0.2], [336, 15, 4, 1.12], [972, 3, 4, 1.07], [11769, 1, 4, 0.2], [11490, 1, 4, 1.04], [11770, 1, 4, 0.48], [410, 1, 5, 0.54], [74, 1, 4, 1.16], [2912, 2, 5, 0.47], [389, 4, 5, 0.38], [6496, 1, 4, 0.47], [35, 1, 4, 0.57], [7567, 3, 5, 1.15], [411, 2, 4, 1.0], [12721, 2, 4, 0.99], [1413, 15, 4, 0.2], [4253, 1, 4, 0.82], [22317, 3, 4, 0.51], [140, 2, 4, 0.93], [8673, 2, 4, 0.47], [8121, 3, 5, 0.2], [1126, 2, 4, 0.58], [4176, 4, 4, 1.31], [2436, 4, 4, 0.2], [9372, 1, 4, 1.7], [21269, 3, 4, 2.24], [8676, 2, 4, 1.7], [8677, 3, 5, 0.4], [22247, 2, 4, 1.38], [10388, 2, 4, 1.08], [10936, 2, 4, 1.7], [12343, 1, 4, 0.66], [11085, 2, 5, 1.27], [12526, 2, 4, 1.08], [9784, 1, 4, 0.47], [1274, 1, 4, 0.23], [6494, 1, 5, 0.29], [12269, 2, 4, 1.03], [37, 1, 4, 0.66], [13023, 3, 4, 1.26], [1429, 2, 4, 0.5], [345, 3, 4, 1.31], [7573, 1, 5, 1.35], [12225, 1, 4, 0.69], [12271, 2, 4, 1.01], [3, 2, 4, 0.38], [96, 11, 12, 0.38], [3577, 25, 4, 0.48], [9, 1, 4, 0.36], [10408, 10, 5, 1.37], [6935, 2, 214, 5.9], [615, 2, 91, 4.78], [2778, 2, 121, 2.77], [305, 2, 113, 2.58], [5493, 2, 91, 4.44], [6936, 2, 214, 5.92], [130, 1, 27, 2.58], [205, 2, 84, 2.69], [616, 2, 91, 4.41], [1504, 2, 156, 2.75], [144, 2, 117, 4.4], [8648, 2, 174, 2.99], [2049, 3, 421, 2.25], [88, 10, 450, 3.45], [8915, 2, 65, 4.29], [326, 2, 70, 3.57], [7036, 1, 99, 3.83], [8650, 2, 174, 2.75], [593, 2, 177, 2.78], [2327, 2, 117, 2.57], [11681, 2, 212, 5.01], [8853, 2, 214, 5.93], [141, 2, 119, 2.6], [2775, 2, 121, 2.77], [206, 2, 84, 2.55], [151, 1, 58, 2.7], [7004, 1, 61, 2.36], [248, 1, 47, 2.25], [11685, 2, 212, 5.4], [3840, 1, 150, 2.17], [3891, 1, 97, 2.88], [2328, 2, 117, 2.62], [2050, 3, 356, 2.34], [5491, 2, 91, 3.06], [2497, 2, 174, 4.13], [2055, 3, 396, 4.89], [143, 2, 115, 2.77], [434, 2, 56, 2.07], [3980, 4, 374, 4.07], [990, 2, 40, 2.77], [2054, 3, 356, 2.34], [624, 2, 91, 5.38], [8649, 2, 194, 4.25], [362, 2, 109, 3.27], [2776, 2, 121, 3.86], [12870, 1, 117, 5.16], [2057, 3, 356, 2.34], [12350, 1, 543, 2.67], [7886, 4, 43, 2.23], [10574, 3, 393, 4.07], [5165, 1, 26, 3.74], [1006, 2, 197, 2.83], [1446, 2, 117, 2.62], [3495, 3, 832, 2.92], [94, 4, 93, 5.25], [75, 2, 112, 3.52], [523, 2, 119, 2.64], [7084, 3, 58, 2.79], [2991, 3, 125, 5.99], [7005, 1, 68, 3.18], [10149, 3, 752, 2.93], [3975, 4, 374, 4.2], [21793, 1, 174, 5.26], [9760, 29, 55, 2.5], [11404, 2, 46, 2.88], [142, 2, 133, 2.39], [12346, 1, 543, 2.67]]</t>
+  </si>
+  <si>
+    <t>[[6935, 2, 7, 1.38], [305, 2, 4, 0.53], [2328, 2, 4, 0.78], [130, 1, 4, 0.2], [141, 2, 5, 0.2], [2778, 2, 5, 0.47], [8650, 2, 4, 0.67], [5491, 2, 4, 0.63], [2327, 2, 4, 0.63], [8672, 2, 5, 0.58], [6936, 2, 4, 1.4], [143, 2, 4, 1.14], [11681, 2, 5, 1.41], [248, 1, 4, 0.46], [145, 2, 4, 0.4], [205, 2, 4, 0.56], [5493, 2, 4, 1.24], [146, 2, 4, 0.56], [417, 2, 4, 0.52], [589, 2, 4, 0.2], [75, 2, 4, 0.37], [11737, 2, 4, 0.38], [11838, 2, 4, 0.57], [1124, 2, 6, 0.2], [523, 2, 5, 0.2], [8648, 2, 4, 1.54], [8853, 2, 4, 1.38], [12721, 2, 6, 0.47], [615, 2, 4, 1.28], [1005, 2, 5, 0.2], [326, 2, 5, 0.47], [206, 2, 5, 0.2], [8915, 2, 4, 0.2], [8673, 2, 5, 0.74], [144, 2, 5, 0.44], [11739, 2, 4, 0.38], [88, 10, 9, 0.82], [434, 2, 4, 0.73], [2776, 2, 4, 0.41], [142, 2, 4, 0.2], [151, 1, 4, 0.75], [8676, 2, 4, 0.47], [6158, 2, 5, 0.2], [2424, 29, 4, 0.2], [8649, 2, 4, 1.19], [2423, 29, 4, 1.81], [11738, 2, 4, 0.38], [2497, 2, 4, 0.55], [7704, 2, 4, 1.08], [2424, 80, 4, 0.49], [1413, 15, 4, 0.77], [10574, 3, 6, 1.26], [2423, 80, 4, 1.75], [3670, 2, 4, 1.96], [11836, 2, 4, 0.2], [7705, 2, 4, 1.08], [2054, 3, 4, 0.4], [3, 2, 4, 0.43], [2859, 15, 4, 1.25], [412, 1, 4, 0.58], [378, 2, 4, 2.48], [7706, 2, 4, 1.08], [12720, 2, 4, 0.98], [22316, 3, 4, 0.46], [2055, 3, 4, 0.47], [12344, 1, 4, 0.48], [10149, 3, 13, 1.12], [3478, 2, 4, 1.07], [74, 1, 5, 1.47], [3429, 15, 4, 0.46], [307, 2, 4, 1.5], [2774, 2, 4, 0.55], [6497, 1, 4, 0.44], [60, 3, 5, 0.41], [12526, 2, 4, 1.43], [7004, 1, 4, 1.02], [418, 2, 4, 0.81], [13928, 1, 4, 0.2], [411, 2, 4, 0.5], [11089, 1, 4, 0.39], [2057, 3, 4, 0.4], [413, 1, 4, 0.54], [11844, 2, 5, 0.2], [14037, 3, 4, 0.96], [7036, 1, 4, 0.43], [20252, 2, 4, 0.58], [2050, 3, 4, 0.4], [3893, 1, 5, 0.44], [13260, 29, 4, 0.67], [8274, 3, 4, 0.88], [6097, 80, 4, 0.64], [6952, 1, 4, 1.09], [3891, 1, 4, 2.08], [94, 4, 5, 1.09], [159, 3, 5, 0.72], [9784, 1, 4, 0.55], [1050, 2, 4, 0.36], [6494, 1, 4, 0.46], [7707, 2, 4, 0.72], [1490, 1, 4, 1.02], [11490, 1, 4, 0.47], [1413, 16, 4, 0.39], [414, 1, 4, 0.66], [7708, 2, 4, 1.15], [1243, 2, 5, 0.2], [3889, 1, 5, 0.37], [1492, 1, 4, 0.62], [565, 2, 4, 0.46], [5208, 3, 5, 0.97], [22317, 3, 5, 0.52], [7703, 2, 4, 1.15], [11491, 2, 4, 0.81], [21793, 1, 4, 0.95], [3495, 3, 13, 0.85], [229, 1, 4, 2.0], [345, 3, 4, 1.26], [410, 1, 4, 0.4], [2422, 80, 4, 1.75], [11504, 2, 4, 0.72], [6098, 80, 4, 1.14], [149, 2, 4, 0.52], [947, 15, 4, 0.39], [6630, 3, 4, 1.31], [3430, 15, 4, 1.23], [147, 1, 4, 0.52], [3674, 2, 4, 0.52], [416, 1, 4, 1.59], [2805, 137, 6, 1.85], [2331, 1, 4, 0.73], [247, 1, 4, 1.18], [9126, 1, 4, 0.47], [6098, 29, 4, 1.19], [8635, 3, 4, 0.89], [6935, 2, 253, 6.0], [305, 2, 132, 3.08], [2328, 2, 135, 3.53], [130, 1, 53, 2.48], [141, 2, 140, 2.84], [2778, 2, 156, 3.07], [8650, 2, 201, 4.37], [5491, 2, 106, 4.31], [2327, 2, 135, 3.26], [8672, 2, 258, 3.33], [6936, 2, 253, 5.42], [11681, 2, 276, 5.75], [248, 1, 37, 2.46], [145, 2, 135, 2.84], [205, 2, 109, 2.81], [5493, 2, 106, 4.23], [146, 2, 135, 3.13], [417, 2, 140, 3.05], [589, 2, 59, 2.91], [75, 2, 145, 3.42], [11737, 2, 57, 2.97], [11838, 2, 269, 2.83], [1124, 2, 168, 2.98], [523, 2, 140, 3.36], [8648, 2, 201, 4.01], [8853, 2, 253, 4.82], [12721, 2, 255, 3.19], [615, 2, 108, 4.14], [326, 2, 81, 3.64], [206, 2, 41, 2.64], [8915, 2, 171, 2.87], [8673, 2, 260, 5.05], [144, 2, 135, 2.91], [11739, 2, 57, 2.97], [88, 10, 504, 3.62], [434, 2, 107, 3.23], [2776, 2, 140, 3.77], [142, 2, 140, 3.16], [151, 1, 33, 2.81], [8676, 2, 258, 2.97], [6158, 2, 235, 2.82], [2424, 29, 24, 2.67], [8649, 2, 201, 3.38], [2423, 29, 32, 4.52], [11738, 2, 57, 2.97], [2497, 2, 184, 3.11], [7704, 2, 158, 3.18], [2424, 80, 153, 3.11], [10574, 3, 450, 4.6], [2423, 80, 162, 4.41], [3670, 2, 212, 5.55], [11836, 2, 242, 2.89], [7705, 2, 158, 3.18], [2054, 3, 473, 3.89], [3, 2, 108, 2.9], [2859, 15, 62, 3.48], [412, 1, 74, 3.17], [378, 2, 224, 6.0], [7706, 2, 158, 3.18], [12720, 2, 255, 2.99], [22316, 3, 318, 2.64], [2055, 3, 425, 2.76], [12344, 1, 620, 2.67], [10149, 3, 866, 4.0], [3478, 2, 43, 4.08], [74, 1, 180, 5.0], [3429, 15, 53, 2.63]]</t>
+  </si>
+  <si>
+    <t>[[8672, 2, 6, 0.26], [305, 2, 4, 0.56], [3, 2, 4, 0.53], [6935, 2, 8, 1.37], [205, 2, 4, 0.47], [143, 2, 4, 0.43], [144, 2, 4, 0.26], [75, 2, 5, 0.49], [12721, 2, 6, 0.56], [145, 2, 4, 0.26], [8915, 2, 6, 0.2], [2778, 2, 4, 0.2], [1776, 1, 4, 0.45], [146, 2, 4, 0.26], [206, 2, 4, 0.56], [20252, 2, 4, 0.48], [6936, 2, 5, 1.3], [1777, 1, 4, 1.16], [8648, 2, 4, 0.89], [151, 1, 4, 0.35], [2328, 2, 4, 0.73], [8650, 2, 4, 1.0], [5151, 2, 4, 0.9], [2050, 3, 4, 0.73], [248, 1, 4, 0.44], [88, 10, 8, 1.09], [7886, 4, 5, 0.39], [9507, 3, 4, 0.36], [74, 1, 4, 0.8], [1446, 2, 4, 0.59], [2991, 3, 4, 1.1], [362, 2, 4, 0.43], [7004, 1, 4, 0.54], [2057, 3, 4, 0.47], [1492, 1, 4, 0.51], [1007, 2, 5, 0.2], [2055, 3, 4, 0.57], [147, 1, 4, 1.02], [76, 2, 4, 0.74], [8649, 2, 4, 1.05], [3889, 1, 4, 0.44], [11234, 2, 6, 0.2], [410, 1, 4, 0.38], [7005, 1, 4, 0.38], [345, 3, 4, 0.47], [10, 2, 5, 0.41], [1429, 2, 4, 0.28], [307, 2, 4, 1.75], [10825, 21, 8, 0.55], [5081, 2, 4, 0.54], [12870, 1, 4, 0.65], [57, 1, 4, 0.44], [10149, 3, 13, 0.71], [7036, 1, 4, 0.94], [3478, 2, 4, 0.54], [7084, 3, 4, 0.87], [1006, 2, 4, 0.56], [1504, 2, 4, 0.2], [3891, 1, 4, 0.2], [21793, 1, 4, 0.89], [94, 4, 4, 1.55], [167, 3, 4, 0.75], [411, 2, 4, 0.47], [9827, 3, 4, 0.2], [3893, 1, 4, 0.2], [79, 1, 4, 0.57], [33, 1, 4, 0.76], [432, 3, 5, 0.62], [8677, 3, 5, 0.4], [11681, 2, 5, 0.82], [148, 1, 4, 1.5], [96, 11, 15, 0.38], [1490, 1, 5, 0.2], [12225, 1, 4, 0.43], [1124, 2, 5, 0.2], [11737, 2, 4, 0.2], [1243, 2, 4, 0.5], [22247, 2, 6, 0.89], [6158, 2, 5, 0.8], [5812, 3, 5, 1.51], [8853, 2, 5, 1.32], [201, 3, 4, 0.47], [412, 1, 4, 1.28], [9760, 29, 4, 0.24], [10574, 3, 6, 1.33], [8651, 2, 5, 0.61], [20927, 1, 4, 0.43], [5208, 3, 5, 0.54], [8676, 2, 6, 0.56], [229, 1, 4, 1.2], [1767, 25, 4, 0.59], [25, 1, 4, 0.76], [45, 2, 4, 1.37], [9069, 1, 4, 0.41], [413, 1, 4, 1.19], [11490, 1, 4, 0.36], [149, 2, 4, 1.7], [159, 3, 5, 0.63], [3495, 3, 15, 0.92], [21269, 3, 4, 1.0], [998, 2, 4, 0.97], [140, 2, 4, 0.78], [95, 3, 10, 0.93], [3980, 4, 5, 1.25], [950, 1, 4, 0.71], [5946, 1, 4, 0.95], [9372, 1, 4, 2.03], [1126, 2, 5, 0.47], [1766, 25, 4, 0.56], [2775, 2, 5, 0.2], [1413, 15, 5, 0.78], [490, 1, 4, 0.4], [506, 1, 4, 1.21], [8674, 2, 5, 0.54], [11489, 1, 4, 0.56], [8898, 3, 4, 0.75], [997, 2, 4, 1.82], [3670, 2, 4, 1.87], [1070, 7, 9, 0.46], [9691, 1, 4, 0.98], [107, 2, 4, 0.52], [974, 3, 5, 0.38], [20498, 1, 4, 0.94], [11954, 1, 4, 0.47], [14037, 3, 5, 0.44], [14017, 3, 4, 0.44], [823, 1, 4, 0.84], [34, 1, 4, 1.26], [5209, 3, 4, 0.54], [972, 3, 5, 0.85], [9784, 1, 5, 0.55], [11739, 2, 4, 0.2], [1091, 1, 4, 0.61], [8672, 2, 193, 4.11], [305, 2, 97, 3.11], [3, 2, 81, 3.34], [6935, 2, 216, 4.9], [205, 2, 83, 2.52], [143, 2, 98, 3.77], [144, 2, 100, 4.38], [75, 2, 112, 2.56], [12721, 2, 216, 2.64], [145, 2, 100, 3.97], [8915, 2, 148, 2.53], [2778, 2, 119, 2.63], [1776, 1, 72, 1.98], [146, 2, 100, 3.97], [206, 2, 93, 2.33], [20252, 2, 79, 2.19], [6936, 2, 216, 4.39], [1777, 1, 82, 3.8], [8648, 2, 171, 3.3], [151, 1, 46, 1.81], [2328, 2, 115, 3.01], [8650, 2, 171, 3.51], [5151, 2, 18, 4.59], [2050, 3, 204, 2.91], [248, 1, 46, 2.11], [88, 10, 428, 4.1], [7886, 4, 79, 2.38], [9507, 3, 86, 1.53], [74, 1, 153, 3.13], [1446, 2, 117, 3.67], [2991, 3, 124, 5.3], [362, 2, 108, 2.45], [7004, 1, 51, 2.45], [2057, 3, 408, 2.17], [1492, 1, 26, 2.52], [1007, 2, 207, 2.48], [2055, 3, 408, 2.35], [147, 1, 74, 5.47], [76, 2, 82, 3.03], [8649, 2, 171, 3.59], [3889, 1, 106, 2.11], [11234, 2, 141, 2.92], [410, 1, 90, 2.0], [7005, 1, 68, 2.01], [345, 3, 226, 2.53], [10, 2, 81, 3.33], [1429, 2, 117, 3.12], [307, 2, 112, 3.95], [10825, 21, 477, 2.64], [5081, 2, 144, 2.66], [12870, 1, 104, 2.86], [57, 1, 73, 2.11], [10149, 3, 666, 2.87], [7036, 1, 98, 3.26], [3478, 2, 64, 2.3], [7084, 3, 98, 3.26], [1006, 2, 175, 2.7], [1504, 2, 157, 2.66], [3891, 1, 95, 3.37], [21793, 1, 202, 4.74], [94, 4, 91, 4.72], [167, 3, 172, 3.03], [411, 2, 83, 2.52], [9827, 3, 67, 2.54], [3893, 1, 95, 2.31], [79, 1, 41, 2.38], [33, 1, 85, 3.19]]</t>
+  </si>
+  <si>
+    <t>[[8672, 2, 6, 0.55], [305, 2, 4, 0.57], [2049, 3, 8, 0.2], [6935, 2, 8, 1.1], [326, 2, 4, 1.08], [141, 2, 4, 0.66], [144, 2, 5, 0.36], [589, 2, 5, 0.2], [151, 1, 4, 0.48], [362, 2, 4, 0.2], [12721, 2, 6, 0.56], [146, 2, 5, 0.41], [1776, 1, 4, 1.16], [145, 2, 4, 0.44], [206, 2, 4, 0.2], [2328, 2, 5, 0.73], [8915, 2, 6, 0.2], [143, 2, 4, 0.58], [990, 2, 4, 0.26], [6936, 2, 5, 1.55], [20252, 2, 4, 0.5], [8650, 2, 4, 1.18], [1777, 1, 4, 0.93], [1007, 2, 5, 0.39], [2778, 2, 5, 0.2], [248, 1, 4, 0.2], [88, 10, 9, 1.09], [22247, 2, 4, 0.78], [2050, 3, 5, 0.38], [76, 2, 4, 1.24], [8649, 2, 5, 1.22], [10149, 3, 17, 1.82], [10, 2, 5, 0.41], [8677, 3, 6, 1.56], [2054, 3, 4, 1.44], [412, 1, 4, 0.62], [2055, 3, 4, 1.36], [13028, 3, 4, 0.75], [413, 1, 4, 1.1], [7004, 1, 4, 0.36], [411, 2, 4, 0.48], [10825, 21, 8, 1.28], [11681, 2, 5, 1.87], [1446, 2, 4, 0.54], [7084, 3, 4, 0.86], [307, 2, 4, 0.47], [3478, 2, 4, 0.89], [1429, 2, 4, 0.2], [3495, 3, 15, 0.92], [1006, 2, 4, 0.47], [147, 1, 4, 0.52], [1492, 1, 4, 0.58], [5081, 2, 4, 0.44], [140, 2, 5, 0.63], [167, 3, 4, 0.75], [7005, 1, 4, 0.36], [7036, 1, 4, 0.61], [9827, 3, 4, 0.2], [45, 2, 5, 0.56], [8676, 2, 4, 0.51], [1124, 2, 6, 0.2], [2049, 1, 4, 0.93], [94, 4, 4, 1.74], [5812, 3, 5, 2.01], [13280, 1, 4, 1.47], [168, 3, 5, 0.29], [1504, 2, 4, 0.2], [12870, 1, 5, 0.54], [57, 1, 4, 0.38], [11234, 2, 4, 0.63], [415, 1, 4, 1.07], [8651, 2, 4, 0.78], [148, 1, 4, 0.52], [418, 2, 4, 0.38], [8853, 2, 5, 1.07], [6097, 29, 4, 1.14], [8939, 2, 4, 0.2], [416, 1, 4, 1.21], [6097, 80, 4, 1.14], [11737, 2, 5, 0.2], [20256, 2, 5, 0.2], [490, 1, 4, 1.05], [1490, 1, 5, 0.2], [998, 2, 4, 1.06], [20927, 1, 4, 0.36], [79, 1, 4, 0.38], [95, 3, 16, 0.19], [6098, 29, 4, 1.08], [14017, 3, 4, 0.52], [6098, 80, 4, 1.08], [414, 1, 4, 0.81], [9069, 1, 4, 0.99], [1070, 7, 10, 0.2], [1243, 2, 4, 0.53], [8898, 3, 5, 1.36], [1126, 2, 4, 0.39], [149, 2, 4, 0.52], [126, 2, 4, 1.43], [13034, 3, 5, 0.66], [997, 2, 4, 1.09], [9760, 29, 4, 0.45], [20498, 1, 5, 0.8], [20255, 2, 5, 0.2], [5086, 1, 4, 0.71], [5513, 2, 4, 0.46], [12924, 1, 5, 0.2], [9784, 1, 4, 0.55], [336, 15, 4, 0.86], [22317, 3, 6, 0.51], [11739, 2, 4, 0.2], [13260, 29, 4, 0.54], [7567, 3, 4, 1.66], [974, 3, 4, 0.88], [1413, 15, 4, 0.33], [11085, 2, 4, 0.45], [5811, 3, 5, 1.26], [229, 1, 4, 1.05], [972, 3, 5, 0.81], [5813, 3, 5, 1.08], [8557, 3, 4, 0.2], [192, 3, 11, 1.1], [9082, 3, 17, 1.28], [506, 1, 4, 0.52], [3049, 3, 5, 1.6], [9691, 1, 4, 1.0], [20498, 3, 5, 0.86], [14018, 3, 4, 0.52], [524, 1, 4, 1.12], [4076, 3, 4, 1.54], [470, 1, 5, 0.2], [1622, 1, 5, 0.38], [11454, 2, 6, 1.6], [2775, 2, 5, 0.2], [8672, 2, 235, 2.23], [305, 2, 121, 2.31], [2049, 3, 450, 1.94], [6935, 2, 235, 4.34], [326, 2, 84, 3.42], [141, 2, 143, 3.4], [144, 2, 125, 1.93], [589, 2, 127, 2.26], [151, 1, 54, 2.16], [362, 2, 117, 2.1], [12721, 2, 234, 2.25], [146, 2, 125, 2.03], [1776, 1, 100, 3.34], [145, 2, 139, 1.96], [206, 2, 90, 1.99], [2328, 2, 126, 2.62], [8915, 2, 161, 2.05], [143, 2, 122, 2.33], [990, 2, 43, 2.66], [6936, 2, 235, 4.51], [20252, 2, 86, 2.06], [8650, 2, 186, 3.42], [1777, 1, 100, 4.11], [1007, 2, 250, 1.96], [2778, 2, 130, 2.06], [248, 1, 45, 1.0], [88, 10, 463, 3.28], [22247, 2, 234, 3.12], [2050, 3, 389, 1.95], [76, 2, 90, 2.63], [8649, 2, 186, 3.51], [10149, 3, 715, 4.79], [10, 2, 87, 2.92], [8677, 3, 243, 4.35], [2054, 3, 324, 5.02], [412, 1, 69, 2.41], [2055, 3, 324, 5.02], [13028, 3, 136, 2.54], [413, 1, 71, 2.36], [7004, 1, 65, 1.93], [411, 2, 101, 2.04], [10825, 21, 575, 3.49], [11681, 2, 227, 5.53], [1446, 2, 126, 3.18], [7084, 3, 107, 1.93], [307, 2, 122, 2.12], [3478, 2, 69, 3.31], [1429, 2, 126, 2.47], [3495, 3, 797, 2.89], [1006, 2, 189, 2.13], [147, 1, 80, 3.88], [1492, 1, 30, 3.25], [5081, 2, 177, 1.96], [140, 2, 75, 2.75], [167, 3, 188, 2.64], [7005, 1, 65, 1.93], [7036, 1, 105, 2.39], [9827, 3, 72, 2.15], [45, 2, 90, 4.21], [8676, 2, 235, 2.21], [1124, 2, 153, 2.07], [2049, 1, 21, 2.85], [94, 4, 99, 4.73], [5812, 3, 543, 4.52], [13280, 1, 261, 3.97], [168, 3, 339, 2.73], [1504, 2, 170, 2.1]]</t>
+  </si>
+  <si>
+    <t>[[11685, 2, 4, 1.88], [6935, 2, 5, 1.18], [130, 1, 4, 0.2], [326, 2, 4, 1.12], [8648, 2, 4, 0.7], [144, 2, 4, 0.2], [593, 2, 4, 0.45], [2327, 2, 4, 0.47], [143, 2, 4, 0.58], [205, 2, 5, 0.53], [8915, 2, 5, 1.45], [2328, 2, 4, 0.5], [11681, 2, 4, 1.35], [6936, 2, 4, 1.18], [305, 2, 5, 0.48], [151, 1, 4, 0.59], [8650, 2, 4, 0.57], [141, 2, 4, 0.48], [2778, 2, 5, 0.2], [206, 2, 4, 0.46], [2049, 3, 8, 0.41], [88, 10, 10, 0.37], [615, 2, 4, 1.69], [7036, 1, 4, 1.57], [8853, 2, 4, 1.18], [8649, 2, 4, 0.97], [5491, 2, 4, 0.47], [248, 1, 4, 0.43], [434, 2, 4, 0.47], [1006, 2, 4, 1.0], [75, 2, 5, 0.99], [2055, 3, 4, 1.75], [11737, 2, 5, 0.2], [990, 2, 4, 0.2], [417, 2, 4, 0.54], [616, 2, 4, 1.5], [3840, 1, 4, 0.39], [2050, 3, 4, 0.34], [1007, 2, 5, 0.51], [12870, 1, 4, 0.92], [12353, 1, 5, 0.19], [523, 2, 4, 1.0], [1504, 2, 4, 1.07], [159, 3, 5, 0.37], [20927, 1, 4, 0.67], [2057, 3, 4, 0.34], [13280, 1, 4, 2.05], [10574, 3, 6, 1.36], [3, 2, 5, 0.2], [142, 2, 4, 0.51], [12346, 1, 4, 0.19], [7084, 3, 4, 0.58], [9760, 29, 4, 0.2], [624, 2, 4, 1.35], [2054, 3, 4, 0.34], [140, 2, 4, 0.93], [2775, 2, 4, 0.2], [21793, 1, 4, 2.3], [3891, 1, 4, 0.53], [8939, 2, 4, 0.2], [1429, 2, 5, 0.2], [96, 11, 13, 0.38], [11739, 2, 4, 0.59], [6158, 2, 4, 0.2], [950, 1, 4, 0.37], [5165, 2, 5, 1.61], [12269, 2, 4, 1.03], [84, 2, 4, 1.02], [1126, 2, 4, 0.58], [9372, 1, 4, 1.7], [10388, 2, 4, 1.08], [411, 2, 4, 0.5], [98, 11, 10, 0.54], [972, 3, 4, 1.07], [5165, 1, 4, 0.58], [2912, 1, 4, 0.2], [8898, 3, 4, 3.33], [413, 1, 4, 1.01], [2776, 2, 4, 1.41], [410, 1, 4, 0.54], [12343, 1, 5, 0.19], [10386, 2, 4, 0.92], [995, 2, 4, 1.84], [9491, 21, 10, 1.07], [956, 2, 4, 0.47], [1492, 1, 5, 0.7], [418, 2, 4, 0.42], [12345, 1, 5, 0.19], [13928, 1, 5, 0.2], [9784, 1, 4, 0.47], [22316, 3, 4, 0.51], [147, 1, 4, 0.53], [22247, 2, 4, 1.23], [412, 1, 4, 0.2], [336, 15, 4, 0.86], [8677, 3, 4, 0.9], [11490, 1, 4, 0.56], [7567, 3, 4, 1.65], [2912, 2, 5, 0.47], [308, 1, 4, 0.91], [432, 3, 5, 0.47], [307, 2, 5, 0.59], [11953, 1, 4, 0.45], [33, 1, 4, 1.06], [11770, 1, 4, 0.48], [10631, 2, 4, 0.92], [414, 1, 4, 0.66], [35, 1, 4, 1.07], [148, 1, 4, 0.55], [20256, 2, 4, 0.44], [10407, 10, 6, 1.44], [22317, 3, 5, 0.51], [1413, 15, 4, 0.45], [10410, 10, 6, 1.64], [10780, 10, 4, 1.52], [13286, 1, 4, 1.32], [415, 1, 4, 0.66], [439, 1, 4, 1.15], [335, 3, 9, 1.35], [7886, 4, 4, 0.47], [9691, 1, 4, 0.55], [7573, 1, 5, 1.45], [11767, 1, 4, 0.5], [12347, 1, 4, 0.19], [972, 1, 4, 1.51], [10387, 2, 4, 0.95], [10149, 3, 13, 0.39], [74, 1, 4, 1.16], [20686, 1, 5, 1.33], [3478, 2, 4, 1.63], [12271, 2, 4, 1.01], [9690, 1, 4, 0.76], [9971, 2, 4, 1.44], [11685, 2, 212, 5.4], [6935, 2, 214, 5.9], [130, 1, 45, 2.58], [326, 2, 40, 3.57], [8648, 2, 174, 2.99], [144, 2, 117, 4.4], [593, 2, 177, 2.78], [2327, 2, 117, 2.57], [143, 2, 115, 2.77], [205, 2, 84, 2.69], [8915, 2, 65, 4.29], [2328, 2, 117, 2.62], [11681, 2, 212, 5.01], [6936, 2, 214, 5.92], [305, 2, 113, 2.58], [151, 1, 58, 2.7], [8650, 2, 174, 2.75], [141, 2, 119, 2.6], [2778, 2, 121, 2.77], [206, 2, 84, 2.55], [2049, 3, 421, 2.25], [88, 10, 450, 3.45], [615, 2, 91, 4.78], [7036, 1, 99, 3.83], [8853, 2, 214, 5.93], [8649, 2, 174, 2.58], [5491, 2, 81, 2.57], [248, 1, 47, 2.25], [434, 2, 56, 2.07], [1006, 2, 177, 2.63], [75, 2, 112, 3.52], [2055, 3, 396, 4.89], [11737, 2, 45, 2.79], [990, 2, 32, 2.77], [417, 2, 133, 2.43], [616, 2, 91, 4.41], [3840, 1, 150, 2.17], [2050, 3, 356, 2.34], [1007, 2, 207, 2.65], [12870, 1, 117, 5.16], [12353, 1, 488, 4.47], [523, 2, 119, 2.64], [1504, 2, 156, 2.75], [159, 3, 619, 2.07], [20927, 1, 68, 3.22], [2057, 3, 356, 2.34], [13280, 1, 246, 5.48], [10574, 3, 393, 4.07], [3, 2, 95, 2.52], [142, 2, 133, 2.39], [12346, 1, 488, 4.15], [7084, 3, 58, 2.79], [9760, 29, 55, 2.5], [624, 2, 91, 5.38], [2054, 3, 356, 2.34], [140, 2, 78, 3.15], [2775, 2, 121, 2.77], [21793, 1, 174, 5.26], [3891, 1, 108, 2.43], [8939, 2, 150, 2.61], [1429, 2, 117, 2.59], [96, 11, 374, 2.81], [11739, 2, 45, 2.79], [6158, 2, 204, 2.54], [950, 1, 41, 2.04], [12269, 2, 55, 3.35], [84, 2, 52, 2.67]]</t>
+  </si>
+  <si>
+    <t>[[8672, 2, 5, 0.47], [141, 2, 4, 0.66], [362, 2, 5, 0.2], [361, 2, 5, 0.54], [6935, 2, 7, 1.06], [205, 2, 4, 0.36], [12721, 2, 5, 1.21], [11737, 2, 4, 0.43], [206, 2, 4, 0.2], [2049, 3, 10, 0.21], [8676, 2, 4, 0.49], [8675, 2, 4, 0.6], [417, 2, 4, 0.57], [3, 2, 4, 0.5], [6936, 2, 4, 1.58], [305, 2, 5, 0.53], [151, 1, 4, 0.75], [523, 2, 4, 0.53], [22247, 2, 4, 1.0], [8650, 2, 4, 0.89], [142, 2, 4, 0.49], [8648, 2, 4, 1.7], [2328, 2, 4, 0.78], [2776, 2, 4, 0.2], [8853, 2, 4, 1.54], [616, 2, 4, 1.12], [11739, 2, 4, 0.43], [2327, 2, 5, 0.63], [11837, 2, 4, 0.45], [411, 2, 4, 0.47], [12352, 1, 4, 1.38], [589, 2, 4, 0.2], [143, 2, 4, 0.87], [146, 2, 4, 0.62], [11835, 2, 4, 0.55], [412, 1, 4, 1.0], [12353, 1, 4, 1.38], [6497, 1, 5, 0.5], [8674, 2, 5, 0.63], [583, 2, 4, 1.31], [145, 2, 4, 0.49], [2805, 137, 8, 0.2], [326, 2, 4, 1.31], [10574, 3, 5, 1.26], [418, 2, 4, 0.54], [144, 2, 4, 0.52], [6097, 80, 4, 1.14], [11738, 2, 4, 0.43], [11836, 2, 4, 0.53], [9784, 1, 4, 0.99], [10149, 3, 13, 0.49], [6097, 29, 5, 0.64], [413, 1, 4, 0.97], [2057, 3, 4, 1.0], [2055, 3, 4, 1.18], [75, 2, 4, 0.56], [11234, 2, 4, 0.63], [12344, 1, 4, 1.38], [1413, 15, 4, 0.2], [20252, 2, 4, 0.47], [11504, 2, 4, 0.2], [12269, 2, 4, 0.57], [8915, 2, 4, 0.39], [414, 1, 4, 0.99], [1492, 1, 4, 0.62], [6098, 80, 4, 1.14], [12346, 1, 4, 1.38], [3429, 15, 4, 0.46], [247, 1, 4, 0.8], [22316, 3, 4, 0.46], [1886, 2, 4, 0.2], [2774, 2, 4, 0.52], [1490, 1, 4, 0.36], [416, 1, 4, 1.16], [6098, 29, 4, 1.19], [9786, 1, 4, 1.55], [3934, 5, 5, 0.56], [2859, 15, 4, 0.57], [2049, 1, 4, 0.41], [201, 3, 4, 0.51], [3670, 2, 4, 0.97], [20555, 2, 4, 0.43], [6158, 2, 5, 0.44], [3478, 2, 4, 0.89], [7084, 3, 4, 0.94], [9785, 1, 4, 0.99], [12526, 2, 4, 0.73], [8599, 1, 4, 0.49], [8938, 2, 4, 0.58], [1703, 2, 4, 0.75], [4253, 1, 4, 0.5], [9760, 29, 4, 0.95], [186, 3, 7, 0.5], [1413, 16, 4, 0.37], [229, 1, 4, 1.15], [11885, 2, 4, 0.39], [107, 2, 4, 1.2], [11887, 2, 5, 0.39], [1050, 2, 4, 0.37], [11811, 1, 4, 0.38], [4232, 80, 4, 1.65], [94, 4, 4, 1.76], [11490, 1, 4, 0.52], [436, 2, 4, 0.51], [107, 7, 5, 1.13], [2438, 2, 5, 1.38], [415, 1, 4, 1.16], [947, 15, 4, 0.39], [11770, 1, 4, 0.43], [3673, 2, 4, 2.08], [11767, 1, 4, 0.48], [11671, 1, 4, 0.45], [5939, 3, 4, 0.5], [2821, 3, 8, 0.45], [11769, 1, 4, 0.48], [11160, 1, 4, 1.87], [11844, 2, 4, 0.47], [12347, 1, 4, 1.38], [5812, 3, 4, 2.0], [7036, 1, 4, 0.43], [9358, 1, 4, 0.44], [140, 2, 4, 1.31], [3495, 3, 13, 0.85], [12764, 2, 5, 0.49], [11771, 1, 4, 1.61], [5813, 3, 5, 1.1], [23920, 2, 4, 0.46], [11954, 1, 4, 0.42], [308, 1, 5, 0.79], [9690, 1, 4, 0.79], [410, 1, 4, 0.8], [5811, 3, 6, 1.16], [22573, 2, 4, 0.39], [8672, 2, 258, 3.11], [141, 2, 156, 3.01], [362, 2, 127, 2.98], [361, 2, 140, 3.1], [6935, 2, 253, 5.12], [205, 2, 110, 2.44], [12721, 2, 285, 4.59], [11737, 2, 57, 3.01], [206, 2, 65, 2.62], [2049, 3, 313, 2.87], [8676, 2, 287, 4.22], [8675, 2, 287, 3.21], [417, 2, 140, 3.15], [3, 2, 109, 3.03], [6936, 2, 253, 4.65], [305, 2, 132, 3.08], [151, 1, 33, 2.81], [523, 2, 140, 3.23], [22247, 2, 285, 3.62], [8650, 2, 202, 4.44], [142, 2, 156, 2.68], [8648, 2, 202, 4.32], [2328, 2, 135, 3.53], [2776, 2, 142, 3.28], [8853, 2, 282, 4.82], [616, 2, 107, 4.01], [11739, 2, 57, 3.01], [2327, 2, 135, 3.26], [11837, 2, 268, 2.61], [411, 2, 110, 2.65], [12352, 1, 607, 4.89], [589, 2, 59, 2.91], [143, 2, 147, 3.39], [146, 2, 151, 2.93], [11835, 2, 241, 3.11], [412, 1, 74, 3.02], [12353, 1, 607, 4.89], [6497, 1, 34, 3.94], [8674, 2, 258, 3.28], [583, 2, 30, 3.93], [145, 2, 151, 2.69], [2805, 137, 166, 3.7], [326, 2, 30, 3.62], [10574, 3, 450, 4.6], [418, 2, 142, 2.79], [144, 2, 151, 2.74], [6097, 80, 61, 5.49], [11738, 2, 57, 3.01], [11836, 2, 268, 2.76], [9784, 1, 64, 3.01], [10149, 3, 906, 2.65], [6097, 29, 30, 5.49], [413, 1, 77, 2.97], [2057, 3, 158, 4.31], [2055, 3, 158, 4.31], [75, 2, 144, 2.82], [11234, 2, 185, 3.11], [12344, 1, 607, 4.33], [1413, 15, 90, 3.0], [20252, 2, 94, 2.66], [11504, 2, 127, 2.78], [12269, 2, 65, 2.84], [8915, 2, 97, 2.14], [414, 1, 77, 3.01], [1492, 1, 37, 2.92], [6098, 80, 66, 4.03], [12346, 1, 607, 4.89]]</t>
+  </si>
+  <si>
+    <t>[[2327, 2, 4, 0.52], [305, 2, 4, 0.45], [6935, 2, 5, 1.77], [2778, 2, 4, 0.2], [144, 2, 4, 0.53], [130, 1, 4, 0.48], [8915, 2, 5, 1.08], [589, 2, 5, 0.2], [143, 2, 4, 0.58], [2328, 2, 4, 0.39], [6936, 2, 4, 1.74], [8648, 2, 5, 1.05], [2775, 2, 4, 0.2], [205, 2, 4, 0.43], [8650, 2, 5, 0.39], [326, 2, 4, 0.65], [593, 2, 4, 0.37], [146, 2, 4, 0.57], [145, 2, 4, 0.51], [7036, 1, 4, 0.44], [2049, 3, 5, 0.42], [2776, 2, 4, 0.2], [615, 2, 4, 0.2], [616, 2, 4, 0.2], [88, 10, 9, 0.93], [141, 2, 4, 0.2], [151, 1, 4, 0.75], [1124, 2, 4, 0.79], [11681, 2, 5, 0.83], [206, 2, 4, 0.37], [1446, 2, 4, 0.2], [9760, 29, 4, 0.37], [8853, 2, 4, 1.79], [990, 2, 5, 0.2], [5491, 2, 4, 0.58], [1007, 2, 4, 0.46], [362, 2, 4, 0.5], [8672, 2, 4, 1.48], [1504, 2, 4, 0.93], [2055, 3, 4, 0.46], [2057, 3, 4, 0.46], [9372, 1, 4, 1.97], [3893, 1, 4, 0.2], [8649, 2, 5, 0.39], [2912, 1, 4, 0.48], [8938, 2, 4, 0.52], [434, 2, 4, 0.2], [12870, 1, 4, 1.22], [10993, 2, 5, 0.2], [624, 2, 4, 1.1], [2050, 3, 4, 0.46], [417, 2, 4, 0.42], [3889, 1, 4, 0.35], [5165, 1, 4, 0.56], [1429, 2, 4, 0.2], [378, 2, 4, 2.29], [7084, 3, 4, 0.86], [10, 2, 4, 0.45], [2991, 3, 4, 1.1], [140, 2, 4, 1.65], [3891, 1, 4, 0.2], [1006, 2, 4, 0.54], [7886, 4, 5, 0.41], [10574, 3, 5, 1.36], [7573, 1, 8, 2.02], [10149, 3, 13, 0.39], [5208, 3, 4, 0.19], [1622, 1, 4, 0.56], [75, 2, 4, 0.39], [3, 2, 4, 0.46], [20927, 1, 4, 0.95], [5165, 2, 5, 1.02], [997, 2, 4, 1.42], [11234, 2, 4, 1.25], [1886, 2, 4, 0.2], [12721, 2, 5, 0.49], [22247, 2, 4, 1.37], [147, 1, 4, 1.75], [346, 3, 4, 0.19], [996, 2, 4, 1.16], [229, 1, 4, 0.47], [11811, 1, 4, 0.2], [20252, 2, 4, 0.38], [11685, 2, 5, 0.83], [94, 4, 4, 1.91], [998, 2, 5, 1.0], [972, 3, 5, 0.51], [2912, 2, 7, 0.2], [9491, 21, 10, 0.44], [76, 2, 4, 0.87], [35, 1, 4, 1.02], [439, 1, 4, 0.46], [413, 1, 4, 1.08], [13028, 3, 5, 1.54], [13928, 1, 4, 0.2], [8104, 1, 4, 0.87], [5076, 1, 4, 0.43], [2805, 137, 4, 0.6], [412, 1, 4, 0.43], [5209, 3, 4, 0.19], [8676, 2, 4, 2.17], [33, 1, 4, 0.97], [83, 2, 4, 0.88], [418, 2, 4, 0.63], [148, 1, 4, 1.76], [2774, 2, 4, 0.63], [3495, 3, 10, 0.82], [8898, 3, 5, 1.44], [7887, 4, 4, 0.94], [12212, 29, 4, 0.2], [20256, 2, 5, 0.2], [38, 1, 4, 1.16], [11490, 1, 5, 0.43], [11770, 1, 4, 0.88], [34, 1, 4, 1.09], [10407, 10, 7, 1.55], [415, 1, 4, 1.02], [9784, 1, 4, 0.52], [84, 2, 5, 0.47], [13928, 2, 4, 0.7], [126, 2, 4, 1.27], [411, 2, 4, 0.39], [11739, 2, 4, 1.42], [3048, 3, 4, 1.15], [9691, 1, 4, 0.57], [9690, 1, 4, 0.37], [8939, 2, 4, 0.2], [5584, 3, 5, 1.25], [11953, 1, 4, 0.46], [39, 1, 4, 1.13], [12351, 1, 4, 0.66], [11954, 1, 4, 0.38], [7567, 3, 5, 1.16], [2327, 2, 132, 2.93], [305, 2, 128, 2.8], [6935, 2, 244, 6.0], [2778, 2, 137, 2.92], [144, 2, 132, 4.54], [130, 1, 43, 2.86], [8915, 2, 165, 2.96], [589, 2, 134, 2.97], [143, 2, 130, 3.03], [2328, 2, 147, 3.37], [6936, 2, 244, 5.39], [8648, 2, 196, 3.91], [2775, 2, 137, 2.92], [205, 2, 95, 2.77], [8650, 2, 196, 3.45], [326, 2, 77, 4.1], [593, 2, 223, 2.53], [146, 2, 132, 3.02], [145, 2, 132, 2.92], [7036, 1, 113, 4.28], [2049, 3, 360, 2.34], [2776, 2, 137, 3.16], [615, 2, 93, 3.01], [616, 2, 93, 2.64], [88, 10, 490, 3.94], [141, 2, 136, 2.69], [151, 1, 32, 2.69], [1124, 2, 182, 3.1], [11681, 2, 234, 5.43], [206, 2, 106, 2.39], [1446, 2, 134, 3.2], [9760, 29, 63, 2.66], [8853, 2, 244, 5.48], [990, 2, 45, 2.69], [5491, 2, 93, 3.05], [1007, 2, 264, 2.49], [362, 2, 124, 2.89], [8672, 2, 247, 4.92], [1504, 2, 180, 3.69], [2055, 3, 314, 2.32], [2057, 3, 314, 2.32], [9372, 1, 201, 5.58], [3893, 1, 109, 2.96], [8649, 2, 196, 3.26], [2912, 1, 48, 2.53], [8938, 2, 125, 2.43], [434, 2, 93, 2.69], [12870, 1, 121, 3.3], [10993, 2, 40, 2.81], [624, 2, 104, 3.83], [2050, 3, 314, 2.32], [417, 2, 136, 2.76], [3889, 1, 122, 2.29], [5165, 1, 32, 3.97], [1429, 2, 134, 2.89], [378, 2, 218, 5.85], [7084, 3, 127, 3.22], [10, 2, 102, 3.24], [2991, 3, 141, 5.62], [140, 2, 77, 4.1], [3891, 1, 109, 2.96], [1006, 2, 200, 2.97], [7886, 4, 83, 2.24], [10574, 3, 278, 4.55], [7573, 1, 336, 6.0], [10149, 3, 848, 3.11], [5208, 3, 493, 2.87]]</t>
+  </si>
+  <si>
+    <t>[[2778, 2, 11, 1.2], [6935, 2, 19, 4.42], [6936, 2, 9, 3.89], [305, 2, 7, 1.48], [8672, 2, 10, 1.28], [615, 2, 7, 1.37], [1504, 2, 11, 0.9], [2775, 2, 9, 1.03], [145, 2, 7, 1.24], [2776, 2, 9, 1.98], [8853, 2, 7, 3.02], [2327, 2, 7, 1.21], [12721, 2, 11, 1.7], [130, 1, 9, 0.78], [143, 2, 7, 1.94], [146, 2, 7, 1.53], [2328, 2, 7, 1.5], [11681, 2, 11, 3.38], [11737, 2, 7, 1.32], [616, 2, 7, 2.16], [5491, 2, 7, 1.03], [141, 2, 7, 2.37], [362, 2, 6, 0.85], [144, 2, 7, 1.3], [2497, 2, 7, 1.14], [205, 2, 7, 0.85], [8650, 2, 11, 2.33], [5493, 2, 9, 0.77], [417, 2, 7, 1.55], [8676, 2, 7, 0.9], [8673, 2, 9, 2.44], [3670, 2, 9, 4.0], [2774, 2, 9, 3.42], [8648, 2, 7, 3.5], [589, 2, 9, 0.8], [3, 2, 7, 0.98], [206, 2, 7, 0.71], [6097, 80, 7, 3.38], [2423, 29, 7, 3.08], [22247, 2, 7, 1.94], [11836, 2, 7, 0.9], [6497, 1, 7, 1.84], [8674, 2, 7, 1.97], [624, 2, 7, 2.32], [12343, 1, 7, 2.59], [2055, 3, 7, 3.23], [2423, 80, 7, 3.02], [523, 2, 7, 1.25], [12344, 1, 7, 1.6], [593, 2, 8, 0.79], [6097, 29, 7, 3.38], [6098, 80, 7, 2.36], [12720, 2, 7, 1.69], [12345, 1, 7, 2.59], [11739, 2, 7, 1.32], [75, 2, 7, 2.15], [8915, 2, 7, 0.75], [88, 10, 14, 2.0], [326, 2, 7, 2.83], [6494, 1, 7, 0.85], [60, 3, 10, 1.49], [13260, 29, 7, 1.16], [142, 2, 7, 2.37], [3429, 15, 7, 0.85], [1492, 1, 7, 1.13], [411, 2, 7, 1.04], [21712, 3, 21, 1.11], [412, 1, 7, 1.93], [2422, 80, 7, 2.41], [1050, 2, 7, 0.7], [10149, 3, 21, 2.21], [2422, 29, 7, 3.8], [378, 2, 9, 2.87], [6098, 29, 7, 2.08], [12346, 1, 7, 2.59], [151, 1, 7, 1.38], [7704, 2, 7, 2.28], [11738, 2, 7, 1.32], [229, 1, 7, 3.68], [22316, 3, 7, 0.85], [1243, 2, 7, 1.32], [1049, 2, 7, 0.7], [20252, 2, 7, 1.06], [13264, 29, 7, 0.95], [345, 3, 7, 2.32], [13258, 29, 9, 2.97], [1490, 1, 7, 0.87], [12269, 2, 7, 0.93], [964, 15, 7, 0.66], [2438, 1, 7, 2.08], [10407, 10, 10, 2.2], [1163, 3, 7, 2.25], [5208, 3, 9, 1.41], [2331, 1, 7, 1.02], [2821, 3, 12, 1.27], [416, 1, 7, 3.06], [201, 3, 7, 4.28], [307, 2, 7, 1.91], [186, 3, 12, 0.9], [7004, 1, 7, 1.03], [149, 2, 7, 1.95], [13259, 29, 7, 2.95], [418, 2, 7, 0.99], [957, 2, 7, 1.05], [7705, 2, 7, 2.28], [12229, 2, 7, 0.96], [7706, 2, 7, 2.28], [11687, 2, 7, 1.02], [10406, 10, 12, 2.42], [410, 1, 7, 1.3], [3478, 2, 9, 1.47], [7036, 1, 7, 0.87], [9784, 1, 7, 1.67], [20255, 2, 7, 1.14], [8938, 2, 7, 1.07], [21713, 3, 13, 0.88], [12870, 1, 7, 4.46], [10408, 10, 10, 1.81], [5490, 2, 7, 0.91], [11402, 1, 7, 0.85], [11404, 2, 7, 0.83], [10410, 10, 10, 2.08], [11161, 1, 10, 3.78], [956, 2, 7, 0.96], [2438, 2, 8, 2.38], [2703, 3, 7, 4.05], [1886, 2, 7, 0.65], [19687, 1, 7, 2.23], [11490, 1, 7, 0.83], [107, 7, 8, 2.46], [21781, 2, 7, 0.86], [22125, 2, 7, 0.66], [11690, 2, 7, 0.66], [412, 1, 74, 3.02], [2422, 80, 187, 4.2], [1050, 2, 38, 1.78], [10149, 3, 866, 4.0], [2422, 29, 33, 5.41], [378, 2, 202, 4.24], [6098, 29, 33, 3.97], [12346, 1, 610, 4.37], [151, 1, 33, 2.81], [7704, 2, 176, 4.07], [11738, 2, 56, 3.11], [229, 1, 81, 5.47], [22316, 3, 318, 2.64], [1243, 2, 99, 3.11], [1049, 2, 38, 1.78], [20252, 2, 92, 2.85], [13264, 29, 73, 2.74], [345, 3, 297, 4.1], [13258, 29, 39, 4.76], [1490, 1, 51, 2.66], [12269, 2, 65, 2.72], [2438, 1, 54, 3.87], [10407, 10, 1201, 4.0], [1163, 3, 114, 3.33], [5208, 3, 561, 3.2], [2331, 1, 119, 2.8], [2821, 3, 746, 3.36], [416, 1, 85, 4.84], [201, 3, 297, 6.0], [307, 2, 148, 3.7], [186, 3, 665, 2.69], [7004, 1, 80, 2.82], [149, 2, 88, 3.74], [13259, 29, 35, 4.73], [418, 2, 143, 2.78], [957, 2, 107, 2.84], [7705, 2, 176, 4.07], [12229, 2, 152, 2.74], [7706, 2, 176, 4.07], [11687, 2, 303, 2.8], [10406, 10, 1784, 4.24], [410, 1, 105, 3.09], [3478, 2, 67, 4.08], [7036, 1, 127, 2.65], [9784, 1, 72, 3.46], [20255, 2, 93, 2.93], [8938, 2, 192, 2.86], [21713, 3, 1121, 2.67], [12870, 1, 137, 6.0], [10408, 10, 785, 3.6], [5490, 2, 108, 2.69], [11402, 1, 45, 2.64], [11404, 2, 105, 2.62], [10410, 10, 1201, 3.88], [11161, 1, 491, 5.57], [956, 2, 107, 2.75], [2438, 2, 643, 4.17], [2703, 3, 300, 5.84], [1886, 2, 158, 2.44], [19687, 1, 30, 4.02], [11490, 1, 98, 2.9], [107, 7, 239, 4.24], [21781, 2, 104, 2.65], [22125, 2, 63, 2.44], [11690, 2, 303, 2.44]]</t>
+  </si>
+  <si>
+    <t>[[141, 2, 7, 1.22], [2328, 2, 7, 1.43], [8650, 2, 7, 2.83], [362, 2, 9, 0.78], [5491, 2, 7, 1.11], [5493, 2, 9, 0.67], [130, 1, 7, 1.38], [589, 2, 7, 0.85], [2327, 2, 7, 1.16], [326, 2, 7, 1.87], [11685, 2, 7, 4.19], [8672, 2, 10, 1.28], [417, 2, 7, 1.03], [6935, 2, 12, 4.21], [205, 2, 7, 0.74], [11681, 2, 11, 3.74], [206, 2, 7, 0.71], [8648, 2, 7, 3.27], [6936, 2, 8, 3.12], [142, 2, 9, 0.8], [8915, 2, 7, 1.26], [11837, 2, 7, 1.01], [12721, 2, 9, 1.92], [11838, 2, 9, 0.99], [2049, 3, 17, 1.18], [1446, 2, 7, 1.82], [523, 2, 7, 1.02], [615, 2, 7, 2.85], [8676, 2, 7, 2.44], [11737, 2, 7, 1.9], [305, 2, 7, 0.98], [616, 2, 7, 2.37], [413, 1, 7, 1.44], [412, 1, 7, 1.93], [411, 2, 7, 0.95], [11739, 2, 7, 1.9], [10574, 3, 9, 2.49], [11835, 2, 7, 1.01], [145, 2, 7, 1.24], [8675, 2, 9, 1.42], [2775, 2, 7, 0.78], [1429, 2, 7, 0.89], [76, 2, 7, 2.04], [8673, 2, 7, 3.38], [143, 2, 7, 1.19], [8674, 2, 7, 1.46], [11836, 2, 9, 0.79], [6158, 2, 9, 2.65], [8938, 2, 7, 1.78], [146, 2, 7, 1.14], [151, 1, 7, 1.38], [12720, 2, 7, 1.69], [2776, 2, 7, 1.37], [10149, 3, 21, 1.48], [3495, 3, 21, 1.51], [2055, 3, 7, 3.23], [75, 2, 7, 2.15], [2057, 3, 7, 3.23], [11738, 2, 7, 1.9], [144, 2, 7, 0.96], [8939, 2, 7, 3.23], [416, 1, 7, 1.34], [7885, 4, 7, 0.81], [22316, 3, 9, 0.85], [88, 10, 16, 2.9], [159, 3, 9, 1.37], [2859, 15, 7, 0.81], [7084, 3, 7, 1.81], [418, 2, 9, 0.68], [10993, 2, 7, 0.94], [20252, 2, 7, 0.68], [9784, 1, 7, 1.61], [7705, 2, 7, 2.28], [5165, 1, 7, 3.14], [410, 1, 7, 0.87], [12526, 2, 7, 2.78], [11844, 2, 7, 1.16], [414, 1, 7, 1.34], [2423, 80, 7, 2.8], [12351, 1, 7, 1.63], [2424, 29, 9, 1.09], [378, 2, 7, 2.23], [2423, 29, 7, 3.08], [12345, 1, 7, 1.19], [60, 3, 10, 4.98], [950, 1, 7, 0.72], [6494, 1, 7, 0.85], [11490, 1, 7, 0.89], [2424, 80, 7, 2.28], [12373, 1, 11, 1.47], [13023, 3, 10, 2.63], [201, 3, 7, 2.12], [13034, 3, 8, 2.37], [1519, 3, 15, 0.69], [11489, 1, 7, 0.68], [5208, 3, 9, 1.01], [345, 3, 7, 1.4], [11770, 1, 7, 0.89], [3, 2, 7, 5.0], [159, 1, 7, 1.33], [6952, 1, 7, 2.01], [3430, 15, 7, 2.26], [20927, 1, 7, 0.87], [11954, 1, 7, 0.77], [7886, 4, 7, 0.8], [432, 3, 7, 3.74], [3429, 15, 7, 0.85], [11504, 2, 7, 0.67], [566, 2, 7, 0.92], [13928, 1, 7, 0.82], [11811, 1, 7, 1.93], [5584, 3, 7, 2.91], [114, 3, 7, 3.01], [2331, 1, 7, 2.78], [10407, 10, 10, 2.2], [1492, 1, 7, 1.13], [105, 3, 7, 3.01], [7004, 1, 7, 1.91], [1490, 1, 7, 3.38], [11089, 1, 7, 0.71], [2703, 3, 7, 4.05], [6098, 80, 7, 2.52], [8274, 3, 7, 4.22], [11674, 1, 7, 0.66], [1886, 2, 7, 0.82], [12348, 1, 7, 1.19], [10410, 10, 10, 2.08], [94, 4, 7, 4.17], [3891, 1, 7, 4.39], [11953, 1, 7, 0.85], [6097, 80, 7, 3.42], [22317, 3, 8, 0.88], [9082, 3, 24, 2.42], [418, 2, 128, 2.79], [10993, 2, 49, 3.0], [20252, 2, 93, 2.46], [9784, 1, 72, 3.4], [7705, 2, 176, 4.07], [410, 1, 53, 2.3], [12526, 2, 273, 4.56], [11844, 2, 186, 2.77], [414, 1, 86, 3.13], [2423, 80, 166, 4.41], [12351, 1, 560, 3.26], [2424, 29, 30, 3.17], [378, 2, 201, 4.24], [2423, 29, 37, 4.87], [12345, 1, 560, 3.26], [950, 1, 30, 2.15], [6494, 1, 52, 2.64], [11490, 1, 109, 2.68], [2424, 80, 170, 4.07], [12373, 1, 533, 3.26], [13023, 3, 592, 4.42], [201, 3, 268, 3.21], [13034, 3, 592, 4.16], [1519, 3, 561, 1.77], [11489, 1, 109, 2.47], [5208, 3, 563, 2.79], [345, 3, 298, 3.19], [11770, 1, 221, 2.67], [3, 2, 118, 6.0], [159, 1, 39, 3.12], [6952, 1, 189, 3.79], [3430, 15, 69, 4.05], [20927, 1, 80, 2.66], [11954, 1, 203, 2.56], [7886, 4, 64, 2.38], [432, 3, 300, 5.53], [3429, 15, 53, 2.63], [11504, 2, 128, 2.78], [566, 2, 175, 2.7], [13928, 1, 49, 2.61], [11811, 1, 451, 3.72], [5584, 3, 229, 4.7], [114, 3, 241, 4.8], [2331, 1, 117, 4.57], [10407, 10, 1201, 4.0], [1492, 1, 37, 2.92], [105, 3, 201, 4.72], [7004, 1, 31, 3.0], [1490, 1, 48, 5.17], [11089, 1, 173, 2.5], [2703, 3, 300, 5.84], [6098, 80, 74, 4.31], [11674, 1, 205, 2.44], [1886, 2, 157, 2.61], [12348, 1, 560, 3.26], [10410, 10, 1201, 3.88], [94, 4, 116, 5.96], [3891, 1, 122, 6.0], [11953, 1, 203, 2.63], [6097, 80, 68, 5.21], [22317, 3, 318, 2.66], [9082, 3, 2453, 4.17]]</t>
+  </si>
+  <si>
+    <t>[[326, 2, 8, 2.27], [6935, 2, 17, 3.32], [2049, 3, 13, 0.72], [362, 2, 7, 1.69], [589, 2, 10, 0.77], [75, 2, 7, 0.75], [141, 2, 7, 2.25], [1776, 1, 9, 0.83], [205, 2, 7, 0.7], [8915, 2, 9, 0.75], [2778, 2, 7, 0.79], [8672, 2, 12, 1.12], [6936, 2, 10, 3.25], [593, 2, 11, 1.01], [7886, 4, 7, 1.04], [305, 2, 7, 0.96], [206, 2, 7, 0.72], [151, 1, 7, 0.87], [8648, 2, 7, 2.14], [1777, 1, 9, 1.98], [2328, 2, 7, 0.65], [88, 10, 14, 1.03], [11681, 2, 10, 4.17], [990, 2, 7, 1.06], [8650, 2, 7, 2.17], [412, 1, 7, 1.64], [5151, 2, 9, 2.35], [2050, 3, 7, 2.4], [76, 2, 9, 2.62], [144, 2, 7, 0.91], [345, 3, 10, 0.97], [10149, 3, 25, 4.03], [2991, 3, 7, 3.64], [22247, 2, 9, 1.34], [57, 1, 7, 0.7], [3478, 2, 7, 2.16], [146, 2, 7, 1.93], [7004, 1, 9, 0.71], [45, 2, 7, 2.94], [2054, 3, 6, 0.93], [143, 2, 6, 0.84], [417, 2, 7, 2.25], [413, 1, 7, 2.13], [21793, 1, 7, 0.83], [167, 3, 9, 0.97], [201, 3, 10, 0.7], [74, 1, 7, 3.37], [1446, 2, 7, 1.41], [346, 1, 9, 0.73], [2055, 3, 7, 0.94], [168, 3, 9, 1.11], [10, 2, 9, 1.61], [11234, 2, 9, 0.72], [7084, 3, 7, 0.69], [1429, 2, 7, 1.71], [7036, 1, 7, 3.47], [12721, 2, 10, 0.9], [3495, 3, 21, 0.95], [5081, 2, 7, 0.81], [8649, 2, 7, 2.48], [308, 1, 9, 2.22], [13028, 3, 7, 0.9], [10825, 21, 14, 2.47], [12870, 1, 7, 2.96], [79, 1, 7, 0.7], [1492, 1, 7, 1.98], [96, 11, 23, 0.81], [23, 1, 7, 1.24], [1006, 2, 7, 1.06], [3893, 1, 7, 1.48], [418, 2, 7, 0.79], [1504, 2, 7, 0.89], [145, 2, 7, 0.79], [5208, 3, 9, 1.57], [9827, 3, 7, 1.36], [3891, 1, 7, 0.98], [432, 3, 7, 0.75], [7005, 1, 7, 1.16], [94, 4, 7, 4.2], [1490, 1, 7, 1.46], [8853, 2, 11, 3.48], [13260, 29, 7, 0.77], [5812, 3, 8, 3.38], [416, 1, 7, 1.53], [8651, 2, 7, 1.54], [12353, 1, 7, 3.09], [20256, 2, 7, 0.92], [8939, 2, 7, 1.39], [21269, 3, 7, 4.99], [13280, 1, 7, 2.64], [12349, 1, 7, 3.22], [950, 1, 7, 0.98], [33, 1, 7, 1.02], [5086, 1, 7, 2.64], [998, 2, 7, 1.84], [12350, 1, 7, 3.09], [9069, 1, 7, 1.87], [1243, 2, 7, 1.64], [229, 1, 7, 2.92], [2878, 1, 6, 1.36], [140, 2, 7, 1.21], [2049, 1, 7, 0.69], [7567, 3, 7, 2.54], [20927, 1, 9, 0.66], [126, 2, 7, 2.22], [346, 3, 8, 0.74], [3980, 4, 7, 2.59], [1703, 2, 7, 1.51], [8274, 3, 7, 1.24], [9691, 1, 7, 2.1], [35, 1, 7, 0.89], [5209, 3, 9, 0.67], [1070, 7, 13, 1.16], [997, 2, 7, 1.98], [5584, 3, 7, 3.35], [11811, 1, 7, 1.83], [1519, 3, 17, 0.69], [11914, 1, 7, 1.42], [5660, 2, 7, 1.66], [856, 1, 7, 0.69], [8898, 3, 7, 4.68], [1091, 1, 7, 1.15], [5513, 2, 7, 0.8], [8926, 1, 7, 2.6], [523, 2, 7, 1.16], [11767, 1, 7, 0.88], [2775, 2, 7, 0.79], [9372, 1, 7, 2.03], [9081, 3, 12, 3.55], [13034, 3, 8, 3.38], [20255, 2, 7, 1.43], [307, 2, 7, 2.19], [11808, 1, 7, 1.16], [23, 1, 92, 2.51], [1006, 2, 189, 2.28], [3893, 1, 103, 2.25], [418, 2, 131, 1.94], [1504, 2, 170, 2.16], [145, 2, 139, 1.94], [5208, 3, 465, 2.33], [9827, 3, 72, 2.12], [3891, 1, 103, 2.25], [432, 3, 253, 2.02], [7005, 1, 65, 1.93], [94, 4, 99, 4.96], [1490, 1, 42, 2.23], [8853, 2, 235, 4.75], [13260, 29, 60, 2.0], [5812, 3, 543, 4.52], [416, 1, 79, 2.68], [8651, 2, 186, 2.73], [12353, 1, 557, 4.25], [20256, 2, 77, 2.19], [21269, 3, 270, 6.0], [13280, 1, 291, 3.8], [12349, 1, 557, 4.37], [950, 1, 55, 2.13], [33, 1, 92, 2.24], [5086, 1, 152, 3.41], [998, 2, 196, 2.61], [12350, 1, 557, 4.25], [9069, 1, 100, 2.12], [1243, 2, 90, 2.79], [229, 1, 75, 4.08], [2878, 1, 66, 2.63], [140, 2, 75, 2.75], [2049, 1, 18, 1.46], [7567, 3, 57, 3.31], [20927, 1, 65, 1.93], [126, 2, 75, 2.98], [346, 3, 525, 2.01], [3980, 4, 443, 3.74], [1703, 2, 149, 2.66], [8274, 3, 159, 2.0], [9691, 1, 62, 2.36], [35, 1, 103, 2.04], [5209, 3, 465, 1.95], [1070, 7, 494, 1.93], [997, 2, 196, 2.24], [5584, 3, 196, 3.55], [11811, 1, 416, 2.98], [1519, 3, 1545, 1.83], [11914, 1, 72, 2.19], [5660, 2, 144, 2.93], [856, 1, 32, 1.84], [8898, 3, 231, 5.05], [1091, 1, 39, 2.42], [5513, 2, 70, 1.95], [8926, 1, 50, 2.84], [523, 2, 143, 2.31], [11767, 1, 151, 2.03], [2775, 2, 130, 2.06], [9372, 1, 210, 3.18], [9081, 3, 379, 4.81], [13034, 3, 486, 4.14], [20255, 2, 77, 2.2], [307, 2, 122, 2.45], [11808, 1, 402, 1.93]]</t>
+  </si>
+  <si>
+    <t>[[88, 10, 16, 1.96], [2327, 2, 7, 1.0], [8915, 2, 8, 1.9], [589, 2, 8, 0.99], [2778, 2, 9, 0.94], [6935, 2, 11, 4.09], [2328, 2, 7, 1.12], [5493, 2, 7, 2.27], [130, 1, 9, 2.43], [305, 2, 6, 0.82], [615, 2, 9, 0.87], [616, 2, 9, 0.66], [6936, 2, 7, 3.42], [326, 2, 7, 2.62], [8650, 2, 7, 1.47], [8648, 2, 7, 2.02], [1446, 2, 7, 1.22], [2049, 3, 10, 0.87], [10, 2, 9, 0.67], [143, 2, 7, 1.55], [159, 3, 8, 1.18], [593, 2, 9, 0.88], [205, 2, 7, 0.83], [5491, 2, 7, 1.12], [2775, 2, 9, 0.94], [7036, 1, 7, 2.3], [144, 2, 7, 3.22], [3840, 1, 7, 1.09], [151, 1, 7, 1.38], [94, 4, 7, 3.68], [434, 2, 9, 0.71], [8938, 2, 7, 0.95], [990, 2, 7, 1.21], [3893, 1, 9, 0.98], [146, 2, 7, 2.06], [8853, 2, 7, 3.51], [1504, 2, 7, 1.79], [12224, 1, 7, 0.84], [624, 2, 7, 2.19], [1429, 2, 7, 0.91], [3891, 1, 7, 0.98], [2776, 2, 7, 1.18], [206, 2, 7, 0.74], [2055, 3, 7, 0.84], [362, 2, 7, 0.96], [141, 2, 7, 1.21], [2057, 3, 7, 0.84], [75, 2, 7, 0.75], [11681, 2, 11, 3.45], [11404, 2, 9, 0.94], [5208, 3, 9, 0.78], [8649, 2, 7, 3.15], [3889, 1, 7, 0.65], [1007, 2, 7, 0.85], [10574, 3, 11, 4.5], [11234, 2, 7, 1.8], [10993, 2, 7, 1.29], [7886, 4, 7, 0.85], [12870, 1, 7, 1.83], [21793, 1, 7, 0.96], [10149, 3, 21, 2.43], [3980, 4, 6, 2.43], [2050, 3, 7, 0.84], [12353, 1, 7, 1.22], [145, 2, 7, 1.94], [7084, 3, 7, 1.58], [11811, 1, 7, 0.8], [8672, 2, 9, 3.66], [20927, 1, 7, 1.83], [998, 2, 7, 2.83], [9760, 29, 7, 0.71], [997, 2, 7, 2.64], [2436, 4, 9, 0.85], [1006, 2, 7, 0.99], [1886, 2, 9, 0.82], [972, 3, 8, 0.89], [2424, 80, 7, 1.91], [3, 2, 7, 1.14], [346, 3, 7, 1.21], [229, 1, 7, 0.86], [6158, 2, 7, 1.38], [3495, 3, 14, 0.98], [12346, 1, 7, 1.22], [5076, 1, 7, 1.3], [7887, 4, 7, 1.42], [12345, 1, 7, 1.22], [20252, 2, 7, 1.43], [126, 2, 7, 2.34], [11953, 1, 7, 0.84], [74, 1, 7, 3.79], [9372, 1, 7, 3.48], [11770, 1, 7, 2.76], [140, 2, 7, 2.34], [12344, 1, 7, 1.22], [8939, 2, 7, 0.92], [11954, 1, 7, 0.7], [11685, 2, 11, 3.45], [1492, 1, 7, 0.95], [12352, 1, 7, 1.22], [996, 2, 7, 2.83], [12721, 2, 7, 4.25], [2774, 2, 7, 1.15], [20256, 2, 9, 0.82], [12350, 1, 7, 1.22], [3981, 3, 22, 1.14], [9081, 3, 12, 0.86], [9491, 21, 21, 0.8], [5434, 1, 7, 1.93], [2423, 80, 7, 1.88], [6497, 1, 7, 3.31], [12343, 1, 7, 1.22], [12229, 2, 7, 0.9], [5584, 3, 7, 3.37], [2438, 2, 8, 1.33], [10388, 2, 7, 1.93], [12351, 1, 7, 1.22], [10407, 10, 10, 3.59], [11179, 1, 7, 1.6], [6496, 1, 7, 3.71], [22317, 3, 7, 1.11], [7573, 1, 22, 5.0], [823, 1, 7, 1.9], [5209, 3, 7, 1.38], [3900, 3, 7, 3.39], [2805, 137, 7, 2.91], [8898, 3, 7, 3.35], [12526, 2, 7, 2.21], [11812, 1, 7, 0.87], [2424, 29, 7, 1.0], [3975, 4, 7, 2.86], [4253, 1, 7, 1.04], [11490, 1, 7, 0.65], [336, 15, 7, 1.79], [9760, 29, 63, 2.66], [997, 2, 232, 4.28], [2436, 4, 101, 2.98], [1006, 2, 200, 2.97], [1886, 2, 136, 2.8], [972, 3, 522, 2.82], [2424, 80, 152, 2.99], [3, 2, 118, 2.78], [346, 3, 557, 2.68], [229, 1, 81, 2.5], [6158, 2, 224, 2.86], [3495, 3, 844, 2.98], [12346, 1, 612, 2.87], [5076, 1, 127, 2.94], [7887, 4, 68, 2.73], [12345, 1, 612, 2.87], [20252, 2, 91, 3.07], [126, 2, 86, 3.98], [11953, 1, 195, 2.48], [74, 1, 171, 4.87], [9372, 1, 224, 5.12], [11770, 1, 206, 4.4], [140, 2, 86, 3.98], [12344, 1, 612, 2.87], [8939, 2, 169, 2.9], [11954, 1, 195, 2.34], [11685, 2, 234, 5.43], [1492, 1, 32, 2.93], [12352, 1, 612, 2.87], [996, 2, 208, 4.81], [12721, 2, 272, 5.89], [2774, 2, 200, 2.79], [20256, 2, 81, 2.94], [12350, 1, 612, 2.87], [3981, 3, 1471, 3.14], [9081, 3, 473, 2.5], [9491, 21, 1872, 2.76], [5434, 1, 42, 2.89], [2423, 80, 164, 3.36], [6497, 1, 35, 4.95], [12343, 1, 612, 2.87], [12229, 2, 133, 2.84], [5584, 3, 206, 4.28], [2438, 2, 553, 2.82], [10388, 2, 211, 3.56], [12351, 1, 612, 2.87], [10407, 10, 645, 5.06], [11179, 1, 85, 3.24], [6496, 1, 38, 5.36], [22317, 3, 308, 2.75], [7573, 1, 336, 6.0], [823, 1, 39, 3.54], [5209, 3, 493, 2.87], [3900, 3, 37, 4.29], [2805, 137, 175, 4.54], [8898, 3, 257, 4.83], [12526, 2, 135, 3.53], [11812, 1, 209, 2.85], [2424, 29, 34, 2.65], [3975, 4, 186, 4.34], [4253, 1, 149, 2.97], [11490, 1, 106, 2.29], [336, 15, 110, 3.43]]</t>
+  </si>
+  <si>
+    <t>[[6935, 2, 15, 3.35], [141, 2, 7, 1.02], [589, 2, 10, 0.69], [2778, 2, 9, 1.18], [6936, 2, 13, 3.74], [8648, 2, 7, 2.18], [362, 2, 7, 0.89], [2327, 2, 7, 1.82], [11681, 2, 22, 3.47], [8650, 2, 7, 2.04], [326, 2, 7, 1.42], [205, 2, 7, 1.04], [2328, 2, 9, 1.41], [1446, 2, 9, 1.08], [305, 2, 7, 2.13], [130, 1, 7, 0.87], [8649, 2, 9, 2.02], [2775, 2, 7, 1.18], [8853, 2, 11, 3.24], [361, 2, 7, 0.96], [2776, 2, 7, 1.18], [593, 2, 7, 1.38], [143, 2, 7, 2.18], [140, 2, 7, 1.42], [1429, 2, 9, 1.24], [206, 2, 9, 0.75], [5493, 2, 7, 0.87], [523, 2, 7, 1.0], [7004, 1, 7, 1.3], [413, 1, 7, 1.96], [7036, 1, 7, 3.04], [5491, 2, 7, 0.92], [412, 1, 7, 1.25], [21793, 1, 7, 3.65], [12350, 1, 7, 0.7], [151, 1, 7, 0.91], [1124, 2, 7, 1.27], [990, 2, 7, 0.82], [12353, 1, 7, 1.26], [5165, 1, 9, 2.64], [8915, 2, 8, 1.49], [615, 2, 7, 2.25], [583, 2, 7, 1.42], [417, 2, 7, 0.83], [21798, 1, 7, 0.95], [146, 2, 7, 2.92], [248, 1, 9, 0.68], [434, 2, 9, 0.79], [201, 3, 7, 1.37], [142, 2, 7, 0.92], [6097, 80, 9, 3.4], [11770, 1, 7, 0.8], [6952, 1, 7, 3.29], [2055, 3, 7, 1.5], [345, 3, 7, 0.9], [3891, 1, 7, 1.8], [9372, 1, 7, 1.55], [2057, 3, 7, 1.5], [616, 2, 7, 1.58], [7084, 3, 7, 2.33], [3670, 2, 7, 2.71], [3893, 1, 7, 1.8], [5165, 2, 12, 3.15], [12346, 1, 7, 0.7], [12870, 1, 7, 2.21], [12343, 1, 7, 0.89], [10574, 3, 8, 2.44], [1886, 2, 7, 0.66], [2424, 80, 7, 2.28], [346, 3, 7, 0.72], [3334, 5, 7, 3.63], [20927, 1, 7, 0.95], [12351, 1, 7, 0.7], [7885, 4, 7, 0.9], [6098, 80, 7, 2.81], [6097, 29, 7, 3.9], [11089, 1, 7, 0.8], [12345, 1, 7, 0.85], [10149, 3, 21, 1.91], [20256, 2, 7, 0.87], [147, 1, 7, 2.36], [22316, 3, 7, 0.66], [1492, 1, 9, 1.48], [11953, 1, 7, 0.81], [432, 3, 7, 1.65], [11491, 2, 7, 0.94], [20252, 2, 7, 0.85], [4032, 29, 7, 0.9], [418, 2, 7, 1.68], [1490, 1, 7, 0.76], [1519, 3, 16, 0.69], [2423, 80, 7, 3.06], [11952, 1, 7, 0.85], [411, 2, 7, 0.96], [12304, 1, 7, 0.92], [5151, 2, 7, 1.13], [229, 1, 7, 3.82], [11769, 1, 7, 0.88], [3576, 25, 7, 1.68], [972, 3, 9, 0.93], [2331, 1, 7, 2.67], [346, 1, 7, 0.7], [995, 2, 7, 2.14], [416, 1, 7, 1.91], [13034, 3, 7, 3.52], [2424, 29, 7, 2.13], [11426, 25, 7, 1.07], [3, 2, 7, 1.01], [11737, 2, 7, 0.91], [5076, 1, 7, 1.17], [11767, 1, 7, 0.88], [439, 1, 7, 3.23], [11490, 1, 7, 1.08], [2805, 137, 7, 1.99], [2160, 68, 7, 2.19], [6494, 1, 7, 3.12], [950, 1, 7, 0.76], [414, 1, 7, 1.47], [3575, 25, 7, 1.81], [12764, 2, 8, 0.87], [1701, 2, 7, 3.79], [11180, 1, 7, 1.04], [8677, 3, 8, 1.86], [75, 2, 7, 1.94], [11586, 1, 14, 3.12], [3577, 25, 7, 0.77], [3478, 2, 7, 1.65], [11585, 29, 7, 2.06], [11813, 1, 7, 3.17], [13023, 3, 8, 2.24], [9998, 80, 9, 2.71], [2438, 2, 8, 1.84], [12526, 2, 9, 3.05], [2424, 80, 146, 3.69], [346, 3, 493, 2.39], [3334, 5, 138, 4.81], [20927, 1, 68, 2.36], [12351, 1, 536, 2.13], [7885, 4, 120, 2.31], [6098, 80, 59, 3.45], [6097, 29, 27, 5.08], [11089, 1, 148, 2.22], [12345, 1, 536, 2.28], [10149, 3, 666, 3.62], [20256, 2, 72, 2.55], [147, 1, 77, 3.78], [22316, 3, 272, 2.08], [1492, 1, 28, 3.66], [11953, 1, 172, 2.22], [432, 3, 236, 2.82], [11491, 2, 121, 2.36], [20252, 2, 72, 2.53], [4032, 29, 73, 2.55], [418, 2, 121, 3.09], [1490, 1, 44, 2.18], [1519, 3, 864, 1.89], [2423, 80, 155, 4.47], [11952, 1, 172, 2.27], [411, 2, 84, 2.61], [12304, 1, 87, 2.6], [5151, 2, 21, 2.55], [229, 1, 70, 5.24], [11769, 1, 140, 2.3], [3576, 25, 87, 3.09], [972, 3, 458, 2.55], [2331, 1, 100, 4.08], [346, 1, 123, 2.39], [995, 2, 206, 3.55], [416, 1, 66, 2.59], [13034, 3, 507, 4.92], [2424, 29, 29, 3.54], [11426, 25, 103, 2.49], [3, 2, 105, 2.43], [11737, 2, 49, 2.33], [5076, 1, 112, 2.58], [11767, 1, 140, 2.3], [439, 1, 74, 4.65], [11490, 1, 84, 2.71], [2805, 137, 154, 3.41], [2160, 68, 112, 3.61], [6494, 1, 42, 4.54], [950, 1, 51, 2.18], [414, 1, 74, 2.89], [3575, 25, 87, 3.22], [12764, 2, 646, 2.28], [1701, 2, 126, 4.58], [11180, 1, 67, 2.67], [8677, 3, 253, 3.28], [75, 2, 124, 3.36], [11586, 1, 296, 3.61], [3577, 25, 76, 2.18], [3478, 2, 65, 3.07], [11585, 29, 148, 3.47], [11813, 1, 266, 4.58], [13023, 3, 509, 3.66], [2438, 2, 551, 3.26]]</t>
+  </si>
+  <si>
+    <t>[[6935, 2, 12, 4.2], [615, 2, 7, 3.33], [2778, 2, 9, 1.07], [305, 2, 7, 0.92], [5493, 2, 7, 2.99], [6936, 2, 11, 4.22], [130, 1, 7, 1.87], [205, 2, 7, 1.02], [616, 2, 7, 2.96], [1504, 2, 7, 1.54], [144, 2, 9, 2.7], [8648, 2, 7, 1.35], [2049, 3, 17, 0.83], [88, 10, 18, 1.22], [8915, 2, 8, 3.38], [326, 2, 7, 2.16], [7036, 1, 7, 3.02], [8650, 2, 7, 1.54], [593, 2, 9, 1.07], [2327, 2, 7, 0.86], [11681, 2, 7, 3.3], [8853, 2, 9, 4.23], [141, 2, 9, 1.19], [2775, 2, 9, 1.07], [206, 2, 9, 0.85], [151, 1, 7, 1.25], [7004, 1, 7, 1.15], [248, 1, 7, 0.8], [11685, 2, 7, 3.69], [3840, 1, 7, 0.72], [3891, 1, 7, 1.68], [2328, 2, 7, 0.96], [2050, 3, 7, 0.64], [5491, 2, 7, 1.61], [2497, 2, 7, 2.68], [2055, 3, 7, 3.44], [143, 2, 7, 1.12], [434, 2, 7, 0.86], [3980, 4, 7, 2.36], [990, 2, 9, 0.88], [2054, 3, 7, 0.67], [624, 2, 7, 3.92], [8649, 2, 7, 2.8], [362, 2, 7, 1.64], [2776, 2, 9, 1.66], [12870, 1, 7, 3.71], [2057, 3, 7, 0.64], [12350, 1, 7, 1.22], [7886, 4, 7, 1.32], [10574, 3, 8, 3.28], [5165, 1, 7, 2.53], [1006, 2, 7, 1.38], [1446, 2, 7, 0.91], [3495, 3, 21, 1.48], [94, 4, 9, 3.04], [75, 2, 7, 2.87], [523, 2, 7, 1.93], [7084, 3, 7, 1.12], [2991, 3, 7, 4.28], [7005, 1, 7, 1.73], [10149, 3, 21, 1.48], [3975, 4, 7, 2.49], [21793, 1, 7, 4.43], [9760, 29, 7, 0.8], [11404, 2, 7, 1.67], [142, 2, 7, 0.94], [12346, 1, 7, 1.22], [6158, 2, 7, 1.33], [20927, 1, 7, 1.77], [3981, 3, 22, 2.03], [5165, 2, 10, 2.64], [417, 2, 7, 0.98], [2912, 1, 7, 0.8], [3982, 3, 17, 2.34], [8939, 2, 7, 0.89], [1007, 2, 7, 0.98], [11953, 1, 7, 0.96], [2774, 2, 7, 1.95], [33, 1, 7, 2.04], [956, 2, 7, 0.86], [11772, 1, 7, 2.97], [286, 3, 7, 2.44], [1492, 1, 7, 2.27], [11767, 1, 7, 0.81], [336, 15, 7, 2.22], [972, 3, 7, 2.05], [11769, 1, 7, 1.46], [11490, 1, 7, 2.0], [11770, 1, 7, 1.8], [410, 1, 7, 1.49], [74, 1, 7, 2.13], [2912, 2, 8, 0.79], [389, 4, 7, 2.13], [6496, 1, 7, 0.85], [35, 1, 7, 1.54], [7567, 3, 7, 2.62], [411, 2, 7, 1.93], [12721, 2, 7, 1.91], [1413, 15, 7, 1.04], [4253, 1, 7, 1.5], [22317, 3, 7, 0.92], [140, 2, 7, 1.7], [8673, 2, 7, 2.48], [8121, 3, 6, 0.85], [1126, 2, 7, 1.26], [4176, 4, 9, 3.25], [2436, 4, 9, 0.73], [9372, 1, 7, 3.34], [21269, 3, 7, 4.87], [8676, 2, 7, 3.11], [8677, 3, 7, 1.51], [22247, 2, 7, 2.66], [10388, 2, 7, 2.13], [10936, 2, 7, 3.12], [12343, 1, 7, 1.22], [11085, 2, 8, 3.16], [12526, 2, 7, 2.15], [9784, 1, 7, 0.9], [1274, 1, 9, 1.03], [6494, 1, 7, 2.34], [12269, 2, 7, 1.9], [37, 1, 7, 1.7], [13023, 3, 7, 2.32], [1429, 2, 7, 0.91], [345, 3, 7, 2.52], [7573, 1, 9, 2.67], [12225, 1, 7, 2.51], [12271, 2, 7, 1.86], [3, 2, 7, 0.7], [96, 11, 22, 1.1], [3577, 25, 7, 0.92], [9, 1, 7, 0.66], [10408, 10, 9, 3.19], [6158, 2, 204, 2.54], [20927, 1, 68, 3.22], [3981, 3, 1251, 3.73], [5165, 2, 163, 4.85], [417, 2, 133, 2.43], [2912, 1, 38, 1.51], [3982, 3, 612, 4.03], [8939, 2, 150, 2.61], [1007, 2, 207, 2.65], [11953, 1, 175, 2.42], [2774, 2, 174, 3.4], [33, 1, 86, 2.74], [956, 2, 93, 2.32], [11772, 1, 170, 4.18], [286, 3, 108, 3.65], [1492, 1, 28, 3.97], [11767, 1, 125, 2.52], [336, 15, 96, 3.67], [972, 3, 459, 2.73], [11769, 1, 125, 3.17], [11490, 1, 48, 2.71], [11770, 1, 170, 3.51], [410, 1, 46, 2.7], [74, 1, 176, 3.58], [2912, 2, 342, 2.25], [389, 4, 162, 3.34], [6496, 1, 35, 2.31], [35, 1, 86, 2.75], [7567, 3, 54, 3.83], [411, 2, 48, 2.73], [12721, 2, 218, 3.11], [1413, 15, 77, 2.75], [4253, 1, 145, 2.95], [22317, 3, 273, 2.38], [140, 2, 78, 3.15], [8673, 2, 240, 3.93], [8121, 3, 228, 2.56], [1126, 2, 197, 2.71], [4176, 4, 374, 4.3], [2436, 4, 89, 2.5], [9372, 1, 196, 4.79], [21269, 3, 254, 6.0], [8676, 2, 245, 4.57], [8677, 3, 229, 2.72], [22247, 2, 218, 3.32], [10388, 2, 186, 3.58], [10936, 2, 115, 4.58], [12343, 1, 543, 2.67], [11085, 2, 414, 4.36], [12526, 2, 235, 3.6], [9784, 1, 56, 2.57], [1274, 1, 63, 3.06], [6494, 1, 23, 3.55], [12269, 2, 55, 3.35], [37, 1, 96, 3.15], [13023, 3, 507, 3.78], [1429, 2, 131, 2.36], [345, 3, 230, 3.19], [7573, 1, 259, 3.67], [12225, 1, 141, 3.96], [12271, 2, 55, 3.31], [3, 2, 106, 2.15], [96, 11, 661, 2.81], [3577, 25, 68, 2.59], [9, 1, 30, 2.11]]</t>
+  </si>
+  <si>
+    <t>[[6935, 2, 23, 4.99], [305, 2, 7, 1.02], [2328, 2, 7, 1.5], [130, 1, 7, 0.78], [141, 2, 9, 0.74], [2778, 2, 13, 1.27], [8650, 2, 9, 2.77], [5491, 2, 7, 2.52], [2327, 2, 7, 1.21], [8672, 2, 12, 1.53], [6936, 2, 9, 3.46], [143, 2, 7, 4.32], [11681, 2, 13, 3.96], [248, 1, 7, 0.85], [145, 2, 7, 0.77], [205, 2, 7, 1.02], [5493, 2, 7, 2.44], [146, 2, 7, 1.08], [417, 2, 7, 1.0], [589, 2, 9, 0.74], [75, 2, 7, 1.63], [11737, 2, 7, 1.18], [11838, 2, 7, 1.04], [1124, 2, 12, 0.72], [523, 2, 9, 0.96], [8648, 2, 7, 2.96], [8853, 2, 7, 2.71], [12721, 2, 9, 1.59], [615, 2, 7, 2.35], [1005, 2, 7, 1.22], [326, 2, 7, 2.21], [206, 2, 7, 1.21], [8915, 2, 9, 0.71], [8673, 2, 9, 2.44], [144, 2, 7, 1.3], [11739, 2, 7, 1.18], [88, 10, 14, 1.5], [434, 2, 7, 1.44], [2776, 2, 9, 1.21], [142, 2, 7, 1.05], [151, 1, 7, 1.38], [8676, 2, 7, 0.9], [6158, 2, 10, 0.73], [2424, 29, 9, 0.85], [8649, 2, 7, 2.29], [2423, 29, 7, 3.48], [11738, 2, 7, 1.18], [2497, 2, 7, 1.06], [7704, 2, 7, 2.08], [2424, 80, 9, 1.21], [1413, 15, 7, 2.34], [10574, 3, 9, 3.0], [2423, 80, 7, 3.37], [3670, 2, 7, 3.77], [11836, 2, 9, 0.79], [7705, 2, 7, 2.08], [2054, 3, 7, 2.1], [3, 2, 7, 0.83], [2859, 15, 7, 2.41], [412, 1, 9, 1.44], [378, 2, 7, 4.55], [7706, 2, 7, 2.08], [12720, 2, 7, 1.89], [22316, 3, 7, 0.85], [2055, 3, 7, 0.88], [12344, 1, 7, 0.88], [10149, 3, 21, 2.21], [3478, 2, 9, 2.65], [74, 1, 7, 3.39], [3429, 15, 7, 0.85], [307, 2, 7, 2.95], [2774, 2, 7, 1.06], [6497, 1, 7, 0.8], [60, 3, 8, 1.99], [12526, 2, 7, 2.76], [7004, 1, 7, 1.96], [418, 2, 7, 1.49], [13928, 1, 7, 0.74], [411, 2, 7, 0.91], [11089, 1, 7, 0.71], [2057, 3, 7, 2.1], [413, 1, 9, 1.34], [11844, 2, 7, 1.79], [14037, 3, 7, 1.85], [7036, 1, 7, 1.74], [20252, 2, 7, 1.06], [2050, 3, 7, 2.1], [3893, 1, 7, 1.3], [13260, 29, 7, 1.29], [8274, 3, 7, 1.68], [6097, 80, 7, 3.38], [6952, 1, 7, 2.01], [3891, 1, 7, 3.83], [94, 4, 7, 2.5], [159, 3, 9, 1.37], [9784, 1, 7, 2.37], [1050, 2, 7, 0.66], [6494, 1, 7, 0.85], [7707, 2, 7, 1.32], [1490, 1, 7, 1.88], [11490, 1, 7, 0.86], [1413, 16, 7, 0.71], [414, 1, 9, 1.63], [7708, 2, 7, 2.28], [1243, 2, 7, 1.32], [3889, 1, 7, 1.17], [1492, 1, 7, 1.13], [565, 2, 7, 0.84], [5208, 3, 9, 1.82], [22317, 3, 8, 0.88], [7703, 2, 7, 2.28], [11491, 2, 7, 1.5], [21793, 1, 7, 1.83], [3495, 3, 21, 1.51], [229, 1, 7, 3.68], [345, 3, 7, 2.32], [410, 1, 7, 0.74], [2422, 80, 9, 4.33], [11504, 2, 7, 1.33], [6098, 80, 7, 2.19], [149, 2, 7, 2.73], [947, 15, 7, 0.71], [6630, 3, 7, 3.21], [3430, 15, 7, 2.26], [147, 1, 7, 2.73], [3674, 2, 7, 0.96], [416, 1, 7, 2.93], [2805, 137, 11, 3.57], [2331, 1, 7, 1.34], [247, 1, 7, 2.33], [9126, 1, 7, 0.87], [6098, 29, 7, 2.55], [8635, 3, 7, 1.71], [307, 2, 82, 5.06], [2774, 2, 184, 3.11], [6497, 1, 38, 2.59], [60, 3, 730, 4.08], [12526, 2, 245, 4.87], [7004, 1, 31, 3.07], [418, 2, 141, 3.27], [13928, 1, 44, 2.85], [411, 2, 109, 2.7], [11089, 1, 173, 2.5], [2057, 3, 473, 3.89], [413, 1, 76, 3.1], [7036, 1, 128, 3.53], [20252, 2, 92, 2.85], [2050, 3, 473, 3.89], [3893, 1, 110, 2.9], [13260, 29, 65, 3.33], [8274, 3, 115, 2.76], [6097, 80, 61, 5.49], [6952, 1, 189, 3.79], [3891, 1, 123, 5.62], [94, 4, 104, 4.11], [159, 3, 709, 3.16], [9784, 1, 71, 4.16], [6494, 1, 52, 2.64], [7707, 2, 176, 3.11], [1490, 1, 50, 3.67], [11490, 1, 109, 2.65], [1413, 16, 50, 2.5], [414, 1, 76, 3.31], [7708, 2, 176, 4.07], [1243, 2, 90, 2.93], [3889, 1, 110, 2.78], [1492, 1, 37, 2.92], [565, 2, 176, 2.63], [5208, 3, 558, 3.6], [22317, 3, 318, 2.66], [7703, 2, 176, 4.07], [11491, 2, 141, 3.28], [21793, 1, 214, 2.94], [3495, 3, 965, 3.31], [229, 1, 81, 5.47], [345, 3, 297, 4.1], [410, 1, 53, 2.17], [2422, 80, 168, 5.46], [11504, 2, 141, 3.12], [6098, 80, 66, 4.03], [149, 2, 87, 4.52], [947, 15, 41, 2.5], [6630, 3, 93, 5.0], [3430, 15, 69, 4.05], [147, 1, 87, 4.52], [3674, 2, 260, 2.74], [416, 1, 85, 4.71], [2805, 137, 182, 5.36], [2331, 1, 118, 3.13], [247, 1, 87, 4.12], [9126, 1, 71, 2.65], [6098, 29, 37, 4.34], [8635, 3, 115, 2.78]]</t>
+  </si>
+  <si>
+    <t>[[8672, 2, 12, 2.94], [305, 2, 7, 1.95], [3, 2, 9, 2.18], [6935, 2, 18, 3.39], [205, 2, 7, 1.36], [143, 2, 7, 3.11], [144, 2, 9, 3.22], [75, 2, 7, 0.9], [12721, 2, 10, 1.03], [145, 2, 9, 2.81], [8915, 2, 12, 0.71], [2778, 2, 9, 0.96], [1776, 1, 7, 0.87], [146, 2, 9, 3.31], [206, 2, 7, 1.02], [20252, 2, 7, 0.88], [6936, 2, 10, 2.86], [1777, 1, 9, 2.87], [8648, 2, 7, 1.71], [151, 1, 7, 0.67], [2328, 2, 7, 1.41], [8650, 2, 9, 2.48], [5151, 2, 7, 3.43], [2050, 3, 7, 2.04], [248, 1, 7, 0.8], [88, 10, 21, 3.14], [7886, 4, 7, 1.22], [9507, 3, 7, 0.66], [74, 1, 7, 1.54], [1446, 2, 7, 1.51], [2991, 3, 7, 3.64], [362, 2, 7, 0.83], [7004, 1, 7, 1.29], [2057, 3, 7, 0.87], [1492, 1, 9, 1.36], [1007, 2, 12, 0.69], [2055, 3, 7, 1.04], [147, 1, 7, 4.17], [76, 2, 7, 1.42], [8649, 2, 9, 2.6], [3889, 1, 7, 0.81], [11234, 2, 11, 0.93], [410, 1, 7, 0.7], [7005, 1, 7, 0.7], [345, 3, 7, 0.9], [10, 2, 9, 1.21], [1429, 2, 7, 1.46], [307, 2, 7, 3.37], [10825, 21, 13, 1.0], [5081, 2, 7, 1.04], [12870, 1, 7, 1.25], [57, 1, 7, 0.8], [10149, 3, 21, 1.27], [7036, 1, 7, 1.81], [3478, 2, 7, 1.0], [7084, 3, 7, 1.67], [1006, 2, 7, 1.53], [1504, 2, 9, 1.0], [3891, 1, 7, 1.71], [21793, 1, 7, 3.43], [94, 4, 7, 3.56], [167, 3, 7, 1.44], [411, 2, 7, 0.9], [9827, 3, 7, 1.38], [3893, 1, 7, 0.65], [79, 1, 7, 1.08], [33, 1, 9, 1.88], [432, 3, 9, 1.23], [8677, 3, 9, 1.51], [11681, 2, 11, 3.45], [148, 1, 7, 3.1], [96, 11, 24, 0.67], [1490, 1, 9, 0.82], [12225, 1, 7, 1.7], [1124, 2, 11, 0.74], [11737, 2, 7, 1.26], [1243, 2, 7, 0.92], [22247, 2, 11, 1.79], [6158, 2, 8, 1.39], [5812, 3, 8, 3.52], [8853, 2, 11, 3.19], [201, 3, 7, 0.9], [412, 1, 7, 2.46], [9760, 29, 9, 1.04], [10574, 3, 9, 2.6], [8651, 2, 7, 1.13], [20927, 1, 7, 0.83], [5208, 3, 11, 1.25], [8676, 2, 12, 1.23], [229, 1, 7, 2.31], [1767, 25, 7, 1.14], [25, 1, 7, 1.4], [45, 2, 7, 2.7], [9069, 1, 7, 0.79], [413, 1, 7, 2.29], [11490, 1, 7, 0.69], [149, 2, 7, 3.27], [159, 3, 9, 1.18], [3495, 3, 21, 1.61], [21269, 3, 7, 2.34], [998, 2, 7, 1.87], [140, 2, 7, 1.5], [95, 3, 17, 3.57], [3980, 4, 7, 2.46], [950, 1, 7, 1.3], [5946, 1, 7, 1.83], [9372, 1, 7, 3.91], [1126, 2, 7, 1.36], [1766, 25, 7, 1.08], [2775, 2, 7, 1.46], [1413, 15, 9, 1.85], [490, 1, 9, 0.99], [506, 1, 7, 4.76], [8674, 2, 7, 0.99], [11489, 1, 7, 1.21], [8898, 3, 7, 3.23], [997, 2, 7, 3.34], [3670, 2, 7, 3.6], [1070, 7, 15, 0.85], [9691, 1, 7, 1.89], [107, 2, 7, 1.46], [974, 3, 7, 1.64], [20498, 1, 7, 1.81], [11954, 1, 7, 0.87], [14037, 3, 7, 0.8], [14017, 3, 9, 1.09], [823, 1, 7, 1.62], [34, 1, 7, 2.43], [5209, 3, 7, 0.98], [972, 3, 8, 1.49], [9784, 1, 7, 1.51], [11739, 2, 7, 1.26], [1091, 1, 7, 1.18], [432, 3, 234, 2.81], [8677, 3, 226, 2.67], [11681, 2, 206, 5.11], [148, 1, 66, 4.77], [96, 11, 651, 2.32], [1490, 1, 38, 2.48], [12225, 1, 71, 2.57], [1124, 2, 143, 2.7], [11737, 2, 32, 2.92], [1243, 2, 83, 2.22], [22247, 2, 216, 3.38], [6158, 2, 221, 2.69], [5812, 3, 502, 4.82], [8853, 2, 216, 4.71], [201, 3, 226, 2.53], [412, 1, 63, 3.1], [9760, 29, 54, 3.01], [10574, 3, 382, 4.26], [8651, 2, 171, 2.79], [20927, 1, 61, 2.46], [5208, 3, 480, 2.56], [8676, 2, 217, 2.65], [229, 1, 63, 2.95], [1767, 25, 132, 2.76], [25, 1, 95, 2.71], [45, 2, 82, 4.36], [9069, 1, 93, 2.41], [413, 1, 65, 2.94], [11490, 1, 83, 2.32], [149, 2, 66, 4.03], [159, 3, 602, 2.48], [3495, 3, 737, 3.28], [21269, 3, 225, 3.5], [998, 2, 181, 2.54], [140, 2, 69, 3.09], [95, 3, 892, 4.89], [3980, 4, 368, 4.11], [950, 1, 25, 2.17], [5946, 1, 95, 2.48], [9372, 1, 173, 4.69], [1126, 2, 175, 2.52], [1766, 25, 144, 2.69], [2775, 2, 119, 2.63], [1413, 15, 53, 4.01], [490, 1, 45, 2.39], [506, 1, 74, 6.0], [8674, 2, 217, 2.66], [11489, 1, 83, 2.87], [8898, 3, 225, 4.39], [997, 2, 202, 4.64], [3670, 2, 180, 4.37], [1070, 7, 453, 2.51], [9691, 1, 57, 2.54], [107, 2, 31, 2.12], [974, 3, 113, 2.8], [20498, 1, 74, 3.4], [11954, 1, 171, 2.17], [14037, 3, 125, 2.18], [14017, 3, 149, 2.47], [823, 1, 30, 3.2], [34, 1, 85, 3.19], [5209, 3, 480, 2.29], [972, 3, 453, 2.26], [9784, 1, 55, 2.67], [11739, 2, 32, 2.92], [1091, 1, 41, 2.48]]</t>
+  </si>
+  <si>
+    <t>[[8672, 2, 10, 1.01], [305, 2, 7, 1.1], [2049, 3, 13, 0.7], [6935, 2, 21, 3.58], [326, 2, 8, 2.27], [141, 2, 7, 2.25], [144, 2, 7, 1.17], [589, 2, 12, 0.77], [151, 1, 7, 0.92], [362, 2, 9, 0.83], [12721, 2, 10, 1.03], [146, 2, 7, 1.26], [1776, 1, 7, 2.19], [145, 2, 7, 0.8], [206, 2, 7, 0.69], [2328, 2, 7, 1.35], [8915, 2, 11, 0.71], [143, 2, 7, 1.12], [990, 2, 9, 1.06], [6936, 2, 10, 3.41], [20252, 2, 7, 0.91], [8650, 2, 7, 2.27], [1777, 1, 7, 2.96], [1007, 2, 10, 0.81], [2778, 2, 7, 0.79], [248, 1, 7, 0.68], [88, 10, 14, 2.0], [22247, 2, 9, 1.93], [2050, 3, 7, 0.69], [76, 2, 7, 2.39], [8649, 2, 7, 2.74], [10149, 3, 25, 3.53], [10, 2, 11, 1.65], [8677, 3, 8, 3.58], [2054, 3, 7, 4.0], [412, 1, 7, 1.64], [2055, 3, 7, 4.0], [13028, 3, 7, 1.38], [413, 1, 7, 2.12], [7004, 1, 9, 0.89], [411, 2, 7, 0.88], [10825, 21, 14, 2.34], [11681, 2, 10, 4.26], [1446, 2, 7, 1.91], [7084, 3, 7, 1.66], [307, 2, 7, 1.35], [3478, 2, 7, 2.16], [1429, 2, 7, 1.21], [3495, 3, 26, 1.77], [1006, 2, 7, 1.36], [147, 1, 7, 2.73], [1492, 1, 6, 1.98], [5081, 2, 7, 0.81], [140, 2, 7, 1.98], [167, 3, 9, 1.86], [7005, 1, 9, 0.89], [7036, 1, 7, 1.62], [9827, 3, 7, 1.38], [45, 2, 7, 2.95], [8676, 2, 7, 0.98], [1124, 2, 9, 0.72], [2049, 1, 7, 1.7], [94, 4, 7, 3.47], [5812, 3, 8, 3.38], [13280, 1, 9, 3.64], [168, 3, 9, 1.46], [1504, 2, 7, 1.33], [12870, 1, 7, 1.5], [57, 1, 7, 0.7], [11234, 2, 8, 1.32], [415, 1, 7, 2.06], [8651, 2, 7, 1.94], [148, 1, 7, 1.56], [418, 2, 7, 0.7], [8853, 2, 14, 3.62], [6097, 29, 7, 3.38], [8939, 2, 7, 0.84], [416, 1, 7, 2.33], [6097, 80, 7, 3.38], [11737, 2, 7, 2.34], [20256, 2, 7, 1.42], [490, 1, 7, 2.02], [1490, 1, 7, 1.27], [998, 2, 7, 3.68], [20927, 1, 9, 0.89], [79, 1, 7, 0.7], [95, 3, 26, 0.85], [6098, 29, 7, 2.08], [14017, 3, 7, 1.0], [6098, 80, 7, 2.08], [414, 1, 7, 1.49], [9069, 1, 7, 1.91], [1070, 7, 16, 0.73], [1243, 2, 7, 0.96], [8898, 3, 7, 2.67], [1126, 2, 7, 1.22], [149, 2, 7, 2.73], [126, 2, 7, 2.75], [13034, 3, 8, 3.38], [997, 2, 7, 3.68], [9760, 29, 7, 0.87], [20498, 1, 7, 1.96], [20255, 2, 7, 1.43], [5086, 1, 9, 1.76], [5513, 2, 7, 0.84], [12924, 1, 9, 0.86], [9784, 1, 7, 1.06], [336, 15, 7, 1.66], [22317, 3, 8, 1.35], [11739, 2, 7, 1.65], [13260, 29, 7, 1.0], [7567, 3, 7, 3.2], [974, 3, 7, 1.64], [1413, 15, 7, 1.52], [11085, 2, 7, 0.83], [5811, 3, 7, 2.82], [229, 1, 7, 2.92], [972, 3, 8, 1.35], [5813, 3, 9, 2.14], [8557, 3, 7, 1.01], [192, 3, 22, 4.76], [9082, 3, 20, 2.38], [506, 1, 7, 2.73], [3049, 3, 7, 3.65], [9691, 1, 9, 2.48], [20498, 3, 8, 2.02], [14018, 3, 7, 1.0], [524, 1, 7, 2.16], [4076, 3, 7, 2.96], [470, 1, 7, 1.35], [1622, 1, 10, 0.79], [11454, 2, 9, 3.15], [2775, 2, 9, 0.73], [12870, 1, 113, 2.27], [57, 1, 79, 1.85], [11234, 2, 170, 2.47], [415, 1, 71, 2.31], [8651, 2, 186, 2.71], [148, 1, 80, 2.71], [418, 2, 131, 1.85], [8853, 2, 235, 4.88], [6097, 29, 27, 4.65], [8939, 2, 76, 2.11], [416, 1, 71, 2.57], [6097, 80, 55, 4.65], [11737, 2, 23, 3.11], [20256, 2, 77, 2.19], [490, 1, 36, 2.28], [1490, 1, 42, 2.03], [998, 2, 218, 4.83], [20927, 1, 65, 1.93], [79, 1, 44, 1.85], [95, 3, 936, 2.19], [6098, 29, 30, 3.21], [14017, 3, 162, 2.22], [6098, 80, 61, 3.2], [414, 1, 79, 2.64], [9069, 1, 100, 2.17], [1070, 7, 494, 2.01], [1243, 2, 90, 2.12], [8898, 3, 231, 3.94], [1126, 2, 189, 1.99], [149, 2, 80, 3.88], [126, 2, 75, 2.98], [13034, 3, 486, 4.14], [997, 2, 218, 4.83], [9760, 29, 59, 2.09], [20498, 1, 79, 2.73], [20255, 2, 77, 2.2], [5086, 1, 152, 3.49], [5513, 2, 70, 1.99], [12924, 1, 44, 2.3], [9784, 1, 60, 2.28], [336, 15, 93, 1.92], [22317, 3, 261, 2.11], [11739, 2, 47, 2.92], [13260, 29, 67, 2.15], [7567, 3, 57, 3.41], [974, 3, 136, 2.79], [1413, 15, 82, 2.79], [11085, 2, 508, 1.97], [5811, 3, 486, 3.58], [229, 1, 75, 4.08], [972, 3, 546, 2.51], [5813, 3, 486, 3.24], [8557, 3, 167, 2.28], [192, 3, 1287, 5.9], [9082, 3, 2070, 3.66], [506, 1, 80, 3.88], [3049, 3, 113, 4.42], [9691, 1, 62, 2.98], [20498, 3, 477, 2.76], [14018, 3, 162, 2.22], [524, 1, 69, 2.41], [4076, 3, 163, 3.19], [470, 1, 21, 2.12], [1622, 1, 50, 1.56], [11454, 2, 277, 4.42], [2775, 2, 130, 2.06]]</t>
+  </si>
+  <si>
+    <t>[[11685, 2, 7, 3.69], [6935, 2, 10, 4.2], [130, 1, 9, 0.77], [326, 2, 9, 2.77], [8648, 2, 7, 1.35], [144, 2, 9, 2.2], [593, 2, 7, 1.57], [2327, 2, 7, 0.9], [143, 2, 7, 1.57], [205, 2, 7, 1.48], [8915, 2, 8, 3.38], [2328, 2, 7, 1.41], [11681, 2, 7, 3.3], [6936, 2, 9, 4.22], [305, 2, 7, 0.88], [151, 1, 7, 1.25], [8650, 2, 7, 1.1], [141, 2, 7, 0.92], [2778, 2, 9, 1.07], [206, 2, 7, 1.35], [2049, 3, 14, 0.83], [88, 10, 18, 1.22], [615, 2, 7, 3.33], [7036, 1, 7, 3.02], [8853, 2, 7, 4.23], [8649, 2, 7, 1.87], [5491, 2, 7, 0.9], [248, 1, 7, 0.8], [434, 2, 7, 0.86], [1006, 2, 7, 1.93], [75, 2, 7, 2.32], [2055, 3, 7, 3.44], [11737, 2, 7, 1.58], [990, 2, 7, 1.06], [417, 2, 7, 0.98], [616, 2, 7, 2.96], [3840, 1, 7, 0.72], [2050, 3, 7, 0.67], [1007, 2, 7, 1.44], [12870, 1, 7, 3.71], [12353, 1, 9, 2.27], [523, 2, 7, 1.93], [1504, 2, 7, 2.06], [159, 3, 8, 0.61], [20927, 1, 7, 1.77], [2057, 3, 9, 0.88], [13280, 1, 9, 5.0], [10574, 3, 8, 2.36], [3, 2, 9, 0.74], [142, 2, 7, 0.94], [12346, 1, 9, 1.93], [7084, 3, 7, 1.12], [9760, 29, 7, 1.3], [624, 2, 7, 3.92], [2054, 3, 9, 0.88], [140, 2, 7, 1.7], [2775, 2, 7, 1.07], [21793, 1, 7, 4.43], [3891, 1, 7, 0.98], [8939, 2, 7, 0.89], [1429, 2, 7, 1.38], [96, 11, 22, 1.59], [11739, 2, 7, 1.14], [6158, 2, 9, 0.75], [950, 1, 7, 0.68], [5165, 2, 8, 3.15], [12269, 2, 7, 1.9], [84, 2, 7, 1.96], [1126, 2, 7, 1.26], [9372, 1, 7, 3.34], [10388, 2, 7, 2.13], [411, 2, 7, 1.02], [98, 11, 16, 0.91], [972, 3, 7, 2.05], [5165, 1, 7, 3.03], [2912, 1, 7, 0.8], [8898, 3, 7, 5.0], [413, 1, 7, 1.94], [2776, 2, 7, 2.59], [410, 1, 7, 1.04], [12343, 1, 7, 3.27], [10386, 2, 7, 1.68], [995, 2, 7, 3.38], [9491, 21, 16, 1.93], [956, 2, 7, 0.86], [1492, 1, 7, 2.77], [418, 2, 7, 0.81], [12345, 1, 7, 2.72], [13928, 1, 7, 1.6], [9784, 1, 7, 0.9], [22316, 3, 7, 0.92], [147, 1, 7, 0.98], [22247, 2, 7, 2.43], [412, 1, 7, 0.84], [336, 15, 7, 1.66], [8677, 3, 7, 1.73], [11490, 1, 7, 1.02], [7567, 3, 7, 3.18], [2912, 2, 8, 0.79], [308, 1, 7, 3.28], [432, 3, 7, 0.86], [307, 2, 7, 1.58], [11953, 1, 7, 0.96], [33, 1, 7, 2.04], [11770, 1, 9, 1.3], [10631, 2, 7, 2.7], [414, 1, 7, 1.24], [35, 1, 7, 2.06], [148, 1, 7, 1.01], [20256, 2, 7, 0.81], [10407, 10, 10, 2.88], [22317, 3, 7, 1.42], [1413, 15, 7, 1.17], [10410, 10, 10, 3.2], [10780, 10, 7, 3.0], [13286, 1, 7, 2.52], [415, 1, 7, 1.24], [439, 1, 7, 2.12], [335, 3, 15, 3.35], [7886, 4, 7, 0.86], [9691, 1, 7, 1.0], [7573, 1, 11, 3.36], [11767, 1, 7, 0.92], [12347, 1, 7, 3.27], [972, 1, 7, 2.77], [10387, 2, 7, 1.75], [10149, 3, 21, 1.48], [74, 1, 7, 2.13], [20686, 1, 7, 2.96], [3478, 2, 7, 3.14], [12271, 2, 7, 1.86], [9690, 1, 7, 1.39], [9971, 2, 7, 2.77], [1126, 2, 197, 2.71], [9372, 1, 196, 4.79], [10388, 2, 186, 3.58], [411, 2, 84, 2.73], [98, 11, 720, 2.35], [972, 3, 459, 2.73], [2912, 1, 38, 2.01], [8898, 3, 242, 6.0], [413, 1, 66, 2.64], [2776, 2, 135, 4.04], [410, 1, 81, 2.7], [12343, 1, 488, 4.47], [10386, 2, 186, 3.14], [995, 2, 208, 4.83], [9491, 21, 1812, 3.36], [956, 2, 93, 2.32], [1492, 1, 14, 3.97], [418, 2, 109, 2.48], [12345, 1, 488, 3.94], [13928, 1, 37, 2.81], [9784, 1, 56, 2.57], [22316, 3, 273, 2.38], [147, 1, 79, 2.43], [22247, 2, 243, 3.88], [412, 1, 65, 2.55], [336, 15, 86, 2.36], [8677, 3, 229, 2.72], [11490, 1, 94, 2.47], [7567, 3, 54, 3.83], [2912, 2, 342, 2.25], [308, 1, 139, 4.73], [432, 3, 237, 2.57], [307, 2, 115, 2.78], [11953, 1, 175, 2.42], [33, 1, 86, 2.74], [11770, 1, 170, 3.51], [10631, 2, 183, 4.15], [414, 1, 74, 2.69], [35, 1, 86, 2.75], [148, 1, 79, 2.46], [20256, 2, 81, 2.26], [10407, 10, 1015, 4.32], [22317, 3, 245, 2.63], [1413, 15, 86, 2.63], [10410, 10, 1015, 4.64], [10780, 10, 316, 4.46], [13286, 1, 246, 3.2], [415, 1, 74, 2.69], [439, 1, 75, 3.57], [335, 3, 1103, 4.78], [7886, 4, 99, 2.22], [9691, 1, 66, 2.45], [7573, 1, 288, 4.82], [11767, 1, 139, 2.37], [12347, 1, 488, 4.47], [972, 1, 85, 4.22], [10387, 2, 186, 3.2], [10149, 3, 752, 2.93], [74, 1, 176, 3.58], [20686, 1, 476, 4.17], [3478, 2, 29, 3.79], [12271, 2, 55, 3.31], [9690, 1, 65, 2.85], [9971, 2, 211, 3.59]]</t>
+  </si>
+  <si>
+    <t>[[8672, 2, 10, 1.03], [141, 2, 7, 1.22], [362, 2, 7, 0.88], [361, 2, 6, 0.99], [6935, 2, 23, 3.83], [205, 2, 7, 0.65], [12721, 2, 11, 2.8], [11737, 2, 7, 1.23], [206, 2, 7, 0.7], [2049, 3, 17, 0.72], [8676, 2, 7, 2.44], [8675, 2, 9, 1.42], [417, 2, 7, 1.55], [3, 2, 7, 0.96], [6936, 2, 7, 3.04], [305, 2, 7, 1.48], [151, 1, 7, 1.38], [523, 2, 7, 1.13], [22247, 2, 7, 1.83], [8650, 2, 7, 2.33], [142, 2, 7, 0.9], [8648, 2, 7, 3.27], [2328, 2, 7, 1.5], [2776, 2, 7, 1.18], [8853, 2, 7, 3.03], [616, 2, 7, 2.22], [11739, 2, 7, 1.23], [2327, 2, 7, 1.66], [11837, 2, 7, 0.82], [411, 2, 7, 0.86], [12352, 1, 7, 3.09], [589, 2, 7, 0.8], [143, 2, 7, 1.6], [146, 2, 7, 1.14], [11835, 2, 7, 1.06], [412, 1, 7, 1.93], [12353, 1, 7, 3.09], [6497, 1, 9, 1.34], [8674, 2, 7, 1.17], [583, 2, 7, 2.85], [145, 2, 7, 0.9], [2805, 137, 14, 1.1], [326, 2, 7, 2.54], [10574, 3, 9, 2.49], [418, 2, 7, 1.0], [144, 2, 7, 0.96], [6097, 80, 7, 3.38], [11738, 2, 7, 1.23], [11836, 2, 7, 0.97], [9784, 1, 7, 1.91], [10149, 3, 21, 0.86], [6097, 29, 7, 3.88], [413, 1, 7, 1.87], [2057, 3, 7, 3.23], [2055, 3, 7, 3.23], [75, 2, 7, 1.04], [11234, 2, 8, 1.32], [12344, 1, 7, 2.54], [1413, 15, 7, 0.89], [20252, 2, 7, 0.87], [11504, 2, 7, 0.67], [12269, 2, 7, 1.05], [8915, 2, 7, 0.71], [414, 1, 7, 1.91], [1492, 1, 7, 1.13], [6098, 80, 7, 2.19], [12346, 1, 7, 3.09], [3429, 15, 7, 0.85], [247, 1, 7, 3.32], [22316, 3, 7, 0.85], [1886, 2, 9, 0.75], [2774, 2, 7, 2.72], [1490, 1, 7, 0.66], [416, 1, 7, 2.14], [6098, 29, 7, 2.55], [9786, 1, 7, 2.84], [3934, 5, 8, 0.94], [2859, 15, 7, 1.05], [2049, 1, 7, 0.75], [201, 3, 7, 2.66], [3670, 2, 9, 3.61], [20555, 2, 7, 1.23], [6158, 2, 9, 1.76], [3478, 2, 7, 2.16], [7084, 3, 7, 1.81], [9785, 1, 7, 1.91], [12526, 2, 7, 2.78], [8599, 1, 7, 2.59], [8938, 2, 7, 1.07], [1703, 2, 7, 1.53], [4253, 1, 7, 0.92], [9760, 29, 7, 1.83], [186, 3, 12, 0.9], [1413, 16, 7, 0.68], [229, 1, 7, 2.94], [11885, 2, 7, 0.71], [107, 2, 7, 2.38], [11887, 2, 8, 0.65], [1050, 2, 7, 0.68], [11811, 1, 7, 1.93], [4232, 80, 7, 3.23], [94, 4, 7, 4.04], [11490, 1, 7, 0.96], [436, 2, 7, 0.94], [107, 7, 8, 1.99], [2438, 2, 8, 2.38], [415, 1, 7, 2.14], [947, 15, 7, 0.71], [11770, 1, 7, 0.8], [3673, 2, 7, 3.82], [11767, 1, 7, 0.88], [11671, 1, 7, 0.83], [5939, 3, 7, 0.91], [2821, 3, 13, 0.77], [11769, 1, 7, 0.88], [11160, 1, 7, 3.67], [11844, 2, 7, 1.16], [12347, 1, 7, 3.55], [5812, 3, 7, 4.0], [7036, 1, 7, 0.87], [9358, 1, 7, 0.81], [140, 2, 7, 2.41], [3495, 3, 21, 1.51], [12764, 2, 8, 0.82], [11771, 1, 7, 3.17], [5813, 3, 8, 1.92], [23920, 2, 7, 0.85], [11954, 1, 7, 0.77], [308, 1, 11, 1.83], [9690, 1, 7, 1.45], [410, 1, 7, 2.74], [5811, 3, 8, 3.52], [22573, 2, 7, 0.71], [3429, 15, 53, 2.63], [247, 1, 86, 5.11], [22316, 3, 318, 2.64], [1886, 2, 141, 2.86], [2774, 2, 205, 4.5], [1490, 1, 51, 2.45], [416, 1, 86, 3.92], [6098, 29, 37, 4.34], [9786, 1, 48, 4.45], [3934, 5, 586, 2.73], [2859, 15, 69, 2.84], [2049, 1, 15, 2.36], [201, 3, 299, 4.45], [3670, 2, 236, 5.41], [20555, 2, 57, 3.01], [6158, 2, 259, 3.55], [3478, 2, 75, 3.95], [7084, 3, 116, 3.92], [9785, 1, 64, 3.01], [12526, 2, 273, 4.56], [8599, 1, 145, 4.37], [8938, 2, 192, 2.86], [1703, 2, 164, 3.32], [4253, 1, 171, 2.71], [9760, 29, 63, 2.93], [186, 3, 665, 2.69], [1413, 16, 50, 2.47], [229, 1, 80, 4.73], [11885, 2, 97, 2.14], [107, 2, 48, 4.16], [11887, 2, 130, 2.26], [11811, 1, 451, 3.72], [4232, 80, 153, 5.02], [94, 4, 119, 5.82], [11490, 1, 110, 2.75], [436, 2, 107, 2.72], [107, 7, 216, 3.2], [2438, 2, 643, 4.17], [415, 1, 86, 3.92], [947, 15, 41, 2.5], [11770, 1, 220, 2.59], [3673, 2, 236, 5.61], [11767, 1, 164, 2.67], [11671, 1, 310, 2.62], [5939, 3, 266, 2.71], [2821, 3, 1338, 2.55], [11769, 1, 164, 2.67], [11160, 1, 491, 5.45], [11844, 2, 186, 2.77], [12347, 1, 607, 5.34], [5812, 3, 589, 5.78], [7036, 1, 127, 2.65], [9358, 1, 59, 2.6], [140, 2, 45, 3.84], [3495, 3, 965, 3.31], [12764, 2, 755, 2.62], [11771, 1, 213, 4.96], [5813, 3, 589, 3.7], [23920, 2, 106, 2.63], [11954, 1, 203, 2.56], [308, 1, 173, 3.62], [9690, 1, 75, 3.24], [410, 1, 35, 3.81], [5811, 3, 530, 5.12], [22573, 2, 36, 2.14]]</t>
+  </si>
+  <si>
+    <t>[[2327, 2, 7, 1.0], [305, 2, 7, 1.32], [6935, 2, 11, 4.28], [2778, 2, 9, 0.81], [144, 2, 9, 2.22], [130, 1, 7, 1.38], [8915, 2, 8, 1.9], [589, 2, 10, 0.99], [143, 2, 7, 1.12], [2328, 2, 7, 1.73], [6936, 2, 7, 3.42], [8648, 2, 7, 1.93], [2775, 2, 9, 0.94], [205, 2, 7, 0.83], [8650, 2, 7, 1.47], [326, 2, 9, 1.62], [593, 2, 9, 0.88], [146, 2, 7, 1.55], [145, 2, 7, 0.98], [7036, 1, 9, 2.3], [2049, 3, 10, 0.87], [2776, 2, 9, 0.94], [615, 2, 9, 0.87], [616, 2, 9, 0.66], [88, 10, 16, 2.46], [141, 2, 7, 0.71], [151, 1, 7, 1.38], [1124, 2, 7, 1.46], [11681, 2, 11, 3.45], [206, 2, 7, 0.74], [1446, 2, 7, 1.22], [9760, 29, 7, 1.18], [8853, 2, 7, 3.51], [990, 2, 7, 0.66], [5491, 2, 9, 1.44], [1007, 2, 7, 0.85], [362, 2, 9, 1.24], [8672, 2, 7, 2.94], [1504, 2, 7, 1.79], [2055, 3, 7, 0.84], [2057, 3, 7, 0.84], [9372, 1, 7, 3.79], [3893, 1, 7, 1.48], [8649, 2, 7, 1.29], [2912, 1, 7, 0.89], [8938, 2, 7, 0.95], [434, 2, 9, 0.71], [12870, 1, 7, 2.35], [10993, 2, 7, 1.34], [624, 2, 7, 2.19], [2050, 3, 7, 0.84], [417, 2, 9, 1.04], [3889, 1, 7, 0.65], [5165, 1, 7, 2.49], [1429, 2, 7, 0.91], [378, 2, 7, 4.21], [7084, 3, 7, 1.58], [10, 2, 7, 1.6], [2991, 3, 7, 3.64], [140, 2, 7, 3.18], [3891, 1, 7, 0.98], [1006, 2, 7, 1.04], [7886, 4, 7, 0.75], [10574, 3, 11, 3.29], [7573, 1, 22, 5.0], [10149, 3, 21, 1.48], [5208, 3, 9, 0.78], [1622, 1, 7, 1.03], [75, 2, 7, 0.75], [3, 2, 7, 0.89], [20927, 1, 7, 1.83], [5165, 2, 10, 2.34], [997, 2, 7, 2.64], [11234, 2, 7, 2.3], [1886, 2, 9, 0.82], [12721, 2, 7, 1.26], [22247, 2, 7, 2.64], [147, 1, 7, 3.37], [346, 3, 9, 0.69], [996, 2, 7, 2.83], [229, 1, 7, 0.86], [11811, 1, 7, 0.8], [20252, 2, 7, 1.43], [11685, 2, 11, 3.45], [94, 4, 7, 3.68], [998, 2, 7, 3.33], [972, 3, 10, 1.12], [2912, 2, 15, 0.66], [9491, 21, 17, 0.8], [76, 2, 7, 1.67], [35, 1, 7, 1.96], [439, 1, 9, 2.21], [413, 1, 7, 2.08], [13028, 3, 7, 4.24], [13928, 1, 7, 1.28], [8104, 1, 7, 1.67], [5076, 1, 7, 0.83], [2805, 137, 7, 1.16], [412, 1, 7, 1.85], [5209, 3, 9, 0.78], [8676, 2, 7, 4.08], [33, 1, 7, 1.87], [83, 2, 7, 1.69], [418, 2, 7, 1.21], [148, 1, 7, 3.39], [2774, 2, 7, 1.15], [3495, 3, 16, 1.41], [8898, 3, 7, 3.35], [7887, 4, 7, 1.81], [12212, 29, 7, 0.98], [20256, 2, 9, 0.82], [38, 1, 7, 2.23], [11490, 1, 7, 1.29], [11770, 1, 7, 2.76], [34, 1, 7, 2.1], [10407, 10, 10, 3.59], [415, 1, 7, 1.96], [9784, 1, 7, 0.96], [84, 2, 7, 1.37], [13928, 2, 7, 1.35], [126, 2, 7, 2.34], [411, 2, 7, 0.72], [11739, 2, 7, 2.61], [3048, 3, 7, 4.58], [9691, 1, 7, 1.05], [9690, 1, 7, 0.69], [8939, 2, 7, 0.92], [5584, 3, 7, 2.81], [11953, 1, 7, 0.84], [39, 1, 7, 2.18], [12351, 1, 7, 1.22], [11954, 1, 7, 0.7], [7567, 3, 7, 2.64], [1622, 1, 105, 2.67], [75, 2, 126, 2.69], [3, 2, 106, 2.81], [20927, 1, 34, 2.64], [5165, 2, 342, 4.82], [997, 2, 232, 4.28], [11234, 2, 179, 3.94], [1886, 2, 136, 2.8], [12721, 2, 244, 3.23], [22247, 2, 244, 3.57], [147, 1, 78, 4.28], [346, 3, 557, 2.68], [996, 2, 208, 4.81], [229, 1, 81, 2.5], [11811, 1, 402, 2.78], [20252, 2, 91, 3.07], [11685, 2, 234, 5.43], [94, 4, 105, 4.77], [998, 2, 208, 4.81], [972, 3, 522, 2.82], [2912, 2, 348, 2.47], [9491, 21, 1872, 2.76], [76, 2, 95, 2.65], [35, 1, 97, 2.93], [439, 1, 76, 4.69], [413, 1, 75, 3.04], [13028, 3, 128, 5.72], [13928, 1, 41, 3.26], [8104, 1, 180, 3.59], [5076, 1, 114, 2.77], [2805, 137, 157, 3.08], [412, 1, 73, 3.83], [5209, 3, 493, 2.87], [8676, 2, 275, 5.72], [33, 1, 97, 3.76], [418, 2, 124, 3.13], [148, 1, 78, 4.3], [2774, 2, 200, 2.79], [3495, 3, 938, 3.05], [8898, 3, 257, 4.83], [7887, 4, 39, 2.3], [12212, 29, 105, 2.95], [20256, 2, 81, 2.94], [38, 1, 97, 3.19], [11490, 1, 80, 2.77], [11770, 1, 206, 4.4], [34, 1, 97, 3.07], [10407, 10, 645, 5.06], [415, 1, 75, 2.92], [9784, 1, 71, 2.6], [84, 2, 58, 2.85], [13928, 2, 20, 3.26], [126, 2, 86, 3.98], [411, 2, 106, 2.37], [11739, 2, 55, 4.25], [3048, 3, 236, 6.0], [9691, 1, 74, 2.7], [9690, 1, 25, 1.67], [8939, 2, 169, 2.9], [5584, 3, 206, 4.28], [11953, 1, 195, 2.48], [39, 1, 97, 3.13], [12351, 1, 612, 2.87], [11954, 1, 195, 2.34], [7567, 3, 60, 4.12]]</t>
   </si>
   <si>
     <t>501QD</t>

</xml_diff>